<commit_message>
db level tappable update
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\data\q-z\Realm Defense\CyraBot\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB1206A-91FC-4E0C-98DD-8796B559DAEA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AD34B1-A50A-4A49-93DE-46FBE2AC63E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17147,8 +17147,8 @@
   <dimension ref="A1:G304"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A226" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E235" sqref="E235"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
level map pic link
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\data\q-z\Realm Defense\CyraBot\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2BA16B-C016-4A85-A0A1-803B838732F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4EE648-1817-46EF-8E93-5137A5CF5A4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4616" uniqueCount="2205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4876" uniqueCount="2367">
   <si>
     <t>name</t>
   </si>
@@ -7034,6 +7034,492 @@
   <si>
     <t>1) Big tree (*loose change*): 50:moneybag: (3x per wave)
 2) Bamboo bush (*hidden enemies*, *seeker*): on the left of big tree, at the start of each wave group of 24 monks will automatically be spawned, kill them for 120:moneybag: each time, (1x per wave), (6 waves so 720:moneybag: total)</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>T10</t>
+  </si>
+  <si>
+    <t>T11</t>
+  </si>
+  <si>
+    <t>T12</t>
+  </si>
+  <si>
+    <t>T13</t>
+  </si>
+  <si>
+    <t>T14</t>
+  </si>
+  <si>
+    <t>T15</t>
+  </si>
+  <si>
+    <t>T16</t>
+  </si>
+  <si>
+    <t>T17</t>
+  </si>
+  <si>
+    <t>T18</t>
+  </si>
+  <si>
+    <t>T19</t>
+  </si>
+  <si>
+    <t>T21</t>
+  </si>
+  <si>
+    <t>T22</t>
+  </si>
+  <si>
+    <t>T23</t>
+  </si>
+  <si>
+    <t>T24</t>
+  </si>
+  <si>
+    <t>T25</t>
+  </si>
+  <si>
+    <t>T26</t>
+  </si>
+  <si>
+    <t>T27</t>
+  </si>
+  <si>
+    <t>T28</t>
+  </si>
+  <si>
+    <t>T29</t>
+  </si>
+  <si>
+    <t>T31</t>
+  </si>
+  <si>
+    <t>T32</t>
+  </si>
+  <si>
+    <t>T33</t>
+  </si>
+  <si>
+    <t>T34</t>
+  </si>
+  <si>
+    <t>T35</t>
+  </si>
+  <si>
+    <t>T36</t>
+  </si>
+  <si>
+    <t>T37</t>
+  </si>
+  <si>
+    <t>T38</t>
+  </si>
+  <si>
+    <t>T39</t>
+  </si>
+  <si>
+    <t>T41</t>
+  </si>
+  <si>
+    <t>T42</t>
+  </si>
+  <si>
+    <t>T43</t>
+  </si>
+  <si>
+    <t>T44</t>
+  </si>
+  <si>
+    <t>T45</t>
+  </si>
+  <si>
+    <t>T46</t>
+  </si>
+  <si>
+    <t>T47</t>
+  </si>
+  <si>
+    <t>T48</t>
+  </si>
+  <si>
+    <t>T49</t>
+  </si>
+  <si>
+    <t>T51</t>
+  </si>
+  <si>
+    <t>T52</t>
+  </si>
+  <si>
+    <t>Flying Tutle Clearing</t>
+  </si>
+  <si>
+    <t>Land Squid Trails</t>
+  </si>
+  <si>
+    <t>Double Frog Court</t>
+  </si>
+  <si>
+    <t>Hanner Grove</t>
+  </si>
+  <si>
+    <t>Parallelogram of Ruin</t>
+  </si>
+  <si>
+    <t>Barb's Pumpkin Hexa-Path</t>
+  </si>
+  <si>
+    <t>Icecube Forest</t>
+  </si>
+  <si>
+    <t>Eye of Odin</t>
+  </si>
+  <si>
+    <t>Double Ansuz</t>
+  </si>
+  <si>
+    <t>Up-Down Diamond</t>
+  </si>
+  <si>
+    <t>T210</t>
+  </si>
+  <si>
+    <t>Ice Onion</t>
+  </si>
+  <si>
+    <t>T212</t>
+  </si>
+  <si>
+    <t>Triple Diamond Camp</t>
+  </si>
+  <si>
+    <t>T215</t>
+  </si>
+  <si>
+    <t>Halla Val</t>
+  </si>
+  <si>
+    <t>Crystal Mine</t>
+  </si>
+  <si>
+    <t>Perfect Angles</t>
+  </si>
+  <si>
+    <t>Tight Oasis</t>
+  </si>
+  <si>
+    <t>Gazi Town</t>
+  </si>
+  <si>
+    <t>T310</t>
+  </si>
+  <si>
+    <t>Omegru Waste</t>
+  </si>
+  <si>
+    <t>Convergence Field</t>
+  </si>
+  <si>
+    <t>Cloud Dreamin'</t>
+  </si>
+  <si>
+    <t>Kerr Black Hole</t>
+  </si>
+  <si>
+    <t>Diverging World Lines</t>
+  </si>
+  <si>
+    <t>Slime's Cave</t>
+  </si>
+  <si>
+    <t>Aki and Kai</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/2/20/160.png/revision/latest?cb=20210216173220</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/e/e2/159.png/revision/latest?cb=20210216173217</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/5/5d/158.png/revision/latest?cb=20210216173215</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/4/49/157.png/revision/latest?cb=20210216173214</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/4/43/156.png/revision/latest?cb=20210216173211</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/3/39/155.png/revision/latest?cb=20210216173208</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/f/fc/154.png/revision/latest?cb=20210216173206</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/0/05/153.png/revision/latest?cb=20210216173206</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/d/db/152.png/revision/latest?cb=20210216173203</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/3/39/151.png/revision/latest?cb=20210216173201</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/0/09/150.png/revision/latest?cb=20210216173159</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/d/d2/149.png/revision/latest?cb=20210216173156</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/5/51/148.png/revision/latest?cb=20210216173154</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/a/a3/147.png/revision/latest?cb=20210216173152</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/d/db/146.png/revision/latest?cb=20210216173150</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/c/c7/145.png/revision/latest?cb=20210216173005</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/9/9a/144.png/revision/latest?cb=20210216173003</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/7/7d/143.png/revision/latest?cb=20210216173002</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/d/d3/142.png/revision/latest?cb=20210216172959</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/6/67/141.png/revision/latest?cb=20210216172958</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/0/09/140.png/revision/latest?cb=20210216172956</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/d/d1/139.png/revision/latest?cb=20210216172954</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/4/4a/138.png/revision/latest?cb=20210216172952</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/9/9d/137.png/revision/latest?cb=20210216172951</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/d/de/136.png/revision/latest?cb=20210216172948</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/7/78/135.png/revision/latest?cb=20210216172822</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/3/3e/134.png/revision/latest?cb=20210216172948</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/6/6c/133.png/revision/latest?cb=20210216172749</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/6/60/132.png/revision/latest?cb=20210216172746</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/83/131.png/revision/latest?cb=20210216172745</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/c/ca/130.png/revision/latest?cb=20210216172743</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/e/ea/129.png/revision/latest?cb=20210216172741</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/3/32/128.png/revision/latest?cb=20210216172739</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/b/be/127.png/revision/latest?cb=20210216172737</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/a/af/126.png/revision/latest?cb=20210216172736</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/2/28/125.png/revision/latest?cb=20210216172736</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/a/a8/124.png/revision/latest?cb=20210216172731</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/81/123.png/revision/latest?cb=20210216172634</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/b/be/122.png/revision/latest?cb=20210216172621</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/d/d2/121.png/revision/latest?cb=20210216172557</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/81/161.png/revision/latest?cb=20210216193503</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/0/0f/162.png/revision/latest?cb=20210216193504</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/a/a4/163.png/revision/latest?cb=20210216193506</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/c/c2/164.png/revision/latest?cb=20210216193508</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/9/9d/165.png/revision/latest?cb=20210216193509</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/4/4f/166.png/revision/latest?cb=20210216193511</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/0/0b/167.png/revision/latest?cb=20210216193513</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/f/f8/168.png/revision/latest?cb=20210216193515</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/0/09/169.png/revision/latest?cb=20210216193516</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/b/be/170.png/revision/latest?cb=20210216193519</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/b/bb/171.png/revision/latest?cb=20210216193520</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/6/60/172.png/revision/latest?cb=20210216193522</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/3/3f/173.png/revision/latest?cb=20210216193524</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/6/65/174.png/revision/latest?cb=20210216193526</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/2/24/175.png/revision/latest?cb=20210216193527</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/d/dd/176.png/revision/latest?cb=20210216193530</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/2/27/177.png/revision/latest?cb=20210216193532</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/0/04/178.png/revision/latest?cb=20210216193534</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/9/93/179.png/revision/latest?cb=20210216193537</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/0/02/180.png/revision/latest?cb=20210216193538</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/83/181.png/revision/latest?cb=20210216193742</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/e/ec/182.png/revision/latest?cb=20210216193746</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/5/5a/183.png/revision/latest?cb=20210216193747</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/5/57/184.png/revision/latest?cb=20210216193749</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/b/b6/185.png/revision/latest?cb=20210216193750</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/7/77/186.png/revision/latest?cb=20210216193752</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/e/e8/187.png/revision/latest?cb=20210216193754</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/d/d4/188.png/revision/latest?cb=20210216193756</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/f/f8/189.png/revision/latest?cb=20210216193758</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/6/60/190.png/revision/latest?cb=20210216193759</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/86/191.png/revision/latest?cb=20210216193801</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/9/90/192.png/revision/latest?cb=20210216193802</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/a/a6/193.png/revision/latest?cb=20210216193805</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/f/f4/194.png/revision/latest?cb=20210216193806</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/3/33/195.png/revision/latest?cb=20210216193808</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/b/b9/196.png/revision/latest?cb=20210216193810</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/6/6d/197.png/revision/latest?cb=20210216193812</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/0/08/198.png/revision/latest?cb=20210216193814</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/2/25/199.png/revision/latest?cb=20210216193816</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/85/200.png/revision/latest?cb=20210216193818</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/2/22/3181AA62-519D-4373-8D9F-653B12D03798.png/revision/latest?cb=20200706132048</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/3/3b/8D5CCB86-7773-49EF-B15C-83F20660BCD4.png/revision/latest?cb=20200706132048</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/88/FB96EC01-6AB3-4ED7-AF89-A366F2225174.png/revision/latest?cb=20200706132048</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/2/26/27170062-35F6-4A07-91E7-A559B1448EFF.png/revision/latest?cb=20200706132049</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/4/4f/31F5E684-1838-4EF1-A169-DC207CFFC87C.png/revision/latest?cb=20200706132048</t>
   </si>
 </sst>
 </file>
@@ -17144,11 +17630,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D798F71-5A72-4731-9B2C-78595D904327}">
-  <dimension ref="A1:G304"/>
+  <dimension ref="A1:G356"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A205" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E215" sqref="E215"/>
+      <pane ySplit="1" topLeftCell="A249" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H290" sqref="H290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20786,7 +21272,7 @@
         <v>979</v>
       </c>
       <c r="F162" s="18" t="s">
-        <v>979</v>
+        <v>2321</v>
       </c>
       <c r="G162" s="18"/>
     </row>
@@ -20808,7 +21294,7 @@
         <v>979</v>
       </c>
       <c r="F163" s="18" t="s">
-        <v>979</v>
+        <v>2320</v>
       </c>
       <c r="G163" s="18"/>
     </row>
@@ -20830,7 +21316,7 @@
         <v>979</v>
       </c>
       <c r="F164" s="18" t="s">
-        <v>979</v>
+        <v>2319</v>
       </c>
       <c r="G164" s="18"/>
     </row>
@@ -20852,7 +21338,7 @@
         <v>979</v>
       </c>
       <c r="F165" s="18" t="s">
-        <v>979</v>
+        <v>2318</v>
       </c>
       <c r="G165" s="18"/>
     </row>
@@ -20874,7 +21360,7 @@
         <v>979</v>
       </c>
       <c r="F166" s="18" t="s">
-        <v>979</v>
+        <v>2317</v>
       </c>
       <c r="G166" s="18"/>
     </row>
@@ -20896,7 +21382,7 @@
         <v>979</v>
       </c>
       <c r="F167" s="18" t="s">
-        <v>979</v>
+        <v>2316</v>
       </c>
       <c r="G167" s="18"/>
     </row>
@@ -20918,7 +21404,7 @@
         <v>979</v>
       </c>
       <c r="F168" s="18" t="s">
-        <v>979</v>
+        <v>2315</v>
       </c>
       <c r="G168" s="18"/>
     </row>
@@ -20940,7 +21426,7 @@
         <v>979</v>
       </c>
       <c r="F169" s="18" t="s">
-        <v>979</v>
+        <v>2314</v>
       </c>
       <c r="G169" s="18"/>
     </row>
@@ -20962,7 +21448,7 @@
         <v>979</v>
       </c>
       <c r="F170" s="18" t="s">
-        <v>979</v>
+        <v>2313</v>
       </c>
       <c r="G170" s="18"/>
     </row>
@@ -20984,7 +21470,7 @@
         <v>979</v>
       </c>
       <c r="F171" s="18" t="s">
-        <v>979</v>
+        <v>2312</v>
       </c>
       <c r="G171" s="18" t="s">
         <v>985</v>
@@ -21008,7 +21494,7 @@
         <v>979</v>
       </c>
       <c r="F172" s="18" t="s">
-        <v>979</v>
+        <v>2311</v>
       </c>
       <c r="G172" s="18"/>
     </row>
@@ -21030,7 +21516,7 @@
         <v>979</v>
       </c>
       <c r="F173" s="18" t="s">
-        <v>979</v>
+        <v>2310</v>
       </c>
       <c r="G173" s="18"/>
     </row>
@@ -21052,7 +21538,7 @@
         <v>979</v>
       </c>
       <c r="F174" s="18" t="s">
-        <v>979</v>
+        <v>2309</v>
       </c>
       <c r="G174" s="18"/>
     </row>
@@ -21074,7 +21560,7 @@
         <v>979</v>
       </c>
       <c r="F175" s="18" t="s">
-        <v>979</v>
+        <v>2308</v>
       </c>
       <c r="G175" s="18"/>
     </row>
@@ -21096,7 +21582,7 @@
         <v>979</v>
       </c>
       <c r="F176" s="18" t="s">
-        <v>979</v>
+        <v>2307</v>
       </c>
       <c r="G176" s="18"/>
     </row>
@@ -21118,7 +21604,7 @@
         <v>979</v>
       </c>
       <c r="F177" s="18" t="s">
-        <v>979</v>
+        <v>2306</v>
       </c>
       <c r="G177" s="18"/>
     </row>
@@ -21140,7 +21626,7 @@
         <v>979</v>
       </c>
       <c r="F178" s="18" t="s">
-        <v>979</v>
+        <v>2305</v>
       </c>
       <c r="G178" s="18"/>
     </row>
@@ -21162,7 +21648,7 @@
         <v>979</v>
       </c>
       <c r="F179" s="18" t="s">
-        <v>979</v>
+        <v>2304</v>
       </c>
       <c r="G179" s="18"/>
     </row>
@@ -21184,7 +21670,7 @@
         <v>979</v>
       </c>
       <c r="F180" s="18" t="s">
-        <v>979</v>
+        <v>2303</v>
       </c>
       <c r="G180" s="18"/>
     </row>
@@ -21206,7 +21692,7 @@
         <v>979</v>
       </c>
       <c r="F181" s="18" t="s">
-        <v>979</v>
+        <v>2302</v>
       </c>
       <c r="G181" s="18" t="s">
         <v>985</v>
@@ -21230,7 +21716,7 @@
         <v>979</v>
       </c>
       <c r="F182" s="18" t="s">
-        <v>979</v>
+        <v>2301</v>
       </c>
       <c r="G182" s="18"/>
     </row>
@@ -21252,7 +21738,7 @@
         <v>979</v>
       </c>
       <c r="F183" s="18" t="s">
-        <v>979</v>
+        <v>2300</v>
       </c>
       <c r="G183" s="18"/>
     </row>
@@ -21274,7 +21760,7 @@
         <v>979</v>
       </c>
       <c r="F184" s="18" t="s">
-        <v>979</v>
+        <v>2299</v>
       </c>
       <c r="G184" s="18"/>
     </row>
@@ -21296,7 +21782,7 @@
         <v>979</v>
       </c>
       <c r="F185" s="18" t="s">
-        <v>979</v>
+        <v>2298</v>
       </c>
       <c r="G185" s="18"/>
     </row>
@@ -21318,7 +21804,7 @@
         <v>979</v>
       </c>
       <c r="F186" s="18" t="s">
-        <v>979</v>
+        <v>2297</v>
       </c>
       <c r="G186" s="18"/>
     </row>
@@ -21340,7 +21826,7 @@
         <v>979</v>
       </c>
       <c r="F187" s="18" t="s">
-        <v>979</v>
+        <v>2296</v>
       </c>
       <c r="G187" s="18"/>
     </row>
@@ -21362,7 +21848,7 @@
         <v>979</v>
       </c>
       <c r="F188" s="18" t="s">
-        <v>979</v>
+        <v>2295</v>
       </c>
       <c r="G188" s="18"/>
     </row>
@@ -21384,7 +21870,7 @@
         <v>979</v>
       </c>
       <c r="F189" s="18" t="s">
-        <v>979</v>
+        <v>2294</v>
       </c>
       <c r="G189" s="18"/>
     </row>
@@ -21406,7 +21892,7 @@
         <v>979</v>
       </c>
       <c r="F190" s="18" t="s">
-        <v>979</v>
+        <v>2293</v>
       </c>
       <c r="G190" s="18"/>
     </row>
@@ -21428,7 +21914,7 @@
         <v>979</v>
       </c>
       <c r="F191" s="18" t="s">
-        <v>979</v>
+        <v>2292</v>
       </c>
       <c r="G191" s="18" t="s">
         <v>985</v>
@@ -21452,7 +21938,7 @@
         <v>979</v>
       </c>
       <c r="F192" s="18" t="s">
-        <v>979</v>
+        <v>2291</v>
       </c>
       <c r="G192" s="18"/>
     </row>
@@ -21474,7 +21960,7 @@
         <v>979</v>
       </c>
       <c r="F193" s="18" t="s">
-        <v>979</v>
+        <v>2290</v>
       </c>
       <c r="G193" s="18"/>
     </row>
@@ -21496,7 +21982,7 @@
         <v>979</v>
       </c>
       <c r="F194" s="18" t="s">
-        <v>979</v>
+        <v>2289</v>
       </c>
       <c r="G194" s="18"/>
     </row>
@@ -21518,7 +22004,7 @@
         <v>979</v>
       </c>
       <c r="F195" s="18" t="s">
-        <v>979</v>
+        <v>2288</v>
       </c>
       <c r="G195" s="18"/>
     </row>
@@ -21540,7 +22026,7 @@
         <v>979</v>
       </c>
       <c r="F196" s="18" t="s">
-        <v>979</v>
+        <v>2287</v>
       </c>
       <c r="G196" s="18"/>
     </row>
@@ -21562,7 +22048,7 @@
         <v>979</v>
       </c>
       <c r="F197" s="18" t="s">
-        <v>979</v>
+        <v>2286</v>
       </c>
       <c r="G197" s="18"/>
     </row>
@@ -21584,7 +22070,7 @@
         <v>979</v>
       </c>
       <c r="F198" s="18" t="s">
-        <v>979</v>
+        <v>2285</v>
       </c>
       <c r="G198" s="18"/>
     </row>
@@ -21606,7 +22092,7 @@
         <v>979</v>
       </c>
       <c r="F199" s="18" t="s">
-        <v>979</v>
+        <v>2284</v>
       </c>
       <c r="G199" s="18"/>
     </row>
@@ -21628,7 +22114,7 @@
         <v>979</v>
       </c>
       <c r="F200" s="18" t="s">
-        <v>979</v>
+        <v>2283</v>
       </c>
       <c r="G200" s="18"/>
     </row>
@@ -21650,7 +22136,7 @@
         <v>979</v>
       </c>
       <c r="F201" s="18" t="s">
-        <v>979</v>
+        <v>2282</v>
       </c>
       <c r="G201" s="18" t="s">
         <v>985</v>
@@ -21674,7 +22160,7 @@
         <v>979</v>
       </c>
       <c r="F202" s="18" t="s">
-        <v>979</v>
+        <v>2322</v>
       </c>
       <c r="G202" s="18"/>
     </row>
@@ -21696,7 +22182,7 @@
         <v>979</v>
       </c>
       <c r="F203" s="18" t="s">
-        <v>979</v>
+        <v>2323</v>
       </c>
       <c r="G203" s="18"/>
     </row>
@@ -21718,7 +22204,7 @@
         <v>979</v>
       </c>
       <c r="F204" s="18" t="s">
-        <v>979</v>
+        <v>2324</v>
       </c>
       <c r="G204" s="18"/>
     </row>
@@ -21740,7 +22226,7 @@
         <v>979</v>
       </c>
       <c r="F205" s="18" t="s">
-        <v>979</v>
+        <v>2325</v>
       </c>
       <c r="G205" s="18"/>
     </row>
@@ -21762,7 +22248,7 @@
         <v>979</v>
       </c>
       <c r="F206" s="18" t="s">
-        <v>979</v>
+        <v>2326</v>
       </c>
       <c r="G206" s="18"/>
     </row>
@@ -21784,7 +22270,7 @@
         <v>979</v>
       </c>
       <c r="F207" s="18" t="s">
-        <v>979</v>
+        <v>2327</v>
       </c>
       <c r="G207" s="18"/>
     </row>
@@ -21806,7 +22292,7 @@
         <v>979</v>
       </c>
       <c r="F208" s="18" t="s">
-        <v>979</v>
+        <v>2328</v>
       </c>
       <c r="G208" s="18"/>
     </row>
@@ -21828,7 +22314,7 @@
         <v>979</v>
       </c>
       <c r="F209" s="18" t="s">
-        <v>979</v>
+        <v>2329</v>
       </c>
       <c r="G209" s="18"/>
     </row>
@@ -21850,7 +22336,7 @@
         <v>979</v>
       </c>
       <c r="F210" s="18" t="s">
-        <v>979</v>
+        <v>2330</v>
       </c>
       <c r="G210" s="18"/>
     </row>
@@ -21872,7 +22358,7 @@
         <v>979</v>
       </c>
       <c r="F211" s="18" t="s">
-        <v>979</v>
+        <v>2331</v>
       </c>
       <c r="G211" s="18" t="s">
         <v>985</v>
@@ -21896,7 +22382,7 @@
         <v>979</v>
       </c>
       <c r="F212" s="18" t="s">
-        <v>979</v>
+        <v>2332</v>
       </c>
       <c r="G212" s="18"/>
     </row>
@@ -21918,7 +22404,7 @@
         <v>2191</v>
       </c>
       <c r="F213" s="18" t="s">
-        <v>979</v>
+        <v>2333</v>
       </c>
       <c r="G213" s="18"/>
     </row>
@@ -21940,7 +22426,7 @@
         <v>979</v>
       </c>
       <c r="F214" s="18" t="s">
-        <v>979</v>
+        <v>2334</v>
       </c>
       <c r="G214" s="18"/>
     </row>
@@ -21962,7 +22448,7 @@
         <v>2204</v>
       </c>
       <c r="F215" s="18" t="s">
-        <v>979</v>
+        <v>2335</v>
       </c>
       <c r="G215" s="18"/>
     </row>
@@ -21984,7 +22470,7 @@
         <v>2190</v>
       </c>
       <c r="F216" s="18" t="s">
-        <v>979</v>
+        <v>2336</v>
       </c>
       <c r="G216" s="18"/>
     </row>
@@ -22006,7 +22492,7 @@
         <v>979</v>
       </c>
       <c r="F217" s="18" t="s">
-        <v>979</v>
+        <v>2337</v>
       </c>
       <c r="G217" s="18"/>
     </row>
@@ -22028,7 +22514,7 @@
         <v>979</v>
       </c>
       <c r="F218" s="18" t="s">
-        <v>979</v>
+        <v>2338</v>
       </c>
       <c r="G218" s="18"/>
     </row>
@@ -22050,7 +22536,7 @@
         <v>979</v>
       </c>
       <c r="F219" s="18" t="s">
-        <v>979</v>
+        <v>2339</v>
       </c>
       <c r="G219" s="18"/>
     </row>
@@ -22072,7 +22558,7 @@
         <v>979</v>
       </c>
       <c r="F220" s="18" t="s">
-        <v>979</v>
+        <v>2340</v>
       </c>
       <c r="G220" s="18"/>
     </row>
@@ -22094,7 +22580,7 @@
         <v>979</v>
       </c>
       <c r="F221" s="18" t="s">
-        <v>979</v>
+        <v>2341</v>
       </c>
       <c r="G221" s="18" t="s">
         <v>985</v>
@@ -22118,7 +22604,7 @@
         <v>979</v>
       </c>
       <c r="F222" s="18" t="s">
-        <v>979</v>
+        <v>2342</v>
       </c>
       <c r="G222" s="18"/>
     </row>
@@ -22140,7 +22626,7 @@
         <v>2188</v>
       </c>
       <c r="F223" s="18" t="s">
-        <v>979</v>
+        <v>2343</v>
       </c>
       <c r="G223" s="18"/>
     </row>
@@ -22162,7 +22648,7 @@
         <v>979</v>
       </c>
       <c r="F224" s="18" t="s">
-        <v>979</v>
+        <v>2344</v>
       </c>
       <c r="G224" s="18"/>
     </row>
@@ -22184,7 +22670,7 @@
         <v>979</v>
       </c>
       <c r="F225" s="18" t="s">
-        <v>979</v>
+        <v>2345</v>
       </c>
       <c r="G225" s="18"/>
     </row>
@@ -22206,7 +22692,7 @@
         <v>979</v>
       </c>
       <c r="F226" s="18" t="s">
-        <v>979</v>
+        <v>2346</v>
       </c>
       <c r="G226" s="18"/>
     </row>
@@ -22228,7 +22714,7 @@
         <v>2189</v>
       </c>
       <c r="F227" s="18" t="s">
-        <v>979</v>
+        <v>2347</v>
       </c>
       <c r="G227" s="18"/>
     </row>
@@ -22250,7 +22736,7 @@
         <v>2188</v>
       </c>
       <c r="F228" s="18" t="s">
-        <v>979</v>
+        <v>2348</v>
       </c>
       <c r="G228" s="18"/>
     </row>
@@ -22272,7 +22758,7 @@
         <v>979</v>
       </c>
       <c r="F229" s="18" t="s">
-        <v>979</v>
+        <v>2349</v>
       </c>
       <c r="G229" s="18"/>
     </row>
@@ -22294,7 +22780,7 @@
         <v>979</v>
       </c>
       <c r="F230" s="18" t="s">
-        <v>979</v>
+        <v>2350</v>
       </c>
       <c r="G230" s="18"/>
     </row>
@@ -22316,7 +22802,7 @@
         <v>2187</v>
       </c>
       <c r="F231" s="18" t="s">
-        <v>979</v>
+        <v>2351</v>
       </c>
       <c r="G231" s="18" t="s">
         <v>985</v>
@@ -22340,7 +22826,7 @@
         <v>979</v>
       </c>
       <c r="F232" s="18" t="s">
-        <v>979</v>
+        <v>2352</v>
       </c>
       <c r="G232" s="18"/>
     </row>
@@ -22362,7 +22848,7 @@
         <v>979</v>
       </c>
       <c r="F233" s="18" t="s">
-        <v>979</v>
+        <v>2353</v>
       </c>
       <c r="G233" s="18"/>
     </row>
@@ -22384,7 +22870,7 @@
         <v>979</v>
       </c>
       <c r="F234" s="18" t="s">
-        <v>979</v>
+        <v>2354</v>
       </c>
       <c r="G234" s="18"/>
     </row>
@@ -22406,7 +22892,7 @@
         <v>979</v>
       </c>
       <c r="F235" s="18" t="s">
-        <v>979</v>
+        <v>2355</v>
       </c>
       <c r="G235" s="18"/>
     </row>
@@ -22428,7 +22914,7 @@
         <v>979</v>
       </c>
       <c r="F236" s="18" t="s">
-        <v>979</v>
+        <v>2356</v>
       </c>
       <c r="G236" s="18"/>
     </row>
@@ -22450,7 +22936,7 @@
         <v>981</v>
       </c>
       <c r="F237" s="18" t="s">
-        <v>979</v>
+        <v>2357</v>
       </c>
       <c r="G237" s="18"/>
     </row>
@@ -22472,7 +22958,7 @@
         <v>979</v>
       </c>
       <c r="F238" s="18" t="s">
-        <v>979</v>
+        <v>2358</v>
       </c>
       <c r="G238" s="18"/>
     </row>
@@ -22494,7 +22980,7 @@
         <v>979</v>
       </c>
       <c r="F239" s="18" t="s">
-        <v>979</v>
+        <v>2359</v>
       </c>
       <c r="G239" s="18"/>
     </row>
@@ -22516,7 +23002,7 @@
         <v>979</v>
       </c>
       <c r="F240" s="18" t="s">
-        <v>979</v>
+        <v>2360</v>
       </c>
       <c r="G240" s="18"/>
     </row>
@@ -22538,7 +23024,7 @@
         <v>2186</v>
       </c>
       <c r="F241" s="18" t="s">
-        <v>979</v>
+        <v>2361</v>
       </c>
       <c r="G241" s="18" t="s">
         <v>985</v>
@@ -23422,7 +23908,7 @@
         <v>979</v>
       </c>
       <c r="F284" s="6" t="s">
-        <v>979</v>
+        <v>2362</v>
       </c>
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.35">
@@ -23442,7 +23928,7 @@
         <v>979</v>
       </c>
       <c r="F285" s="6" t="s">
-        <v>979</v>
+        <v>2363</v>
       </c>
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.35">
@@ -23462,7 +23948,7 @@
         <v>979</v>
       </c>
       <c r="F286" s="6" t="s">
-        <v>979</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.35">
@@ -23482,7 +23968,7 @@
         <v>979</v>
       </c>
       <c r="F287" s="6" t="s">
-        <v>979</v>
+        <v>2365</v>
       </c>
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.35">
@@ -23502,7 +23988,7 @@
         <v>979</v>
       </c>
       <c r="F288" s="6" t="s">
-        <v>979</v>
+        <v>2366</v>
       </c>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.35">
@@ -23850,6 +24336,1046 @@
       </c>
       <c r="G304" s="6" t="s">
         <v>2019</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A305" t="s">
+        <v>2205</v>
+      </c>
+      <c r="B305" s="8">
+        <v>1</v>
+      </c>
+      <c r="C305" s="10" t="s">
+        <v>773</v>
+      </c>
+      <c r="D305" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E305" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F305" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A306" t="s">
+        <v>2206</v>
+      </c>
+      <c r="B306" s="8">
+        <v>1</v>
+      </c>
+      <c r="C306" s="10" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D306" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E306" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F306" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A307" t="s">
+        <v>2207</v>
+      </c>
+      <c r="B307" s="8">
+        <v>1</v>
+      </c>
+      <c r="C307" s="10" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D307" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E307" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F307" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A308" t="s">
+        <v>2208</v>
+      </c>
+      <c r="B308" s="8">
+        <v>1</v>
+      </c>
+      <c r="C308" s="10" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D308" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E308" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F308" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A309" t="s">
+        <v>2209</v>
+      </c>
+      <c r="B309" s="8">
+        <v>1</v>
+      </c>
+      <c r="C309" s="10" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D309" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E309" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F309" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A310" t="s">
+        <v>2210</v>
+      </c>
+      <c r="B310" s="8">
+        <v>1</v>
+      </c>
+      <c r="C310" s="10" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D310" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E310" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F310" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A311" t="s">
+        <v>2211</v>
+      </c>
+      <c r="B311" s="8">
+        <v>1</v>
+      </c>
+      <c r="C311" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="D311" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E311" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F311" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A312" t="s">
+        <v>2212</v>
+      </c>
+      <c r="B312" s="8">
+        <v>1</v>
+      </c>
+      <c r="C312" s="10" t="s">
+        <v>758</v>
+      </c>
+      <c r="D312" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E312" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F312" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A313" t="s">
+        <v>2213</v>
+      </c>
+      <c r="B313" s="8">
+        <v>1</v>
+      </c>
+      <c r="C313" s="10" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D313" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E313" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F313" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A314" t="s">
+        <v>2214</v>
+      </c>
+      <c r="B314" s="8">
+        <v>1</v>
+      </c>
+      <c r="C314" s="10" t="s">
+        <v>2253</v>
+      </c>
+      <c r="D314" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E314" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F314" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A315" t="s">
+        <v>2215</v>
+      </c>
+      <c r="B315" s="8">
+        <v>1</v>
+      </c>
+      <c r="C315" s="10" t="s">
+        <v>2254</v>
+      </c>
+      <c r="D315" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E315" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F315" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A316" t="s">
+        <v>2216</v>
+      </c>
+      <c r="B316" s="8">
+        <v>1</v>
+      </c>
+      <c r="C316" s="10" t="s">
+        <v>2255</v>
+      </c>
+      <c r="D316" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E316" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F316" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A317" t="s">
+        <v>2217</v>
+      </c>
+      <c r="B317" s="8">
+        <v>1</v>
+      </c>
+      <c r="C317" s="10" t="s">
+        <v>2256</v>
+      </c>
+      <c r="D317" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E317" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F317" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A318" t="s">
+        <v>2218</v>
+      </c>
+      <c r="B318" s="8">
+        <v>1</v>
+      </c>
+      <c r="C318" s="10" t="s">
+        <v>2257</v>
+      </c>
+      <c r="D318" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E318" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F318" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A319" t="s">
+        <v>2219</v>
+      </c>
+      <c r="B319" s="8">
+        <v>1</v>
+      </c>
+      <c r="C319" s="10" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D319" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E319" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F319" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A320" t="s">
+        <v>2220</v>
+      </c>
+      <c r="B320" s="8">
+        <v>1</v>
+      </c>
+      <c r="C320" s="10" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D320" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E320" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F320" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A321" t="s">
+        <v>2221</v>
+      </c>
+      <c r="B321" s="8">
+        <v>1</v>
+      </c>
+      <c r="C321" s="10" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D321" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E321" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F321" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A322" t="s">
+        <v>2222</v>
+      </c>
+      <c r="B322" s="8">
+        <v>1</v>
+      </c>
+      <c r="C322" t="s">
+        <v>2258</v>
+      </c>
+      <c r="D322" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E322" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F322" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="323" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A323" t="s">
+        <v>2223</v>
+      </c>
+      <c r="B323" s="8">
+        <v>1</v>
+      </c>
+      <c r="C323" s="10" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D323" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E323" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F323" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A324" t="s">
+        <v>2224</v>
+      </c>
+      <c r="B324">
+        <v>2</v>
+      </c>
+      <c r="C324" t="s">
+        <v>1983</v>
+      </c>
+      <c r="D324" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E324" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F324" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A325" t="s">
+        <v>2225</v>
+      </c>
+      <c r="B325">
+        <v>2</v>
+      </c>
+      <c r="C325" s="10" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D325" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E325" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F325" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A326" t="s">
+        <v>2226</v>
+      </c>
+      <c r="B326">
+        <v>2</v>
+      </c>
+      <c r="C326" t="s">
+        <v>2259</v>
+      </c>
+      <c r="D326" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E326" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F326" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A327" t="s">
+        <v>2227</v>
+      </c>
+      <c r="B327">
+        <v>2</v>
+      </c>
+      <c r="C327" t="s">
+        <v>2260</v>
+      </c>
+      <c r="D327" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E327" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F327" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A328" t="s">
+        <v>2228</v>
+      </c>
+      <c r="B328">
+        <v>2</v>
+      </c>
+      <c r="C328" t="s">
+        <v>2261</v>
+      </c>
+      <c r="D328" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E328" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F328" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A329" t="s">
+        <v>2229</v>
+      </c>
+      <c r="B329">
+        <v>2</v>
+      </c>
+      <c r="C329" t="s">
+        <v>780</v>
+      </c>
+      <c r="D329" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E329" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F329" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A330" t="s">
+        <v>2230</v>
+      </c>
+      <c r="B330">
+        <v>2</v>
+      </c>
+      <c r="C330" s="10" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D330" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E330" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F330" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A331" t="s">
+        <v>2231</v>
+      </c>
+      <c r="B331">
+        <v>2</v>
+      </c>
+      <c r="C331" t="s">
+        <v>787</v>
+      </c>
+      <c r="D331" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E331" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F331" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A332" t="s">
+        <v>2232</v>
+      </c>
+      <c r="B332">
+        <v>2</v>
+      </c>
+      <c r="C332" t="s">
+        <v>2262</v>
+      </c>
+      <c r="D332" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E332" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F332" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A333" t="s">
+        <v>2263</v>
+      </c>
+      <c r="B333">
+        <v>2</v>
+      </c>
+      <c r="C333" t="s">
+        <v>2264</v>
+      </c>
+      <c r="D333" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E333" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F333" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A334" t="s">
+        <v>2265</v>
+      </c>
+      <c r="B334">
+        <v>2</v>
+      </c>
+      <c r="C334" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D334" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E334" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F334" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A335" t="s">
+        <v>2267</v>
+      </c>
+      <c r="B335">
+        <v>2</v>
+      </c>
+      <c r="C335" t="s">
+        <v>2268</v>
+      </c>
+      <c r="D335" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E335" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F335" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A336" t="s">
+        <v>2233</v>
+      </c>
+      <c r="B336">
+        <v>3</v>
+      </c>
+      <c r="C336" s="10" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D336" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E336" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F336" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A337" t="s">
+        <v>2234</v>
+      </c>
+      <c r="B337">
+        <v>3</v>
+      </c>
+      <c r="C337" t="s">
+        <v>805</v>
+      </c>
+      <c r="D337" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E337" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F337" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A338" t="s">
+        <v>2235</v>
+      </c>
+      <c r="B338">
+        <v>3</v>
+      </c>
+      <c r="C338" s="10" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D338" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E338" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F338" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A339" t="s">
+        <v>2236</v>
+      </c>
+      <c r="B339">
+        <v>3</v>
+      </c>
+      <c r="C339" s="10" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D339" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E339" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F339" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A340" t="s">
+        <v>2237</v>
+      </c>
+      <c r="B340">
+        <v>3</v>
+      </c>
+      <c r="C340" t="s">
+        <v>811</v>
+      </c>
+      <c r="D340" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E340" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F340" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A341" t="s">
+        <v>2238</v>
+      </c>
+      <c r="B341">
+        <v>3</v>
+      </c>
+      <c r="C341" t="s">
+        <v>2269</v>
+      </c>
+      <c r="D341" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E341" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F341" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A342" t="s">
+        <v>2239</v>
+      </c>
+      <c r="B342">
+        <v>3</v>
+      </c>
+      <c r="C342" t="s">
+        <v>2270</v>
+      </c>
+      <c r="D342" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E342" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F342" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A343" t="s">
+        <v>2240</v>
+      </c>
+      <c r="B343">
+        <v>3</v>
+      </c>
+      <c r="C343" t="s">
+        <v>2271</v>
+      </c>
+      <c r="D343" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E343" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F343" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A344" t="s">
+        <v>2241</v>
+      </c>
+      <c r="B344">
+        <v>3</v>
+      </c>
+      <c r="C344" t="s">
+        <v>2272</v>
+      </c>
+      <c r="D344" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E344" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F344" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A345" t="s">
+        <v>2273</v>
+      </c>
+      <c r="B345">
+        <v>3</v>
+      </c>
+      <c r="C345" t="s">
+        <v>2274</v>
+      </c>
+      <c r="D345" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E345" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F345" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A346" t="s">
+        <v>2242</v>
+      </c>
+      <c r="B346">
+        <v>4</v>
+      </c>
+      <c r="C346" t="s">
+        <v>2275</v>
+      </c>
+      <c r="D346" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E346" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F346" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A347" t="s">
+        <v>2243</v>
+      </c>
+      <c r="B347">
+        <v>4</v>
+      </c>
+      <c r="C347" t="s">
+        <v>2276</v>
+      </c>
+      <c r="D347" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E347" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F347" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A348" t="s">
+        <v>2244</v>
+      </c>
+      <c r="B348">
+        <v>4</v>
+      </c>
+      <c r="C348" t="s">
+        <v>2277</v>
+      </c>
+      <c r="D348" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E348" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F348" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A349" t="s">
+        <v>2245</v>
+      </c>
+      <c r="B349">
+        <v>4</v>
+      </c>
+      <c r="C349" s="10" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D349" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E349" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F349" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A350" t="s">
+        <v>2246</v>
+      </c>
+      <c r="B350">
+        <v>4</v>
+      </c>
+      <c r="C350" s="10" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D350" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E350" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F350" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A351" t="s">
+        <v>2247</v>
+      </c>
+      <c r="B351">
+        <v>4</v>
+      </c>
+      <c r="C351" t="s">
+        <v>2278</v>
+      </c>
+      <c r="D351" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E351" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F351" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A352" t="s">
+        <v>2248</v>
+      </c>
+      <c r="B352">
+        <v>4</v>
+      </c>
+      <c r="C352" s="10" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D352" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E352" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F352" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A353" t="s">
+        <v>2249</v>
+      </c>
+      <c r="B353">
+        <v>4</v>
+      </c>
+      <c r="C353" s="10" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D353" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E353" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F353" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A354" t="s">
+        <v>2250</v>
+      </c>
+      <c r="B354">
+        <v>4</v>
+      </c>
+      <c r="C354" s="10" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D354" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E354" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F354" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A355" t="s">
+        <v>2251</v>
+      </c>
+      <c r="B355">
+        <v>5</v>
+      </c>
+      <c r="C355" t="s">
+        <v>2279</v>
+      </c>
+      <c r="D355" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E355" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F355" s="6" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A356" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B356">
+        <v>5</v>
+      </c>
+      <c r="C356" t="s">
+        <v>2280</v>
+      </c>
+      <c r="D356" s="32" t="s">
+        <v>979</v>
+      </c>
+      <c r="E356" s="13" t="s">
+        <v>979</v>
+      </c>
+      <c r="F356" s="6" t="s">
+        <v>979</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
level image link to SR
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\data\q-z\Realm Defense\CyraBot\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4EE648-1817-46EF-8E93-5137A5CF5A4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EC7B32-2CA3-47F6-91ED-1EA354027574}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4876" uniqueCount="2367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4876" uniqueCount="2410">
   <si>
     <t>name</t>
   </si>
@@ -7520,6 +7520,135 @@
   </si>
   <si>
     <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/4/4f/31F5E684-1838-4EF1-A169-DC207CFFC87C.png/revision/latest?cb=20200706132048</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/0/05/World_6_Endless.jpg/revision/latest?cb=20210219234858</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/2/28/S1_-_Deadly_Meadow.png/revision/latest?cb=20210220031942</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/5/54/S2_-_Forest_Run.png/revision/latest?cb=20210220032044</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/e/e9/S3_-_Never_Ending_Pond.png/revision/latest?cb=20210220032210</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/2/20/S4_-_Sword_Hilt_Clearing.png/revision/latest?cb=20210220032253</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/1/18/S5_-_Poison_Valley.png/revision/latest?cb=20210220032352</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/4/4e/S6_-_Thundering_Ice.png/revision/latest?cb=20210220032506</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/3/3a/S7_-_Frosty_Thief.png/revision/latest?cb=20210220032557</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/e/e4/S8_-_Ice_Diamond.png/revision/latest?cb=20210220032702</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/9/9b/S9_-_Twin_Clearings.png/revision/latest?cb=20210220032740</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/2/27/S10_-_Permafrost_Crossing.png/revision/latest?cb=20210220032758</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/9/97/S11_-_Valley_of_the_Bandit.png/revision/latest?cb=20210220032836</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/85/S12_-_Town_of_Nothere.png/revision/latest?cb=20210220032903</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/e/ed/S13_-_Lost_Temple_of_Sands.png/revision/latest?cb=20210220032922</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/81/S14_-_Tomb_Raiders.png/revision/latest?cb=20210220032940</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/e/e3/S15-_Sickle_of_the_Sands.png/revision/latest?cb=20210220033005</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/a/aa/S16_-_He_Rises_Again....png/revision/latest?cb=20210220033047</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/d/d9/S17_-_You_Thought_it_Was....png/revision/latest?cb=20210220033109</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/f/fc/S18_-_Over%3F_But_no....png/revision/latest?cb=20210220033142</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/b/b7/S19_-_It_was_me%21.png/revision/latest?cb=20210220033206</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/3/3e/S20_-_Lord_Nivek_Again.png/revision/latest?cb=20210220033226</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/5/54/S21_-_Tiltkay_Oasis.png/revision/latest?cb=20210220033353</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/7/72/S22_-_Crossed_Curves.png/revision/latest?cb=20210220033410</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/c/c2/S23_-_Terrace_of_the_Why.png/revision/latest?cb=20210220033428</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/9/9f/S24_-_Tangled_Snakes_Valley.png/revision/latest?cb=20210220033445</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/4/42/S25_-_Valley_of_the_Sine.png/revision/latest?cb=20210220033502</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/c/c3/S26_-_Frosty_Waves_of_Survival.png/revision/latest?cb=20210220033537</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/c/c7/S27_-_Snowy_Robbery.png/revision/latest?cb=20210220033552</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/5/5d/S28_-_Sleepy_Ice.png/revision/latest?cb=20210220033607</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/86/S29_-_Snow_Thieves.png/revision/latest?cb=20210220033623</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/a/a8/S30_-_Survival_of_the_Coldest.png/revision/latest?cb=20210220033701</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/d/d0/S31_-_A_Hot_Time_Ago.png/revision/latest?cb=20210220033732</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/4/45/S32_-_In_a_Land_So_Hot.png/revision/latest?cb=20210220033751</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/5/51/S33_-_The_Sun_was_Fire.png/revision/latest?cb=20210220033808</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/1/14/S34_-_The_Ground_Burned.png/revision/latest?cb=20210220033827</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/7/7c/S35_-_All_was_sand.png/revision/latest?cb=20210220033847</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/4/40/S36_-_A_Split_in_the_Horde.png/revision/latest?cb=20210220034135</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/7/75/S37_-_Trapped_by_the_wall.png/revision/latest?cb=20210220034153</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/b/b0/S38_-_Thundering_snow_circles.png/revision/latest?cb=20210220034213</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/c/cc/S39_-_The_Ice_Temple.png/revision/latest?cb=20210220034239</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/d/d3/S40_-_Cornered_in_Ice.png/revision/latest?cb=20210220034317</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/c/c2/Potions_V_Slimes.png/revision/latest?cb=20210220014217</t>
+  </si>
+  <si>
+    <t>endless buff</t>
   </si>
 </sst>
 </file>
@@ -17633,8 +17762,8 @@
   <dimension ref="A1:G356"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A249" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H290" sqref="H290"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17644,7 +17773,8 @@
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="18.1796875" customWidth="1"/>
     <col min="5" max="5" width="50.90625" customWidth="1"/>
-    <col min="6" max="7" width="7.7265625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="11.6328125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="7.7265625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -17687,7 +17817,7 @@
         <v>979</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>979</v>
+        <v>2368</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>985</v>
@@ -17710,7 +17840,7 @@
         <v>979</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>979</v>
+        <v>2369</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>2017</v>
@@ -17733,7 +17863,7 @@
         <v>979</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>979</v>
+        <v>2370</v>
       </c>
       <c r="G4" s="15" t="s">
         <v>2018</v>
@@ -17756,7 +17886,7 @@
         <v>979</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>979</v>
+        <v>2371</v>
       </c>
       <c r="G5" s="15" t="s">
         <v>2017</v>
@@ -17779,7 +17909,7 @@
         <v>979</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>979</v>
+        <v>2372</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>985</v>
@@ -17802,7 +17932,7 @@
         <v>979</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>979</v>
+        <v>2373</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>985</v>
@@ -17825,7 +17955,7 @@
         <v>979</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>979</v>
+        <v>2374</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>2017</v>
@@ -17848,7 +17978,7 @@
         <v>979</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>979</v>
+        <v>2375</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>2018</v>
@@ -17871,7 +18001,7 @@
         <v>979</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>979</v>
+        <v>2376</v>
       </c>
       <c r="G10" s="15" t="s">
         <v>985</v>
@@ -17894,7 +18024,7 @@
         <v>979</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>979</v>
+        <v>2377</v>
       </c>
       <c r="G11" s="15" t="s">
         <v>985</v>
@@ -17917,7 +18047,7 @@
         <v>979</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>979</v>
+        <v>2378</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>2017</v>
@@ -17940,7 +18070,7 @@
         <v>979</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>979</v>
+        <v>2379</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>2018</v>
@@ -17963,7 +18093,7 @@
         <v>979</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>979</v>
+        <v>2380</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>2018</v>
@@ -17986,7 +18116,7 @@
         <v>979</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>979</v>
+        <v>2381</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>2017</v>
@@ -18009,7 +18139,7 @@
         <v>979</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>979</v>
+        <v>2382</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>2018</v>
@@ -18032,10 +18162,10 @@
         <v>979</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>979</v>
+        <v>2383</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>2018</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -18055,10 +18185,10 @@
         <v>979</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>979</v>
+        <v>2384</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>2018</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -18078,10 +18208,10 @@
         <v>979</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>979</v>
+        <v>2385</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>2018</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -18101,10 +18231,10 @@
         <v>979</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>979</v>
+        <v>2386</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>2018</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -18124,10 +18254,10 @@
         <v>979</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>979</v>
+        <v>2387</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>2018</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -18147,7 +18277,7 @@
         <v>979</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>979</v>
+        <v>2388</v>
       </c>
       <c r="G22" s="15" t="s">
         <v>2017</v>
@@ -18170,7 +18300,7 @@
         <v>979</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>979</v>
+        <v>2389</v>
       </c>
       <c r="G23" s="15" t="s">
         <v>2018</v>
@@ -18193,7 +18323,7 @@
         <v>979</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>979</v>
+        <v>2390</v>
       </c>
       <c r="G24" s="15" t="s">
         <v>2017</v>
@@ -18216,7 +18346,7 @@
         <v>979</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>979</v>
+        <v>2391</v>
       </c>
       <c r="G25" s="15" t="s">
         <v>2018</v>
@@ -18239,7 +18369,7 @@
         <v>979</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>979</v>
+        <v>2392</v>
       </c>
       <c r="G26" s="15" t="s">
         <v>2017</v>
@@ -18262,7 +18392,7 @@
         <v>979</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>979</v>
+        <v>2393</v>
       </c>
       <c r="G27" s="15" t="s">
         <v>2018</v>
@@ -18285,7 +18415,7 @@
         <v>979</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>979</v>
+        <v>2394</v>
       </c>
       <c r="G28" s="15" t="s">
         <v>2017</v>
@@ -18308,7 +18438,7 @@
         <v>979</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>979</v>
+        <v>2395</v>
       </c>
       <c r="G29" s="15" t="s">
         <v>2018</v>
@@ -18331,7 +18461,7 @@
         <v>979</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>979</v>
+        <v>2396</v>
       </c>
       <c r="G30" s="15" t="s">
         <v>2017</v>
@@ -18354,7 +18484,7 @@
         <v>979</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>979</v>
+        <v>2397</v>
       </c>
       <c r="G31" s="15" t="s">
         <v>2018</v>
@@ -18377,7 +18507,7 @@
         <v>979</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>979</v>
+        <v>2398</v>
       </c>
       <c r="G32" s="15" t="s">
         <v>2019</v>
@@ -18400,7 +18530,7 @@
         <v>979</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>979</v>
+        <v>2399</v>
       </c>
       <c r="G33" s="15" t="s">
         <v>2018</v>
@@ -18423,7 +18553,7 @@
         <v>979</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>979</v>
+        <v>2400</v>
       </c>
       <c r="G34" s="15" t="s">
         <v>2018</v>
@@ -18446,7 +18576,7 @@
         <v>979</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>979</v>
+        <v>2401</v>
       </c>
       <c r="G35" s="15" t="s">
         <v>2017</v>
@@ -18469,7 +18599,7 @@
         <v>979</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>979</v>
+        <v>2402</v>
       </c>
       <c r="G36" s="15" t="s">
         <v>2019</v>
@@ -18492,7 +18622,7 @@
         <v>979</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>979</v>
+        <v>2403</v>
       </c>
       <c r="G37" s="15" t="s">
         <v>985</v>
@@ -18515,7 +18645,7 @@
         <v>979</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>979</v>
+        <v>2404</v>
       </c>
       <c r="G38" s="15" t="s">
         <v>2019</v>
@@ -18538,7 +18668,7 @@
         <v>979</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>979</v>
+        <v>2405</v>
       </c>
       <c r="G39" s="15" t="s">
         <v>985</v>
@@ -18561,7 +18691,7 @@
         <v>979</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>979</v>
+        <v>2406</v>
       </c>
       <c r="G40" s="15" t="s">
         <v>2019</v>
@@ -18584,7 +18714,7 @@
         <v>979</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>979</v>
+        <v>2407</v>
       </c>
       <c r="G41" s="15" t="s">
         <v>2019</v>
@@ -24008,7 +24138,7 @@
         <v>979</v>
       </c>
       <c r="F289" s="6" t="s">
-        <v>979</v>
+        <v>2367</v>
       </c>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.35">
@@ -24028,7 +24158,7 @@
         <v>979</v>
       </c>
       <c r="F290" s="6" t="s">
-        <v>979</v>
+        <v>2408</v>
       </c>
       <c r="G290" s="6" t="s">
         <v>2019</v>
@@ -24051,7 +24181,7 @@
         <v>979</v>
       </c>
       <c r="F291" s="6" t="s">
-        <v>979</v>
+        <v>2408</v>
       </c>
       <c r="G291" s="6" t="s">
         <v>2019</v>
@@ -24074,7 +24204,7 @@
         <v>979</v>
       </c>
       <c r="F292" s="6" t="s">
-        <v>979</v>
+        <v>2408</v>
       </c>
       <c r="G292" s="6" t="s">
         <v>2019</v>

</xml_diff>

<commit_message>
level map link update
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\data\q-z\Realm Defense\CyraBot\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC675A6F-16A7-4BA3-B6C1-160A2AFB3D7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB4AF2B-3507-458C-8D76-B8531F5F658D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4882" uniqueCount="2412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4882" uniqueCount="2464">
   <si>
     <t>name</t>
   </si>
@@ -7656,6 +7656,162 @@
 **Ice Burst**: 20s cooldown, launches 9 icicles across the map, freezing hit targets within range 1 on trajectory for 5s.
 **Remorseless Winter**: 30s cooldown, freezes 3 random towers for 10s.
 **Puppeteer**: Summon 1/2/3 Crystal Guardians at 100%/67%/33% HP, cannot be damaged while the Crystal Guardians are alive</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/5/51/Connie_Chapter_1.jpg/revision/latest?cb=20210221035649</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/0/04/Connie_Chapter_2.jpg/revision/latest?cb=20210221035716</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/7/77/Connie_Chapter_3.jpg/revision/latest?cb=20210221035744</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/a/ae/Connie_Chapter_4.jpg/revision/latest?cb=20210221035813</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/6/68/Connie_Chapter_5_and_6.jpg/revision/latest?cb=20210221035843</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/0/03/Present_Plunder_1.jpg/revision/latest?cb=20210221040149</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/3/35/Present_Plunder_2.jpg/revision/latest?cb=20210221040226</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/4/48/Present_Plunder_3.jpg/revision/latest?cb=20210221040251</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/a/ac/Secret_Weapon_1.jpg/revision/latest?cb=20210221040322</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/f/fa/Secret_Weapon_2.jpg/revision/latest?cb=20210221040345</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/e/ed/Secret_Weapon_3.jpg/revision/latest?cb=20210221040406</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/6/61/Siberian_Match_1.jpg/revision/latest?cb=20210221040435</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/2/2c/Siberian_Match_2.jpg/revision/latest?cb=20210221040500</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/e/ec/Siberian_Match_3.jpg/revision/latest?cb=20210221040523</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/c/c2/Defense_of_Athena_1.jpg/revision/latest?cb=20210221040602</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/2/2f/Defense_of_Athena_2.jpg/revision/latest?cb=20210221040747</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/7/74/Defense_of_Athena_3.jpg/revision/latest?cb=20210221040832</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/b/b3/C1-1.jpg/revision/latest?cb=20210221030851</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/b/b1/C1-2.jpg/revision/latest?cb=20210221031026</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/9/98/C1-3.jpg/revision/latest?cb=20210221031128</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/b/ba/C1-4.jpg/revision/latest?cb=20210221031200</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/6/6b/C1-5.jpg/revision/latest?cb=20210221031236</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/d/dd/C2-1.jpg/revision/latest?cb=20210221031318</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/8c/C2-2.jpg/revision/latest?cb=20210221031347</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/2/2c/C2-3.jpg/revision/latest?cb=20210221031412</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/c/c6/C2-4.jpg/revision/latest?cb=20210221031437</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/9/97/C2-5.jpg/revision/latest?cb=20210221031503</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/1/15/C2-6.jpg/revision/latest?cb=20210221031531</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/9/99/C2-7.jpg/revision/latest?cb=20210221031601</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/88/C2-8.jpg/revision/latest?cb=20210221031631</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/6/62/C2-9.jpg/revision/latest?cb=20210221031654</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/8b/C2-10.jpg/revision/latest?cb=20210221031721</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/9/95/C3-1.jpg/revision/latest?cb=20210221031803</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/1/10/C3-2.jpg/revision/latest?cb=20210221031837</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/1/15/C3-3.jpg/revision/latest?cb=20210221031904</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/a/a5/C3-4.jpg/revision/latest?cb=20210221031928</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/4/4e/C3-5.jpg/revision/latest?cb=20210221031954</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/c/cc/C3-6.jpg/revision/latest?cb=20210221032017</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/6/6c/C3-7.jpg/revision/latest?cb=20210221032038</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/8d/C3-8.jpg/revision/latest?cb=20210221032109</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/a/a2/C3-9.jpg/revision/latest?cb=20210221032134</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/7/75/C3-10.jpg/revision/latest?cb=20210221032157</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/2/26/C6-1.jpg/revision/latest?cb=20210221032228</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/6/6b/C6-2.jpg/revision/latest?cb=20210221032255</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/b/b1/C6-3.jpg/revision/latest?cb=20210221032322</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/c/c9/C6-4.jpg/revision/latest?cb=20210221032350</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/c/cb/C6-5.jpg/revision/latest?cb=20210221032415</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/8e/C6-6.jpg/revision/latest?cb=20210221032440</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/6/6d/C6-7.jpg/revision/latest?cb=20210221032505</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/2/2d/C6-8.jpg/revision/latest?cb=20210221032530</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/9/96/C6-9.jpg/revision/latest?cb=20210221032553</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/8d/C6-10.jpg/revision/latest?cb=20210221032621</t>
   </si>
 </sst>
 </file>
@@ -17769,8 +17925,8 @@
   <dimension ref="A1:G356"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A278" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G289" sqref="G289"/>
+      <pane ySplit="1" topLeftCell="A298" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E305" sqref="E305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23184,7 +23340,7 @@
         <v>979</v>
       </c>
       <c r="F242" s="6" t="s">
-        <v>979</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.35">
@@ -23204,7 +23360,7 @@
         <v>979</v>
       </c>
       <c r="F243" s="6" t="s">
-        <v>979</v>
+        <v>2430</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.35">
@@ -23224,7 +23380,7 @@
         <v>979</v>
       </c>
       <c r="F244" s="6" t="s">
-        <v>979</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.35">
@@ -23244,7 +23400,7 @@
         <v>979</v>
       </c>
       <c r="F245" s="6" t="s">
-        <v>979</v>
+        <v>2432</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.35">
@@ -23264,7 +23420,7 @@
         <v>979</v>
       </c>
       <c r="F246" s="6" t="s">
-        <v>979</v>
+        <v>2433</v>
       </c>
       <c r="G246" s="18" t="s">
         <v>985</v>
@@ -23287,7 +23443,7 @@
         <v>979</v>
       </c>
       <c r="F247" s="6" t="s">
-        <v>979</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.35">
@@ -23307,7 +23463,7 @@
         <v>979</v>
       </c>
       <c r="F248" s="6" t="s">
-        <v>979</v>
+        <v>2435</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.35">
@@ -23327,7 +23483,7 @@
         <v>979</v>
       </c>
       <c r="F249" s="6" t="s">
-        <v>979</v>
+        <v>2436</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.35">
@@ -23347,7 +23503,7 @@
         <v>979</v>
       </c>
       <c r="F250" s="6" t="s">
-        <v>979</v>
+        <v>2437</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.35">
@@ -23367,7 +23523,7 @@
         <v>979</v>
       </c>
       <c r="F251" s="6" t="s">
-        <v>979</v>
+        <v>2438</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.35">
@@ -23387,7 +23543,7 @@
         <v>979</v>
       </c>
       <c r="F252" s="6" t="s">
-        <v>979</v>
+        <v>2439</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.35">
@@ -23407,7 +23563,7 @@
         <v>979</v>
       </c>
       <c r="F253" s="6" t="s">
-        <v>979</v>
+        <v>2440</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.35">
@@ -23427,7 +23583,7 @@
         <v>979</v>
       </c>
       <c r="F254" s="6" t="s">
-        <v>979</v>
+        <v>2441</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.35">
@@ -23447,7 +23603,7 @@
         <v>979</v>
       </c>
       <c r="F255" s="6" t="s">
-        <v>979</v>
+        <v>2442</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.35">
@@ -23467,7 +23623,7 @@
         <v>979</v>
       </c>
       <c r="F256" s="6" t="s">
-        <v>979</v>
+        <v>2443</v>
       </c>
       <c r="G256" s="18" t="s">
         <v>985</v>
@@ -23490,7 +23646,7 @@
         <v>979</v>
       </c>
       <c r="F257" s="6" t="s">
-        <v>979</v>
+        <v>2444</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.35">
@@ -23510,7 +23666,7 @@
         <v>979</v>
       </c>
       <c r="F258" s="6" t="s">
-        <v>979</v>
+        <v>2445</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.35">
@@ -23530,7 +23686,7 @@
         <v>979</v>
       </c>
       <c r="F259" s="6" t="s">
-        <v>979</v>
+        <v>2446</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.35">
@@ -23550,7 +23706,7 @@
         <v>979</v>
       </c>
       <c r="F260" s="6" t="s">
-        <v>979</v>
+        <v>2447</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.35">
@@ -23570,7 +23726,7 @@
         <v>979</v>
       </c>
       <c r="F261" s="6" t="s">
-        <v>979</v>
+        <v>2448</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.35">
@@ -23590,7 +23746,7 @@
         <v>979</v>
       </c>
       <c r="F262" s="6" t="s">
-        <v>979</v>
+        <v>2449</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.35">
@@ -23610,7 +23766,7 @@
         <v>979</v>
       </c>
       <c r="F263" s="6" t="s">
-        <v>979</v>
+        <v>2450</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.35">
@@ -23630,7 +23786,7 @@
         <v>979</v>
       </c>
       <c r="F264" s="6" t="s">
-        <v>979</v>
+        <v>2451</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.35">
@@ -23650,7 +23806,7 @@
         <v>979</v>
       </c>
       <c r="F265" s="6" t="s">
-        <v>979</v>
+        <v>2452</v>
       </c>
       <c r="G265" s="6" t="s">
         <v>985</v>
@@ -23673,7 +23829,7 @@
         <v>979</v>
       </c>
       <c r="F266" s="6" t="s">
-        <v>979</v>
+        <v>2453</v>
       </c>
       <c r="G266" s="18" t="s">
         <v>985</v>
@@ -23696,7 +23852,7 @@
         <v>979</v>
       </c>
       <c r="F267" s="6" t="s">
-        <v>979</v>
+        <v>2454</v>
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.35">
@@ -23716,7 +23872,7 @@
         <v>979</v>
       </c>
       <c r="F268" s="6" t="s">
-        <v>979</v>
+        <v>2455</v>
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.35">
@@ -23736,7 +23892,7 @@
         <v>979</v>
       </c>
       <c r="F269" s="6" t="s">
-        <v>979</v>
+        <v>2456</v>
       </c>
       <c r="G269" s="18" t="s">
         <v>985</v>
@@ -23759,7 +23915,7 @@
         <v>979</v>
       </c>
       <c r="F270" s="6" t="s">
-        <v>979</v>
+        <v>2457</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.35">
@@ -23779,7 +23935,7 @@
         <v>979</v>
       </c>
       <c r="F271" s="6" t="s">
-        <v>979</v>
+        <v>2458</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.35">
@@ -23799,7 +23955,7 @@
         <v>979</v>
       </c>
       <c r="F272" s="6" t="s">
-        <v>979</v>
+        <v>2459</v>
       </c>
       <c r="G272" s="18" t="s">
         <v>985</v>
@@ -23822,7 +23978,7 @@
         <v>979</v>
       </c>
       <c r="F273" s="6" t="s">
-        <v>979</v>
+        <v>2460</v>
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.35">
@@ -23842,7 +23998,7 @@
         <v>979</v>
       </c>
       <c r="F274" s="6" t="s">
-        <v>979</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.35">
@@ -23862,7 +24018,7 @@
         <v>979</v>
       </c>
       <c r="F275" s="6" t="s">
-        <v>979</v>
+        <v>2462</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.35">
@@ -23882,7 +24038,7 @@
         <v>979</v>
       </c>
       <c r="F276" s="6" t="s">
-        <v>979</v>
+        <v>2463</v>
       </c>
       <c r="G276" s="18" t="s">
         <v>985</v>
@@ -23905,7 +24061,7 @@
         <v>979</v>
       </c>
       <c r="F277" s="6" t="s">
-        <v>979</v>
+        <v>2412</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.35">
@@ -23925,7 +24081,7 @@
         <v>979</v>
       </c>
       <c r="F278" s="6" t="s">
-        <v>979</v>
+        <v>2413</v>
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.35">
@@ -23945,7 +24101,7 @@
         <v>979</v>
       </c>
       <c r="F279" s="6" t="s">
-        <v>979</v>
+        <v>2414</v>
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.35">
@@ -23965,7 +24121,7 @@
         <v>979</v>
       </c>
       <c r="F280" s="6" t="s">
-        <v>979</v>
+        <v>2415</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.35">
@@ -23985,7 +24141,7 @@
         <v>979</v>
       </c>
       <c r="F281" s="6" t="s">
-        <v>979</v>
+        <v>2416</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.35">
@@ -24005,7 +24161,7 @@
         <v>979</v>
       </c>
       <c r="F282" s="6" t="s">
-        <v>979</v>
+        <v>2416</v>
       </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.35">
@@ -24025,7 +24181,7 @@
         <v>979</v>
       </c>
       <c r="F283" s="6" t="s">
-        <v>979</v>
+        <v>2412</v>
       </c>
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.35">
@@ -24252,7 +24408,7 @@
         <v>979</v>
       </c>
       <c r="F293" s="6" t="s">
-        <v>979</v>
+        <v>2417</v>
       </c>
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.35">
@@ -24272,7 +24428,7 @@
         <v>979</v>
       </c>
       <c r="F294" s="6" t="s">
-        <v>979</v>
+        <v>2418</v>
       </c>
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.35">
@@ -24292,7 +24448,7 @@
         <v>979</v>
       </c>
       <c r="F295" s="6" t="s">
-        <v>979</v>
+        <v>2419</v>
       </c>
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.35">
@@ -24312,7 +24468,7 @@
         <v>979</v>
       </c>
       <c r="F296" s="6" t="s">
-        <v>979</v>
+        <v>2420</v>
       </c>
       <c r="G296" s="6" t="s">
         <v>2410</v>
@@ -24335,7 +24491,7 @@
         <v>979</v>
       </c>
       <c r="F297" s="6" t="s">
-        <v>979</v>
+        <v>2421</v>
       </c>
       <c r="G297" s="6" t="s">
         <v>2410</v>
@@ -24358,7 +24514,7 @@
         <v>979</v>
       </c>
       <c r="F298" s="6" t="s">
-        <v>979</v>
+        <v>2422</v>
       </c>
       <c r="G298" s="6" t="s">
         <v>2410</v>
@@ -24381,7 +24537,7 @@
         <v>979</v>
       </c>
       <c r="F299" s="6" t="s">
-        <v>979</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="300" spans="1:7" x14ac:dyDescent="0.35">
@@ -24401,7 +24557,7 @@
         <v>979</v>
       </c>
       <c r="F300" s="6" t="s">
-        <v>979</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="301" spans="1:7" x14ac:dyDescent="0.35">
@@ -24421,7 +24577,7 @@
         <v>979</v>
       </c>
       <c r="F301" s="6" t="s">
-        <v>979</v>
+        <v>2425</v>
       </c>
     </row>
     <row r="302" spans="1:7" x14ac:dyDescent="0.35">
@@ -24441,7 +24597,7 @@
         <v>979</v>
       </c>
       <c r="F302" s="6" t="s">
-        <v>979</v>
+        <v>2426</v>
       </c>
       <c r="G302" s="6" t="s">
         <v>2410</v>
@@ -24464,7 +24620,7 @@
         <v>979</v>
       </c>
       <c r="F303" s="6" t="s">
-        <v>979</v>
+        <v>2427</v>
       </c>
       <c r="G303" s="6" t="s">
         <v>2410</v>
@@ -24487,7 +24643,7 @@
         <v>979</v>
       </c>
       <c r="F304" s="6" t="s">
-        <v>979</v>
+        <v>2428</v>
       </c>
       <c r="G304" s="6" t="s">
         <v>2410</v>

</xml_diff>

<commit_message>
new tournament boss info
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\data\q-z\Realm Defense\CyraBot\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CEC763-BFEA-4345-814C-B4690434EE08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0065900-34D9-4626-996F-AD588E490F71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hero" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5079" uniqueCount="2472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5084" uniqueCount="2474">
   <si>
     <t>name</t>
   </si>
@@ -7836,6 +7836,13 @@
   </si>
   <si>
     <t>1s cooldown, Caldera switches between true and giant forms at the cost of 20% hp, and triggers __*Ring Of Fire*__. He gains the following buff at giant form: hp x8, ND x8, physical armor +100%, cast speed x2, move speed -2, and constant life drain which allows him to stand 67s starting at FULL hp</t>
+  </si>
+  <si>
+    <t>Rokujo Tournament</t>
+  </si>
+  <si>
+    <t>**Melee**: 2s cooldown, deals `(1 ND) MD` to a target.
+**Ama no Murakumo no Turugi**: 10s cooldown, empowers 2 random allies for 20s. Increase their health and speed x1.125, dodge x1.1. This spell can only be used 3 times.</t>
   </si>
 </sst>
 </file>
@@ -13829,7 +13836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D323"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
@@ -26493,11 +26500,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B78993A1-ED23-4BA3-9898-CFB8D57B537E}">
-  <dimension ref="A1:N158"/>
+  <dimension ref="A1:N159"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F131" sqref="F131"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32130,9 +32137,9 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A135" s="23" t="s">
-        <v>2042</v>
+        <v>2472</v>
       </c>
       <c r="B135" s="26">
         <v>6</v>
@@ -32141,7 +32148,7 @@
         <v>655</v>
       </c>
       <c r="D135" s="26">
-        <v>15200000</v>
+        <v>4500</v>
       </c>
       <c r="E135" s="26">
         <v>0</v>
@@ -32156,7 +32163,7 @@
         <v>1</v>
       </c>
       <c r="I135" s="26">
-        <v>800</v>
+        <v>130</v>
       </c>
       <c r="J135" s="26">
         <v>0</v>
@@ -32165,7 +32172,7 @@
         <v>0</v>
       </c>
       <c r="L135" s="23" t="s">
-        <v>1251</v>
+        <v>2473</v>
       </c>
       <c r="M135" s="25" t="s">
         <v>982</v>
@@ -32174,9 +32181,9 @@
         <v>1515</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A136" s="23" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="B136" s="26">
         <v>6</v>
@@ -32185,22 +32192,22 @@
         <v>655</v>
       </c>
       <c r="D136" s="26">
-        <v>8400000</v>
+        <v>15200000</v>
       </c>
       <c r="E136" s="26">
+        <v>0</v>
+      </c>
+      <c r="F136" s="26">
+        <v>0</v>
+      </c>
+      <c r="G136" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="H136" s="26">
         <v>1</v>
       </c>
-      <c r="F136" s="26">
-        <v>1</v>
-      </c>
-      <c r="G136" s="26">
-        <v>0</v>
-      </c>
-      <c r="H136" s="26">
-        <v>0.7</v>
-      </c>
       <c r="I136" s="26">
-        <v>750</v>
+        <v>800</v>
       </c>
       <c r="J136" s="26">
         <v>0</v>
@@ -32209,18 +32216,18 @@
         <v>0</v>
       </c>
       <c r="L136" s="23" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="M136" s="25" t="s">
         <v>982</v>
       </c>
       <c r="N136" s="27" t="s">
-        <v>1516</v>
-      </c>
-    </row>
-    <row r="137" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A137" s="23" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="B137" s="26">
         <v>6</v>
@@ -32229,22 +32236,22 @@
         <v>655</v>
       </c>
       <c r="D137" s="26">
-        <v>9100000</v>
+        <v>8400000</v>
       </c>
       <c r="E137" s="26">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F137" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G137" s="26">
         <v>0</v>
       </c>
       <c r="H137" s="26">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="I137" s="26">
-        <v>720</v>
+        <v>750</v>
       </c>
       <c r="J137" s="26">
         <v>0</v>
@@ -32253,18 +32260,18 @@
         <v>0</v>
       </c>
       <c r="L137" s="23" t="s">
-        <v>1768</v>
+        <v>1252</v>
       </c>
       <c r="M137" s="25" t="s">
         <v>982</v>
       </c>
       <c r="N137" s="27" t="s">
-        <v>1517</v>
-      </c>
-    </row>
-    <row r="138" spans="1:14" ht="130.5" x14ac:dyDescent="0.35">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A138" s="23" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="B138" s="26">
         <v>6</v>
@@ -32273,13 +32280,13 @@
         <v>655</v>
       </c>
       <c r="D138" s="26">
-        <v>10500000</v>
+        <v>9100000</v>
       </c>
       <c r="E138" s="26">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="F138" s="26">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="G138" s="26">
         <v>0</v>
@@ -32288,7 +32295,7 @@
         <v>1</v>
       </c>
       <c r="I138" s="26">
-        <v>3750</v>
+        <v>720</v>
       </c>
       <c r="J138" s="26">
         <v>0</v>
@@ -32297,18 +32304,18 @@
         <v>0</v>
       </c>
       <c r="L138" s="23" t="s">
-        <v>1253</v>
+        <v>1768</v>
       </c>
       <c r="M138" s="25" t="s">
         <v>982</v>
       </c>
       <c r="N138" s="27" t="s">
-        <v>1518</v>
-      </c>
-    </row>
-    <row r="139" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A139" s="23" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="B139" s="26">
         <v>6</v>
@@ -32317,10 +32324,10 @@
         <v>655</v>
       </c>
       <c r="D139" s="26">
-        <v>8400000</v>
+        <v>10500000</v>
       </c>
       <c r="E139" s="26">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="F139" s="26">
         <v>0.65</v>
@@ -32341,18 +32348,18 @@
         <v>0</v>
       </c>
       <c r="L139" s="23" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="M139" s="25" t="s">
         <v>982</v>
       </c>
       <c r="N139" s="27" t="s">
-        <v>1519</v>
-      </c>
-    </row>
-    <row r="140" spans="1:14" ht="116" x14ac:dyDescent="0.35">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A140" s="23" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="B140" s="26">
         <v>6</v>
@@ -32361,7 +32368,7 @@
         <v>655</v>
       </c>
       <c r="D140" s="26">
-        <v>6300000</v>
+        <v>8400000</v>
       </c>
       <c r="E140" s="26">
         <v>0.75</v>
@@ -32370,7 +32377,7 @@
         <v>0.65</v>
       </c>
       <c r="G140" s="26">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H140" s="26">
         <v>1</v>
@@ -32385,18 +32392,18 @@
         <v>0</v>
       </c>
       <c r="L140" s="23" t="s">
-        <v>1767</v>
+        <v>1254</v>
       </c>
       <c r="M140" s="25" t="s">
         <v>982</v>
       </c>
       <c r="N140" s="27" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="141" spans="1:14" ht="116" x14ac:dyDescent="0.35">
       <c r="A141" s="23" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="B141" s="26">
         <v>6</v>
@@ -32405,7 +32412,7 @@
         <v>655</v>
       </c>
       <c r="D141" s="26">
-        <v>8400000</v>
+        <v>6300000</v>
       </c>
       <c r="E141" s="26">
         <v>0.75</v>
@@ -32414,7 +32421,7 @@
         <v>0.65</v>
       </c>
       <c r="G141" s="26">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H141" s="26">
         <v>1</v>
@@ -32429,18 +32436,18 @@
         <v>0</v>
       </c>
       <c r="L141" s="23" t="s">
-        <v>1255</v>
+        <v>1767</v>
       </c>
       <c r="M141" s="25" t="s">
         <v>982</v>
       </c>
       <c r="N141" s="27" t="s">
-        <v>1521</v>
-      </c>
-    </row>
-    <row r="142" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14" ht="116" x14ac:dyDescent="0.35">
       <c r="A142" s="23" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="B142" s="26">
         <v>6</v>
@@ -32449,22 +32456,22 @@
         <v>655</v>
       </c>
       <c r="D142" s="26">
-        <v>4000</v>
+        <v>8400000</v>
       </c>
       <c r="E142" s="26">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="F142" s="26">
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="G142" s="26">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H142" s="26">
         <v>1</v>
       </c>
       <c r="I142" s="26">
-        <v>150</v>
+        <v>3750</v>
       </c>
       <c r="J142" s="26">
         <v>0</v>
@@ -32473,18 +32480,18 @@
         <v>0</v>
       </c>
       <c r="L142" s="23" t="s">
-        <v>1766</v>
+        <v>1255</v>
       </c>
       <c r="M142" s="25" t="s">
         <v>982</v>
       </c>
       <c r="N142" s="27" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="143" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A143" s="23" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="B143" s="26">
         <v>6</v>
@@ -32493,22 +32500,22 @@
         <v>655</v>
       </c>
       <c r="D143" s="26">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="E143" s="26">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="F143" s="26">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="G143" s="26">
-        <v>0.35</v>
+        <v>0.5</v>
       </c>
       <c r="H143" s="26">
         <v>1</v>
       </c>
       <c r="I143" s="26">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="J143" s="26">
         <v>0</v>
@@ -32517,17 +32524,61 @@
         <v>0</v>
       </c>
       <c r="L143" s="23" t="s">
-        <v>1256</v>
+        <v>1766</v>
       </c>
       <c r="M143" s="25" t="s">
         <v>982</v>
       </c>
       <c r="N143" s="27" t="s">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A144" s="23" t="s">
+        <v>2050</v>
+      </c>
+      <c r="B144" s="26">
+        <v>6</v>
+      </c>
+      <c r="C144" s="26" t="s">
+        <v>655</v>
+      </c>
+      <c r="D144" s="26">
+        <v>5000</v>
+      </c>
+      <c r="E144" s="26">
+        <v>0.25</v>
+      </c>
+      <c r="F144" s="26">
+        <v>0.35</v>
+      </c>
+      <c r="G144" s="26">
+        <v>0.35</v>
+      </c>
+      <c r="H144" s="26">
+        <v>1</v>
+      </c>
+      <c r="I144" s="26">
+        <v>100</v>
+      </c>
+      <c r="J144" s="26">
+        <v>0</v>
+      </c>
+      <c r="K144" s="26">
+        <v>0</v>
+      </c>
+      <c r="L144" s="23" t="s">
+        <v>1256</v>
+      </c>
+      <c r="M144" s="25" t="s">
+        <v>982</v>
+      </c>
+      <c r="N144" s="27" t="s">
         <v>1521</v>
       </c>
     </row>
-    <row r="158" spans="14:14" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="N158" s="29"/>
+    <row r="159" spans="14:14" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="N159" s="29"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -32663,19 +32714,20 @@
     <hyperlink ref="N110" r:id="rId130" xr:uid="{5B501AD1-8ED8-42D6-9514-2A4D3A7B0447}"/>
     <hyperlink ref="N111" r:id="rId131" xr:uid="{15C6C868-812E-4D15-8876-4893C7209DE0}"/>
     <hyperlink ref="N113" r:id="rId132" xr:uid="{7E5AC770-3B2A-4647-BB58-3C4FE4456DD4}"/>
-    <hyperlink ref="N135" r:id="rId133" xr:uid="{D78A8660-97E6-41E7-84B2-C1FF94F625C9}"/>
-    <hyperlink ref="N136" r:id="rId134" xr:uid="{FBA63F17-91D5-4EA3-87FA-CDF9659555CA}"/>
-    <hyperlink ref="N137" r:id="rId135" xr:uid="{6C8B3F3F-172A-4913-B6D9-7C8896C20EF7}"/>
-    <hyperlink ref="N138" r:id="rId136" xr:uid="{276A4B61-CC5A-44FC-90BA-CD3A674AACFA}"/>
-    <hyperlink ref="N139" r:id="rId137" xr:uid="{A2E00727-104D-46AC-B79C-F058CB70407F}"/>
-    <hyperlink ref="N140" r:id="rId138" xr:uid="{45DA676B-8D65-47B3-B2F2-2F9B729BE70B}"/>
-    <hyperlink ref="N142" r:id="rId139" xr:uid="{D37B1EEE-C26A-4AAB-9FA7-682438E57679}"/>
-    <hyperlink ref="N141" r:id="rId140" xr:uid="{9EDBDAF2-3EE5-4011-8C1B-CB7B96F58EA3}"/>
-    <hyperlink ref="N143" r:id="rId141" xr:uid="{94F8F863-4995-440F-AC42-04ECC832B018}"/>
+    <hyperlink ref="N136" r:id="rId133" xr:uid="{D78A8660-97E6-41E7-84B2-C1FF94F625C9}"/>
+    <hyperlink ref="N137" r:id="rId134" xr:uid="{FBA63F17-91D5-4EA3-87FA-CDF9659555CA}"/>
+    <hyperlink ref="N138" r:id="rId135" xr:uid="{6C8B3F3F-172A-4913-B6D9-7C8896C20EF7}"/>
+    <hyperlink ref="N139" r:id="rId136" xr:uid="{276A4B61-CC5A-44FC-90BA-CD3A674AACFA}"/>
+    <hyperlink ref="N140" r:id="rId137" xr:uid="{A2E00727-104D-46AC-B79C-F058CB70407F}"/>
+    <hyperlink ref="N141" r:id="rId138" xr:uid="{45DA676B-8D65-47B3-B2F2-2F9B729BE70B}"/>
+    <hyperlink ref="N143" r:id="rId139" xr:uid="{D37B1EEE-C26A-4AAB-9FA7-682438E57679}"/>
+    <hyperlink ref="N142" r:id="rId140" xr:uid="{9EDBDAF2-3EE5-4011-8C1B-CB7B96F58EA3}"/>
+    <hyperlink ref="N144" r:id="rId141" xr:uid="{94F8F863-4995-440F-AC42-04ECC832B018}"/>
     <hyperlink ref="N22" r:id="rId142" xr:uid="{ABC9D378-BFCA-4E9E-BF38-C445452246DC}"/>
+    <hyperlink ref="N135" r:id="rId143" xr:uid="{F7BADB22-9B4C-41EE-A700-D9F0B3350D7A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId143"/>
+  <pageSetup orientation="portrait" r:id="rId144"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
w7 enemies and towers
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\data\q-z\Realm Defense\CyraBot\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F86FFDF-2507-4BDC-B016-A7502779D3C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D30398C-8B49-406D-B260-E98AB65B066A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hero" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5314" uniqueCount="2586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5326" uniqueCount="2598">
   <si>
     <t>name</t>
   </si>
@@ -8065,21 +8065,6 @@
     <t>7s cooldown, Hogan deals `(1 ND) PD` in melee and summons a boar which inherits his damage, and gives all summoned units a 50% speed haste for 3.5s. The boar will deal `(10 ND) PD` to a strong target and stun it for 6s</t>
   </si>
   <si>
-    <t>By spending 900 coins you are able to hire one of the mercenary below, they will join the battle in next wave:
-(1) **Sylvan Archer**
-- 1000 HP, 30% physical armor, 10% magical armor, 150 ND, 1.5 move speed
-- Ranged: range 5, air-furthest, `(1 ND) PD` every 1.1s
-- Melee: `(0.666 ND) PD` every 1.1s
-(2) **Sylvan Fighter**
-- 1300 HP, 128 ND, 1.5 move speed
-- Melee: `(1 ND) PD`with 2 attacks, each 1.75s cooldown
-- Aura of Encouragement: haste tower troops by 50% in range 1.5
-(3) **Sylvan Caster**
-- 950 HP, 142 ND, 1.5 move speed
-- Ranged: range 5, low magic armor-furthest, `(1 ND) MD` every 1.4s
-- Melee: `(0.666 ND) MD` every 1.4s</t>
-  </si>
-  <si>
     <t>Ground Slime</t>
   </si>
   <si>
@@ -8235,6 +8220,57 @@
   </si>
   <si>
     <t>No volari perch</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/1/12/W7_enemy_01.jpg/revision/latest?cb=20210424200603</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/f/fc/W7_enemy_02.jpg/revision/latest?cb=20210424200612</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/7/72/W7_enemy_03.jpg/revision/latest?cb=20210424200619</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/f/ff/W7_enemy_04.jpg/revision/latest?cb=20210424200627</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/a/aa/W7_enemy_05.jpg/revision/latest?cb=20210424200637</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/b/b7/W7_enemy_06.jpg/revision/latest?cb=20210424200650</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/5/5d/W7_enemy_07.jpg/revision/latest?cb=20210424200700</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/9/93/RhoThrower.jpg/revision/latest?cb=20210424144426</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/7/77/CrystalKeep.jpg/revision/latest?cb=20210424144527</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/7/71/GammaSentry.jpg/revision/latest?cb=20210424144404</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/1/15/VolariPerch.jpg/revision/latest?cb=20210424144141</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/a/a5/Mercenary_Board.png/revision/latest?cb=20210424201429</t>
+  </si>
+  <si>
+    <t>By spending 900 coins you are able to hire one of the mercenary below, they will join the battle in next wave:
+**(1) Sylvan Archer**
+- 1000 HP, 30% physical armor, 10% magical armor, 150 ND, 1.5 move speed
+- Ranged: range 5, air-furthest, `(1 ND) PD` every 1.1s
+- Melee: `(0.666 ND) PD` every 1.1s
+**(2) Sylvan Fighter**
+- 1300 HP, 128 ND, 1.5 move speed
+- Melee: `(1 ND) PD`with 2 attacks, each 1.75s cooldown
+- Aura of Encouragement: haste tower troops by 50% in range 1.5
+**(3) Sylvan Caster**
+- 950 HP, 142 ND, 1.5 move speed
+- Ranged: range 5, low magic armor-furthest, `(1 ND) MD` every 1.4s
+- Melee: `(0.666 ND) MD` every 1.4s</t>
   </si>
 </sst>
 </file>
@@ -14558,7 +14594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D337"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C117" sqref="C117"/>
     </sheetView>
@@ -18857,8 +18893,8 @@
   <dimension ref="A1:H366"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E249" sqref="E249"/>
+      <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G248" sqref="G248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24898,15 +24934,15 @@
         <v>7</v>
       </c>
       <c r="C242" s="10" t="s">
-        <v>2558</v>
+        <v>2557</v>
       </c>
       <c r="D242" s="12" t="s">
-        <v>2582</v>
+        <v>2581</v>
       </c>
       <c r="E242" s="12"/>
       <c r="F242" s="14"/>
-      <c r="G242" s="18" t="s">
-        <v>2568</v>
+      <c r="G242" s="17" t="s">
+        <v>2567</v>
       </c>
       <c r="H242" s="18"/>
     </row>
@@ -24919,19 +24955,19 @@
         <v>7</v>
       </c>
       <c r="C243" s="10" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
       <c r="D243" s="12" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
       <c r="E243" s="12" t="s">
         <v>2341</v>
       </c>
       <c r="F243" s="14" t="s">
-        <v>2579</v>
+        <v>2578</v>
       </c>
       <c r="G243" s="18" t="s">
-        <v>2569</v>
+        <v>2568</v>
       </c>
       <c r="H243" s="18"/>
     </row>
@@ -24944,19 +24980,19 @@
         <v>7</v>
       </c>
       <c r="C244" s="10" t="s">
-        <v>2560</v>
+        <v>2559</v>
       </c>
       <c r="D244" s="12" t="s">
-        <v>2584</v>
+        <v>2583</v>
       </c>
       <c r="E244" s="12" t="s">
         <v>2340</v>
       </c>
       <c r="F244" s="14" t="s">
-        <v>2578</v>
+        <v>2577</v>
       </c>
       <c r="G244" s="18" t="s">
-        <v>2570</v>
+        <v>2569</v>
       </c>
       <c r="H244" s="18"/>
     </row>
@@ -24969,19 +25005,19 @@
         <v>7</v>
       </c>
       <c r="C245" s="10" t="s">
-        <v>2561</v>
+        <v>2560</v>
       </c>
       <c r="D245" s="12" t="s">
-        <v>2585</v>
+        <v>2584</v>
       </c>
       <c r="E245" s="12" t="s">
         <v>2341</v>
       </c>
       <c r="F245" s="14" t="s">
-        <v>2580</v>
+        <v>2579</v>
       </c>
       <c r="G245" s="18" t="s">
-        <v>2571</v>
+        <v>2570</v>
       </c>
       <c r="H245" s="18"/>
     </row>
@@ -24994,17 +25030,17 @@
         <v>7</v>
       </c>
       <c r="C246" s="10" t="s">
-        <v>2562</v>
+        <v>2561</v>
       </c>
       <c r="D246" s="12" t="s">
-        <v>2582</v>
+        <v>2581</v>
       </c>
       <c r="E246" s="12" t="s">
         <v>2340</v>
       </c>
       <c r="F246" s="14"/>
       <c r="G246" s="18" t="s">
-        <v>2572</v>
+        <v>2571</v>
       </c>
       <c r="H246" s="18"/>
     </row>
@@ -25017,17 +25053,17 @@
         <v>7</v>
       </c>
       <c r="C247" s="10" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="D247" s="12" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
       <c r="E247" s="12" t="s">
         <v>2341</v>
       </c>
       <c r="F247" s="14"/>
       <c r="G247" s="18" t="s">
-        <v>2573</v>
+        <v>2572</v>
       </c>
       <c r="H247" s="18"/>
     </row>
@@ -25040,19 +25076,19 @@
         <v>7</v>
       </c>
       <c r="C248" s="10" t="s">
-        <v>2564</v>
+        <v>2563</v>
       </c>
       <c r="D248" s="12" t="s">
-        <v>2584</v>
+        <v>2583</v>
       </c>
       <c r="E248" s="12" t="s">
         <v>2340</v>
       </c>
       <c r="F248" s="14" t="s">
-        <v>2581</v>
+        <v>2580</v>
       </c>
       <c r="G248" s="18" t="s">
-        <v>2574</v>
+        <v>2573</v>
       </c>
       <c r="H248" s="18"/>
     </row>
@@ -25065,17 +25101,17 @@
         <v>7</v>
       </c>
       <c r="C249" s="10" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
       <c r="D249" s="12" t="s">
-        <v>2585</v>
+        <v>2584</v>
       </c>
       <c r="E249" s="12" t="s">
         <v>2341</v>
       </c>
       <c r="F249" s="14"/>
       <c r="G249" s="18" t="s">
-        <v>2575</v>
+        <v>2574</v>
       </c>
       <c r="H249" s="18"/>
     </row>
@@ -25088,19 +25124,19 @@
         <v>7</v>
       </c>
       <c r="C250" s="10" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="D250" s="12" t="s">
-        <v>2582</v>
+        <v>2581</v>
       </c>
       <c r="E250" s="12" t="s">
         <v>2340</v>
       </c>
       <c r="F250" s="14" t="s">
-        <v>2578</v>
+        <v>2577</v>
       </c>
       <c r="G250" s="18" t="s">
-        <v>2576</v>
+        <v>2575</v>
       </c>
       <c r="H250" s="18"/>
     </row>
@@ -25113,19 +25149,19 @@
         <v>7</v>
       </c>
       <c r="C251" s="10" t="s">
-        <v>2567</v>
+        <v>2566</v>
       </c>
       <c r="D251" s="12" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
       <c r="E251" s="12" t="s">
         <v>2340</v>
       </c>
       <c r="F251" s="14" t="s">
-        <v>2578</v>
+        <v>2577</v>
       </c>
       <c r="G251" s="18" t="s">
-        <v>2577</v>
+        <v>2576</v>
       </c>
       <c r="H251" s="18"/>
     </row>
@@ -27633,9 +27669,10 @@
     <hyperlink ref="G59" r:id="rId18" xr:uid="{6AF54B96-9CFB-4CA6-AB09-165E5843E722}"/>
     <hyperlink ref="G60" r:id="rId19" xr:uid="{39F54BBD-A2A3-4C15-A9D8-3607D016A156}"/>
     <hyperlink ref="G61" r:id="rId20" xr:uid="{0459B543-5E9E-4A4D-9DC6-ABA61BA83172}"/>
+    <hyperlink ref="G242" r:id="rId21" xr:uid="{7FF9EE7A-BA9D-4E73-BFCA-EB801C90D5EC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -27644,8 +27681,8 @@
   <dimension ref="A1:N159"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L155" sqref="L155"/>
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L147" sqref="L147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32645,7 +32682,7 @@
         <v>0</v>
       </c>
       <c r="L119" s="23" t="s">
-        <v>2552</v>
+        <v>2551</v>
       </c>
       <c r="M119" s="25" t="s">
         <v>1249</v>
@@ -33720,7 +33757,7 @@
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A145" s="23" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="B145" s="26">
         <v>7</v>
@@ -33753,12 +33790,12 @@
         <v>0</v>
       </c>
       <c r="L145" s="23" t="s">
-        <v>2548</v>
+        <v>2547</v>
       </c>
     </row>
     <row r="146" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A146" s="23" t="s">
-        <v>2540</v>
+        <v>2539</v>
       </c>
       <c r="B146" s="26">
         <v>7</v>
@@ -33791,12 +33828,15 @@
         <v>0</v>
       </c>
       <c r="L146" s="23" t="s">
-        <v>2551</v>
+        <v>2550</v>
+      </c>
+      <c r="N146" s="30" t="s">
+        <v>2591</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A147" s="23" t="s">
-        <v>2541</v>
+        <v>2540</v>
       </c>
       <c r="B147" s="26">
         <v>7</v>
@@ -33829,12 +33869,15 @@
         <v>0</v>
       </c>
       <c r="L147" s="23" t="s">
-        <v>2549</v>
+        <v>2548</v>
+      </c>
+      <c r="N147" s="30" t="s">
+        <v>2587</v>
       </c>
     </row>
     <row r="148" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A148" s="23" t="s">
-        <v>2542</v>
+        <v>2541</v>
       </c>
       <c r="B148" s="26">
         <v>7</v>
@@ -33867,12 +33910,15 @@
         <v>0</v>
       </c>
       <c r="L148" s="23" t="s">
-        <v>2550</v>
+        <v>2549</v>
+      </c>
+      <c r="N148" s="30" t="s">
+        <v>2586</v>
       </c>
     </row>
     <row r="149" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A149" s="23" t="s">
-        <v>2543</v>
+        <v>2542</v>
       </c>
       <c r="B149" s="26">
         <v>7</v>
@@ -33905,12 +33951,15 @@
         <v>0</v>
       </c>
       <c r="L149" s="23" t="s">
-        <v>2553</v>
+        <v>2552</v>
+      </c>
+      <c r="N149" s="30" t="s">
+        <v>2585</v>
       </c>
     </row>
     <row r="150" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A150" s="23" t="s">
-        <v>2544</v>
+        <v>2543</v>
       </c>
       <c r="B150" s="26">
         <v>7</v>
@@ -33943,12 +33992,15 @@
         <v>0</v>
       </c>
       <c r="L150" s="23" t="s">
-        <v>2554</v>
+        <v>2553</v>
+      </c>
+      <c r="N150" s="30" t="s">
+        <v>2589</v>
       </c>
     </row>
     <row r="151" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A151" s="23" t="s">
-        <v>2545</v>
+        <v>2544</v>
       </c>
       <c r="B151" s="26">
         <v>7</v>
@@ -33981,12 +34033,15 @@
         <v>0</v>
       </c>
       <c r="L151" s="23" t="s">
-        <v>2555</v>
+        <v>2554</v>
+      </c>
+      <c r="N151" s="30" t="s">
+        <v>2588</v>
       </c>
     </row>
     <row r="152" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A152" s="23" t="s">
-        <v>2546</v>
+        <v>2545</v>
       </c>
       <c r="B152" s="26">
         <v>7</v>
@@ -34019,12 +34074,15 @@
         <v>0</v>
       </c>
       <c r="L152" s="23" t="s">
-        <v>2556</v>
+        <v>2555</v>
+      </c>
+      <c r="N152" s="30" t="s">
+        <v>2590</v>
       </c>
     </row>
     <row r="153" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A153" s="23" t="s">
-        <v>2547</v>
+        <v>2546</v>
       </c>
       <c r="B153" s="26">
         <v>7</v>
@@ -34057,7 +34115,7 @@
         <v>0</v>
       </c>
       <c r="L153" s="23" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="M153" s="25" t="s">
         <v>976</v>
@@ -34221,10 +34279,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED1689C-43D8-4482-B475-EE9D75A4CF53}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -35318,6 +35376,9 @@
       <c r="L26" s="19" t="s">
         <v>2508</v>
       </c>
+      <c r="N26" s="6" t="s">
+        <v>2592</v>
+      </c>
     </row>
     <row r="27" spans="1:14" ht="174" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
@@ -35356,6 +35417,9 @@
       <c r="L27" s="19" t="s">
         <v>2518</v>
       </c>
+      <c r="N27" s="6" t="s">
+        <v>2593</v>
+      </c>
     </row>
     <row r="28" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
@@ -35394,6 +35458,9 @@
       <c r="L28" s="19" t="s">
         <v>2525</v>
       </c>
+      <c r="N28" s="6" t="s">
+        <v>2594</v>
+      </c>
     </row>
     <row r="29" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
@@ -35432,6 +35499,9 @@
       <c r="L29" s="19" t="s">
         <v>2534</v>
       </c>
+      <c r="N29" s="6" t="s">
+        <v>2595</v>
+      </c>
     </row>
     <row r="30" spans="1:14" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
@@ -35450,7 +35520,7 @@
         <v>2504</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>2538</v>
+        <v>2597</v>
       </c>
       <c r="G30" s="19" t="s">
         <v>2535</v>
@@ -35469,6 +35539,9 @@
       </c>
       <c r="L30" s="19" t="s">
         <v>2535</v>
+      </c>
+      <c r="N30" s="6" t="s">
+        <v>2596</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
better battle cry text
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\data\q-z\Realm Defense\CyraBot\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEDF5CE2-0203-41EB-819C-7AB88A38C2F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BD8909-A490-45A3-992A-06BD3ACAA4DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hero" sheetId="1" r:id="rId1"/>
@@ -7962,9 +7962,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>7s cooldown, Hogan deals `(1 ND) PD` in melee and summons a boar which inherits his damage, and gives all summoned units a 50% speed haste for 3.5s. The boar will deal `(10 ND) PD` to a strong target and stun it for 6s</t>
-  </si>
-  <si>
     <t>Ground Slime</t>
   </si>
   <si>
@@ -8284,6 +8281,9 @@
 8⭐**Accelerator**: Cooldown is reduced to 4s, cooldowns of left/right branch spells are decreased by 5s/1s; Also reduce the cost of level upgrade and left branch by 5%
 10⭐**Volari's Acient Power**: Change the two spear warriors of Crystal Keep to one powerful Volari warrior
 (Cost/cooldown reductions are already counted in upgrades)</t>
+  </si>
+  <si>
+    <t>7s cooldown, Hogan deals `(1 ND) PD` in melee and summons a boar with 4 move speed and 1+100% damage, and gives all summoned units a 50% speed haste for 3.5s. The boar will run through the lane and deal `(10 ND) PD` to Hogan's target and stun it for 6s</t>
   </si>
 </sst>
 </file>
@@ -14607,9 +14607,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D337"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C117" sqref="C117"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16125,7 +16125,7 @@
         <v>269</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>2518</v>
+        <v>2601</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -24947,15 +24947,15 @@
         <v>7</v>
       </c>
       <c r="C242" s="10" t="s">
-        <v>2537</v>
+        <v>2536</v>
       </c>
       <c r="D242" s="12" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="E242" s="12"/>
       <c r="F242" s="14"/>
       <c r="G242" s="17" t="s">
-        <v>2547</v>
+        <v>2546</v>
       </c>
       <c r="H242" s="18"/>
     </row>
@@ -24968,19 +24968,19 @@
         <v>7</v>
       </c>
       <c r="C243" s="10" t="s">
-        <v>2538</v>
+        <v>2537</v>
       </c>
       <c r="D243" s="12" t="s">
-        <v>2558</v>
+        <v>2557</v>
       </c>
       <c r="E243" s="12" t="s">
         <v>2341</v>
       </c>
       <c r="F243" s="14" t="s">
-        <v>2574</v>
+        <v>2573</v>
       </c>
       <c r="G243" s="18" t="s">
-        <v>2548</v>
+        <v>2547</v>
       </c>
       <c r="H243" s="18"/>
     </row>
@@ -24993,19 +24993,19 @@
         <v>7</v>
       </c>
       <c r="C244" s="10" t="s">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="D244" s="12" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
       <c r="E244" s="12" t="s">
         <v>2340</v>
       </c>
       <c r="F244" s="14" t="s">
-        <v>2575</v>
+        <v>2574</v>
       </c>
       <c r="G244" s="18" t="s">
-        <v>2549</v>
+        <v>2548</v>
       </c>
       <c r="H244" s="18"/>
     </row>
@@ -25018,19 +25018,19 @@
         <v>7</v>
       </c>
       <c r="C245" s="10" t="s">
-        <v>2540</v>
+        <v>2539</v>
       </c>
       <c r="D245" s="12" t="s">
-        <v>2560</v>
+        <v>2559</v>
       </c>
       <c r="E245" s="12" t="s">
         <v>2341</v>
       </c>
       <c r="F245" s="14" t="s">
-        <v>2576</v>
+        <v>2575</v>
       </c>
       <c r="G245" s="18" t="s">
-        <v>2550</v>
+        <v>2549</v>
       </c>
       <c r="H245" s="18"/>
     </row>
@@ -25043,17 +25043,17 @@
         <v>7</v>
       </c>
       <c r="C246" s="10" t="s">
-        <v>2541</v>
+        <v>2540</v>
       </c>
       <c r="D246" s="12" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="E246" s="12" t="s">
         <v>2340</v>
       </c>
       <c r="F246" s="14"/>
       <c r="G246" s="18" t="s">
-        <v>2551</v>
+        <v>2550</v>
       </c>
       <c r="H246" s="18"/>
     </row>
@@ -25066,17 +25066,17 @@
         <v>7</v>
       </c>
       <c r="C247" s="10" t="s">
-        <v>2542</v>
+        <v>2541</v>
       </c>
       <c r="D247" s="12" t="s">
-        <v>2558</v>
+        <v>2557</v>
       </c>
       <c r="E247" s="12" t="s">
         <v>2341</v>
       </c>
       <c r="F247" s="14"/>
       <c r="G247" s="18" t="s">
-        <v>2552</v>
+        <v>2551</v>
       </c>
       <c r="H247" s="18"/>
     </row>
@@ -25089,19 +25089,19 @@
         <v>7</v>
       </c>
       <c r="C248" s="10" t="s">
-        <v>2543</v>
+        <v>2542</v>
       </c>
       <c r="D248" s="12" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
       <c r="E248" s="12" t="s">
         <v>2340</v>
       </c>
       <c r="F248" s="14" t="s">
-        <v>2577</v>
+        <v>2576</v>
       </c>
       <c r="G248" s="18" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="H248" s="18"/>
     </row>
@@ -25114,19 +25114,19 @@
         <v>7</v>
       </c>
       <c r="C249" s="10" t="s">
-        <v>2544</v>
+        <v>2543</v>
       </c>
       <c r="D249" s="12" t="s">
-        <v>2560</v>
+        <v>2559</v>
       </c>
       <c r="E249" s="12" t="s">
         <v>2341</v>
       </c>
       <c r="F249" s="14" t="s">
-        <v>2578</v>
+        <v>2577</v>
       </c>
       <c r="G249" s="18" t="s">
-        <v>2554</v>
+        <v>2553</v>
       </c>
       <c r="H249" s="18"/>
     </row>
@@ -25139,19 +25139,19 @@
         <v>7</v>
       </c>
       <c r="C250" s="10" t="s">
-        <v>2545</v>
+        <v>2544</v>
       </c>
       <c r="D250" s="12" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="E250" s="12" t="s">
         <v>2340</v>
       </c>
       <c r="F250" s="14" t="s">
-        <v>2575</v>
+        <v>2574</v>
       </c>
       <c r="G250" s="18" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="H250" s="18"/>
     </row>
@@ -25164,19 +25164,19 @@
         <v>7</v>
       </c>
       <c r="C251" s="10" t="s">
-        <v>2546</v>
+        <v>2545</v>
       </c>
       <c r="D251" s="12" t="s">
-        <v>2558</v>
+        <v>2557</v>
       </c>
       <c r="E251" s="12" t="s">
         <v>2340</v>
       </c>
       <c r="F251" s="14" t="s">
-        <v>2575</v>
+        <v>2574</v>
       </c>
       <c r="G251" s="18" t="s">
-        <v>2556</v>
+        <v>2555</v>
       </c>
       <c r="H251" s="18"/>
     </row>
@@ -32697,7 +32697,7 @@
         <v>0</v>
       </c>
       <c r="L119" s="23" t="s">
-        <v>2532</v>
+        <v>2531</v>
       </c>
       <c r="M119" s="25" t="s">
         <v>1249</v>
@@ -33772,7 +33772,7 @@
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A145" s="23" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="B145" s="26">
         <v>7</v>
@@ -33805,12 +33805,12 @@
         <v>0</v>
       </c>
       <c r="L145" s="23" t="s">
-        <v>2528</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="146" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A146" s="23" t="s">
-        <v>2520</v>
+        <v>2519</v>
       </c>
       <c r="B146" s="26">
         <v>7</v>
@@ -33843,15 +33843,15 @@
         <v>0</v>
       </c>
       <c r="L146" s="23" t="s">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="N146" s="30" t="s">
-        <v>2567</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A147" s="23" t="s">
-        <v>2521</v>
+        <v>2520</v>
       </c>
       <c r="B147" s="26">
         <v>7</v>
@@ -33884,15 +33884,15 @@
         <v>0</v>
       </c>
       <c r="L147" s="23" t="s">
-        <v>2529</v>
+        <v>2528</v>
       </c>
       <c r="N147" s="30" t="s">
-        <v>2563</v>
+        <v>2562</v>
       </c>
     </row>
     <row r="148" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A148" s="23" t="s">
-        <v>2522</v>
+        <v>2521</v>
       </c>
       <c r="B148" s="26">
         <v>7</v>
@@ -33925,15 +33925,15 @@
         <v>0</v>
       </c>
       <c r="L148" s="23" t="s">
-        <v>2530</v>
+        <v>2529</v>
       </c>
       <c r="N148" s="30" t="s">
-        <v>2562</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="149" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A149" s="23" t="s">
-        <v>2523</v>
+        <v>2522</v>
       </c>
       <c r="B149" s="26">
         <v>7</v>
@@ -33966,15 +33966,15 @@
         <v>0</v>
       </c>
       <c r="L149" s="23" t="s">
-        <v>2533</v>
+        <v>2532</v>
       </c>
       <c r="N149" s="30" t="s">
-        <v>2561</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="150" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A150" s="23" t="s">
-        <v>2524</v>
+        <v>2523</v>
       </c>
       <c r="B150" s="26">
         <v>7</v>
@@ -34007,15 +34007,15 @@
         <v>0</v>
       </c>
       <c r="L150" s="23" t="s">
-        <v>2579</v>
+        <v>2578</v>
       </c>
       <c r="N150" s="30" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
     </row>
     <row r="151" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A151" s="23" t="s">
-        <v>2525</v>
+        <v>2524</v>
       </c>
       <c r="B151" s="26">
         <v>7</v>
@@ -34048,15 +34048,15 @@
         <v>0</v>
       </c>
       <c r="L151" s="23" t="s">
-        <v>2534</v>
+        <v>2533</v>
       </c>
       <c r="N151" s="30" t="s">
-        <v>2564</v>
+        <v>2563</v>
       </c>
     </row>
     <row r="152" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A152" s="23" t="s">
-        <v>2526</v>
+        <v>2525</v>
       </c>
       <c r="B152" s="26">
         <v>7</v>
@@ -34089,15 +34089,15 @@
         <v>0</v>
       </c>
       <c r="L152" s="23" t="s">
-        <v>2535</v>
+        <v>2534</v>
       </c>
       <c r="N152" s="30" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
     </row>
     <row r="153" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A153" s="23" t="s">
-        <v>2527</v>
+        <v>2526</v>
       </c>
       <c r="B153" s="26">
         <v>7</v>
@@ -34130,7 +34130,7 @@
         <v>0</v>
       </c>
       <c r="L153" s="23" t="s">
-        <v>2536</v>
+        <v>2535</v>
       </c>
       <c r="M153" s="25" t="s">
         <v>976</v>
@@ -34294,7 +34294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED1689C-43D8-4482-B475-EE9D75A4CF53}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
@@ -34378,7 +34378,7 @@
         <v>1767</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>2585</v>
+        <v>2584</v>
       </c>
       <c r="H2" s="19" t="s">
         <v>2357</v>
@@ -34419,7 +34419,7 @@
         <v>1122</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>2586</v>
+        <v>2585</v>
       </c>
       <c r="H3" s="19" t="s">
         <v>2360</v>
@@ -34460,7 +34460,7 @@
         <v>1769</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>2587</v>
+        <v>2586</v>
       </c>
       <c r="H4" s="19" t="s">
         <v>2363</v>
@@ -34501,7 +34501,7 @@
         <v>1768</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
       <c r="H5" s="19" t="s">
         <v>2366</v>
@@ -34542,7 +34542,7 @@
         <v>1770</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>2589</v>
+        <v>2588</v>
       </c>
       <c r="H6" s="19" t="s">
         <v>2369</v>
@@ -34624,7 +34624,7 @@
         <v>2065</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>2590</v>
+        <v>2589</v>
       </c>
       <c r="H8" s="19" t="s">
         <v>2375</v>
@@ -34665,7 +34665,7 @@
         <v>1771</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>2591</v>
+        <v>2590</v>
       </c>
       <c r="H9" s="19" t="s">
         <v>2378</v>
@@ -34952,7 +34952,7 @@
         <v>1776</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>2592</v>
+        <v>2591</v>
       </c>
       <c r="H16" s="19" t="s">
         <v>2399</v>
@@ -35034,7 +35034,7 @@
         <v>1778</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>2593</v>
+        <v>2592</v>
       </c>
       <c r="H18" s="19" t="s">
         <v>2405</v>
@@ -35198,7 +35198,7 @@
         <v>1779</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>2597</v>
+        <v>2596</v>
       </c>
       <c r="H22" s="19" t="s">
         <v>2417</v>
@@ -35242,7 +35242,7 @@
         <v>1129</v>
       </c>
       <c r="G23" s="19" t="s">
-        <v>2594</v>
+        <v>2593</v>
       </c>
       <c r="H23" s="19" t="s">
         <v>2420</v>
@@ -35286,7 +35286,7 @@
         <v>1132</v>
       </c>
       <c r="G24" s="19" t="s">
-        <v>2595</v>
+        <v>2594</v>
       </c>
       <c r="H24" s="19" t="s">
         <v>2424</v>
@@ -35330,7 +35330,7 @@
         <v>2492</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>2596</v>
+        <v>2595</v>
       </c>
       <c r="H25" s="19" t="s">
         <v>2428</v>
@@ -35374,7 +35374,7 @@
         <v>2498</v>
       </c>
       <c r="G26" s="19" t="s">
-        <v>2598</v>
+        <v>2597</v>
       </c>
       <c r="H26" s="19" t="s">
         <v>2493</v>
@@ -35392,7 +35392,7 @@
         <v>2495</v>
       </c>
       <c r="N26" s="6" t="s">
-        <v>2568</v>
+        <v>2567</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="188.5" x14ac:dyDescent="0.35">
@@ -35415,10 +35415,10 @@
         <v>2497</v>
       </c>
       <c r="G27" s="19" t="s">
-        <v>2599</v>
+        <v>2598</v>
       </c>
       <c r="H27" s="19" t="s">
-        <v>2582</v>
+        <v>2581</v>
       </c>
       <c r="I27" s="19" t="s">
         <v>2502</v>
@@ -35433,7 +35433,7 @@
         <v>2503</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>2569</v>
+        <v>2568</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
@@ -35456,10 +35456,10 @@
         <v>2510</v>
       </c>
       <c r="G28" s="19" t="s">
-        <v>2600</v>
+        <v>2599</v>
       </c>
       <c r="H28" s="19" t="s">
-        <v>2584</v>
+        <v>2583</v>
       </c>
       <c r="I28" s="19" t="s">
         <v>2504</v>
@@ -35474,7 +35474,7 @@
         <v>2507</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>2570</v>
+        <v>2569</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
@@ -35497,7 +35497,7 @@
         <v>2511</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>2601</v>
+        <v>2600</v>
       </c>
       <c r="H29" s="19" t="s">
         <v>2509</v>
@@ -35515,7 +35515,7 @@
         <v>2515</v>
       </c>
       <c r="N29" s="6" t="s">
-        <v>2571</v>
+        <v>2570</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="246.5" x14ac:dyDescent="0.35">
@@ -35535,7 +35535,7 @@
         <v>2491</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>2573</v>
+        <v>2572</v>
       </c>
       <c r="G30" s="19" t="s">
         <v>2516</v>
@@ -35556,7 +35556,7 @@
         <v>2516</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>2572</v>
+        <v>2571</v>
       </c>
     </row>
   </sheetData>
@@ -35801,7 +35801,7 @@
         <v>651</v>
       </c>
       <c r="C20" t="s">
-        <v>2580</v>
+        <v>2579</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -35812,7 +35812,7 @@
         <v>973</v>
       </c>
       <c r="C21" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -35823,7 +35823,7 @@
         <v>639</v>
       </c>
       <c r="C22" t="s">
-        <v>2581</v>
+        <v>2580</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remark boss for level 210
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\data\q-z\Realm Defense\CyraBot\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4172B3CE-3BF0-472F-8ABD-E0EAA86C858E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CE676E-CD9C-4417-B9FD-59933A99165D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hero" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5330" uniqueCount="2602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5331" uniqueCount="2602">
   <si>
     <t>name</t>
   </si>
@@ -14625,7 +14625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D337"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A305" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D322" sqref="D322"/>
     </sheetView>
@@ -18923,9 +18923,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D798F71-5A72-4731-9B2C-78595D904327}">
   <dimension ref="A1:H366"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A241" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F247" sqref="F247"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A240" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H249" sqref="H249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25196,7 +25196,9 @@
       <c r="G251" s="18" t="s">
         <v>2548</v>
       </c>
-      <c r="H251" s="18"/>
+      <c r="H251" s="18" t="s">
+        <v>975</v>
+      </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A252" t="s">

</xml_diff>

<commit_message>
w7 hogan bug fix
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\data\q-z\Realm Defense\CyraBot\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A18B3CC-2A32-4A82-998F-27BE2EA3E12E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726ECDAD-1CD2-44B9-9811-41DB1946530A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hero" sheetId="1" r:id="rId1"/>
@@ -7564,12 +7564,6 @@
     <t>5s cooldown, Hogan throws an axe to an air-furthest enemy in range 3 and deals `100 TD + (1.5 SD) PD`</t>
   </si>
   <si>
-    <t>Damage is reduced to `100 TD + (1 SD) PD`, the axe has 2% chance to do a critical hit, which deals `100 TD + (3000 SD) PD` instead</t>
-  </si>
-  <si>
-    <t>Damage is reduced to `100 TD + (1 SD) PD`, the axe must bounce once, but the chance for the sequential bounces is reduced to 36%</t>
-  </si>
-  <si>
     <t>7s cooldown, pig Bacon spins an axe for 3s, deals `(9 ND) PD` and slows enemies by 50% for 0.5s in an AOE range 1.5. Bacon can cast this spell even if Hogan is moving or dead but cannot be hasted</t>
   </si>
   <si>
@@ -8025,9 +8019,6 @@
   </si>
   <si>
     <t>The Timeless Beauty. Yan, is the greatest Time Mage in existence. Her reckless ambition has gotten her into trouble uncountable times. A true lady never tells you her age, but she is far older than her beauty would lead you to believe.</t>
-  </si>
-  <si>
-    <t>30s cooldown, Hogan launches Bacon's jetpack, deals `(180+1.5 ND) PD` to enemies in AOE range 1.75 with 60% chance to stun the targets for 5s, and grounds the flying enemies for 4s (grounding not working)</t>
   </si>
   <si>
     <t>Cylindrical Device: (2x per wave, can use at wave 0) once to activate it, second time to self destruct (effect unknown)</t>
@@ -8206,14 +8197,6 @@
     <t>This spell can be upgraded by __*Fast Chop*__</t>
   </si>
   <si>
-    <t>Hogan has two friends: Bacon and boar. They have 1.5 move speed and inherit Hogan's damage but cannot be hasted. When Hogan is within range 1.5 of Bacon, he is healed `(50+1 SD)` every 2s</t>
-  </si>
-  <si>
-    <t>(1) 2s cooldown, pig Bacon launches jetpack, deals `(3 ND) PD` and slows enemies by 50% for 4s and ground flying enemies for 3s in an AOE range 2 (grounding not working)
-(2) 6s cooldown, the boar tramples, deals `(9 ND) PD` and slows enemies by 50% for 0.5s in an AOE range 1.5. 
-Bacon and the boar can cast the spells even if Hogan is moving or dead</t>
-  </si>
-  <si>
     <t>When paired with __*Bolton*__, each arrow from __*Ranged*__ has 30% chance to summon lightning, which deals `(1800+3 ND) MD` to the target and bounces once in range 4, with 35% chance to shock the original and chained target for 2s</t>
   </si>
   <si>
@@ -8254,12 +8237,6 @@
     <t>Elara spawns an aura when in __*Goddess Form*__, consistently debuffs enemies (including bosses) in AOE range 2 every 0.133s, reduces their damage by 20% for 0.033s and 3% chance terrifies them for 3s; also increases the magical armor of allies by 15% for 0.033s</t>
   </si>
   <si>
-    <t>7s cooldown, Hogan deals `(1 ND) PD` in melee and triggers the following effects:
-(1) Gives all summoned units a buff for 3.5s: speed x1.5, damage x1.1
-(2) Summons a boar at entry. The boar has 4 move speed, 1+100% damage, will run to the exit unit it hits Hogan's target. When running, with 0.667s cooldown, the boar deals `(0.5 ND) PD` to a nearest ground enemy in range 0.5. When hitting the target, the boar deals `(10 ND) PD`, stuns it for 6s, and turns into defense state for 10s. At defense state, the boar stops 2 enemies and performs melee/ranged attack which has 1.5s cooldown, and deals `(2 ND) PD` to all ground enemies within its range 1.5
-(3) Summons a flying pig at exit if there is a flying enemy. The flying pig has 4 move speed, 1+100% damage, will fly to the entry, deal `(10 ND) PD` and stun the first flying enemy for 6s</t>
-  </si>
-  <si>
     <t>When paired with __*Sethos*__, each arrow from __*Ranged*__ has 25% chance to throw a poison bomb, which applies venom for 12s and deals `20 TD + (0.6 SD) MD` every 0.42s to enemies in range 1</t>
   </si>
   <si>
@@ -8336,6 +8313,29 @@
   <si>
     <t>(1) When engaged, Hogan's move speed is increased by 40%, cast speed is increased by 80%
 (2) Each time Hogan melees, increases the critical chance of melee, 0% -&gt; 2% -&gt; 4% -&gt; 5% -&gt; 6% (max). When unengaged, critical chance is reset to 0. Critical attack deals additional `(3665 SD) MD`.</t>
+  </si>
+  <si>
+    <t>Damage is increased to `100 TD + (1.65 SD) PD`, the axe has 2% chance to do a critical hit, which deals `100 TD + (3000 SD) PD` instead</t>
+  </si>
+  <si>
+    <t>Damage is increased to `100 TD + (1.65 SD) PD`, the axe must bounce once, but the chance for the sequential bounces is reduced to 36%</t>
+  </si>
+  <si>
+    <t>30s cooldown, Hogan launches Bacon's jetpack, deals `(180+1.5 ND) PD` to enemies in AOE range 1.75 with 60% chance to stun the targets for 5s, and grounds the flying enemies for 4s</t>
+  </si>
+  <si>
+    <t>Hogan has two friends: Bacon and boar. They have 1.5 move speed and inherit Hogan's ND but cannot be hasted. When Hogan is within range 1.5 of Bacon, he is healed `(50+1 SD)` every 2s</t>
+  </si>
+  <si>
+    <t>(1) 2s cooldown, pig Bacon launches jetpack, deals `(3 ND) PD` and slows enemies by 50% for 4s and ground flying enemies for 3s in an AOE range 2
+(2) 6s cooldown, the boar tramples, deals `(9 ND) PD` and slows enemies by 50% for 0.5s in an AOE range 1.5. 
+Bacon and the boar can cast the spells even if Hogan is moving or dead</t>
+  </si>
+  <si>
+    <t>7s cooldown, Hogan deals `(1 ND) PD` in melee and triggers the following effects:
+(1) Gives all summoned units a buff for 3.5s: speed x1.5, damage x1.1
+(2) Summons a boar at entry. The boar has 4 move speed, 1+100% damage, will run to the exit unit it hits Hogan's target. When running, with 0.667s cooldown, the boar deals `(0.5 ND) PD` to a nearest ground enemy in range 0.5. When hitting the target, the boar deals `(12 ND) PD`, stuns it for 6s, and turns into defense state for 10s. At defense state, the boar stops 2 enemies and performs melee/ranged attack which has 1.5s cooldown, and deals `(2 ND) PD` to all ground enemies within its range 1.5
+(3) Summons a flying pig at exit if there is a flying enemy. The flying pig has 4 move speed, 1+100% damage, will fly to the entry, deal `(12 ND) PD` and stun the first flying enemy for 6s</t>
   </si>
 </sst>
 </file>
@@ -9013,7 +9013,7 @@
         <v>6</v>
       </c>
       <c r="X2" t="s">
-        <v>2509</v>
+        <v>2507</v>
       </c>
       <c r="Y2" s="31" t="s">
         <v>1662</v>
@@ -9090,7 +9090,7 @@
         <v>6</v>
       </c>
       <c r="X3" t="s">
-        <v>2510</v>
+        <v>2508</v>
       </c>
       <c r="Y3" s="31" t="s">
         <v>1663</v>
@@ -9167,7 +9167,7 @@
         <v>6</v>
       </c>
       <c r="X4" t="s">
-        <v>2511</v>
+        <v>2509</v>
       </c>
       <c r="Y4" s="31" t="s">
         <v>1664</v>
@@ -9244,7 +9244,7 @@
         <v>6</v>
       </c>
       <c r="X5" t="s">
-        <v>2512</v>
+        <v>2510</v>
       </c>
       <c r="Y5" s="31" t="s">
         <v>1645</v>
@@ -9321,7 +9321,7 @@
         <v>6</v>
       </c>
       <c r="X6" t="s">
-        <v>2515</v>
+        <v>2513</v>
       </c>
       <c r="Y6" s="31" t="s">
         <v>1646</v>
@@ -9398,7 +9398,7 @@
         <v>7</v>
       </c>
       <c r="X7" t="s">
-        <v>2517</v>
+        <v>2515</v>
       </c>
       <c r="Y7" s="31" t="s">
         <v>1647</v>
@@ -9475,7 +9475,7 @@
         <v>6</v>
       </c>
       <c r="X8" t="s">
-        <v>2518</v>
+        <v>2516</v>
       </c>
       <c r="Y8" s="31" t="s">
         <v>1648</v>
@@ -9552,7 +9552,7 @@
         <v>7</v>
       </c>
       <c r="X9" t="s">
-        <v>2519</v>
+        <v>2517</v>
       </c>
       <c r="Y9" s="31" t="s">
         <v>1649</v>
@@ -9629,7 +9629,7 @@
         <v>6</v>
       </c>
       <c r="X10" t="s">
-        <v>2519</v>
+        <v>2517</v>
       </c>
       <c r="Y10" s="31" t="s">
         <v>1649</v>
@@ -9706,7 +9706,7 @@
         <v>6</v>
       </c>
       <c r="X11" t="s">
-        <v>2520</v>
+        <v>2518</v>
       </c>
       <c r="Y11" s="31" t="s">
         <v>1650</v>
@@ -9783,7 +9783,7 @@
         <v>7</v>
       </c>
       <c r="X12" t="s">
-        <v>2521</v>
+        <v>2519</v>
       </c>
       <c r="Y12" s="31" t="s">
         <v>1651</v>
@@ -9860,7 +9860,7 @@
         <v>6</v>
       </c>
       <c r="X13" t="s">
-        <v>2522</v>
+        <v>2520</v>
       </c>
       <c r="Y13" s="31" t="s">
         <v>1652</v>
@@ -9937,7 +9937,7 @@
         <v>6</v>
       </c>
       <c r="X14" t="s">
-        <v>2523</v>
+        <v>2521</v>
       </c>
       <c r="Y14" s="31" t="s">
         <v>1653</v>
@@ -10014,7 +10014,7 @@
         <v>7</v>
       </c>
       <c r="X15" t="s">
-        <v>2524</v>
+        <v>2522</v>
       </c>
       <c r="Y15" s="31" t="s">
         <v>1654</v>
@@ -10091,7 +10091,7 @@
         <v>6</v>
       </c>
       <c r="X16" t="s">
-        <v>2525</v>
+        <v>2523</v>
       </c>
       <c r="Y16" s="31" t="s">
         <v>1655</v>
@@ -10168,7 +10168,7 @@
         <v>6</v>
       </c>
       <c r="X17" t="s">
-        <v>2526</v>
+        <v>2524</v>
       </c>
       <c r="Y17" s="31" t="s">
         <v>1656</v>
@@ -10245,7 +10245,7 @@
         <v>6</v>
       </c>
       <c r="X18" t="s">
-        <v>2527</v>
+        <v>2525</v>
       </c>
       <c r="Y18" s="31" t="s">
         <v>1657</v>
@@ -10322,7 +10322,7 @@
         <v>6</v>
       </c>
       <c r="X19" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="Y19" s="31" t="s">
         <v>1658</v>
@@ -10399,7 +10399,7 @@
         <v>6</v>
       </c>
       <c r="X20" t="s">
-        <v>2529</v>
+        <v>2527</v>
       </c>
       <c r="Y20" s="31" t="s">
         <v>1659</v>
@@ -10476,7 +10476,7 @@
         <v>6</v>
       </c>
       <c r="X21" t="s">
-        <v>2530</v>
+        <v>2528</v>
       </c>
       <c r="Y21" s="31" t="s">
         <v>1660</v>
@@ -10553,7 +10553,7 @@
         <v>6</v>
       </c>
       <c r="X22" t="s">
-        <v>2531</v>
+        <v>2529</v>
       </c>
       <c r="Y22" s="31" t="s">
         <v>1661</v>
@@ -10630,7 +10630,7 @@
         <v>1</v>
       </c>
       <c r="X23" t="s">
-        <v>2513</v>
+        <v>2511</v>
       </c>
       <c r="Y23" s="31" t="s">
         <v>1645</v>
@@ -10707,7 +10707,7 @@
         <v>6</v>
       </c>
       <c r="X24" t="s">
-        <v>2514</v>
+        <v>2512</v>
       </c>
       <c r="Y24" s="31" t="s">
         <v>1665</v>
@@ -10784,7 +10784,7 @@
         <v>6</v>
       </c>
       <c r="X25" t="s">
-        <v>2516</v>
+        <v>2514</v>
       </c>
       <c r="Y25" s="31" t="s">
         <v>1666</v>
@@ -11962,7 +11962,7 @@
         <v>29</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>2576</v>
+        <v>2573</v>
       </c>
       <c r="G58" s="1">
         <v>-2</v>
@@ -11988,7 +11988,7 @@
         <v>0</v>
       </c>
       <c r="I59" s="20" t="s">
-        <v>2596</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -12014,7 +12014,7 @@
         <v>1</v>
       </c>
       <c r="I60" s="20" t="s">
-        <v>2599</v>
+        <v>2593</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
@@ -12037,7 +12037,7 @@
         <v>2</v>
       </c>
       <c r="I61" s="20" t="s">
-        <v>2598</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
@@ -12060,7 +12060,7 @@
         <v>3</v>
       </c>
       <c r="I62" s="20" t="s">
-        <v>2597</v>
+        <v>2591</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -14661,9 +14661,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D339"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E116" sqref="E116"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E120" sqref="E120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15757,7 +15757,7 @@
         <v>314</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>2579</v>
+        <v>2574</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -15785,7 +15785,7 @@
         <v>312</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>2580</v>
+        <v>2575</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -15799,7 +15799,7 @@
         <v>311</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>2581</v>
+        <v>2576</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -15813,7 +15813,7 @@
         <v>310</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>2590</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="145" x14ac:dyDescent="0.35">
@@ -15827,7 +15827,7 @@
         <v>309</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>2582</v>
+        <v>2577</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -16019,7 +16019,7 @@
         <v>13</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>2383</v>
+        <v>106</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>266</v>
@@ -16039,7 +16039,7 @@
         <v>268</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>2591</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -16053,7 +16053,7 @@
         <v>317</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>2532</v>
+        <v>2606</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -16095,7 +16095,7 @@
         <v>298</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>2396</v>
+        <v>2604</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -16109,7 +16109,7 @@
         <v>317</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>2507</v>
+        <v>2505</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -16123,7 +16123,7 @@
         <v>298</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>2397</v>
+        <v>2605</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -16137,7 +16137,7 @@
         <v>317</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>2592</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
@@ -16151,7 +16151,7 @@
         <v>298</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>2609</v>
+        <v>2603</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -16162,10 +16162,10 @@
         <v>106</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>2577</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+        <v>2607</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>250</v>
       </c>
@@ -16176,7 +16176,7 @@
         <v>266</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>2578</v>
+        <v>2608</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -16204,7 +16204,7 @@
         <v>269</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>2589</v>
+        <v>2609</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -16314,7 +16314,7 @@
         <v>317</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>2508</v>
+        <v>2506</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
@@ -16370,7 +16370,7 @@
         <v>266</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>2398</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -16809,7 +16809,7 @@
         <v>317</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>2502</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -16915,7 +16915,7 @@
         <v>317</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>2503</v>
+        <v>2501</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -18668,7 +18668,7 @@
         <v>317</v>
       </c>
       <c r="D316" s="1" t="s">
-        <v>2505</v>
+        <v>2503</v>
       </c>
     </row>
     <row r="317" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -18682,7 +18682,7 @@
         <v>317</v>
       </c>
       <c r="D317" s="1" t="s">
-        <v>2504</v>
+        <v>2502</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.35">
@@ -18710,7 +18710,7 @@
         <v>317</v>
       </c>
       <c r="D319" s="1" t="s">
-        <v>2506</v>
+        <v>2504</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.35">
@@ -18794,7 +18794,7 @@
         <v>268</v>
       </c>
       <c r="D325" s="1" t="s">
-        <v>2586</v>
+        <v>2581</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.35">
@@ -18830,7 +18830,7 @@
         <v>591</v>
       </c>
       <c r="D329" s="1" t="s">
-        <v>2593</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="330" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18858,7 +18858,7 @@
         <v>317</v>
       </c>
       <c r="D331" s="1" t="s">
-        <v>2584</v>
+        <v>2579</v>
       </c>
     </row>
     <row r="332" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -18872,7 +18872,7 @@
         <v>317</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>2583</v>
+        <v>2578</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.35">
@@ -18900,7 +18900,7 @@
         <v>317</v>
       </c>
       <c r="D334" s="1" t="s">
-        <v>2595</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="335" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18914,7 +18914,7 @@
         <v>611</v>
       </c>
       <c r="D335" s="1" t="s">
-        <v>2594</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="336" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18942,7 +18942,7 @@
         <v>268</v>
       </c>
       <c r="D337" s="1" t="s">
-        <v>2585</v>
+        <v>2580</v>
       </c>
     </row>
     <row r="338" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -18956,7 +18956,7 @@
         <v>317</v>
       </c>
       <c r="D338" s="1" t="s">
-        <v>2587</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="339" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -18970,7 +18970,7 @@
         <v>267</v>
       </c>
       <c r="D339" s="1" t="s">
-        <v>2588</v>
+        <v>2583</v>
       </c>
     </row>
   </sheetData>
@@ -18984,7 +18984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED1689C-43D8-4482-B475-EE9D75A4CF53}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
@@ -19065,10 +19065,10 @@
         <v>1024</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>2537</v>
+        <v>2534</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>2490</v>
+        <v>2488</v>
       </c>
       <c r="H2" s="19" t="s">
         <v>2296</v>
@@ -19106,10 +19106,10 @@
         <v>1026</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>2538</v>
+        <v>2535</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>2491</v>
+        <v>2489</v>
       </c>
       <c r="H3" s="19" t="s">
         <v>2299</v>
@@ -19147,10 +19147,10 @@
         <v>1028</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>2565</v>
+        <v>2562</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>2492</v>
+        <v>2490</v>
       </c>
       <c r="H4" s="19" t="s">
         <v>2302</v>
@@ -19188,10 +19188,10 @@
         <v>1030</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>2539</v>
+        <v>2536</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>2493</v>
+        <v>2491</v>
       </c>
       <c r="H5" s="19" t="s">
         <v>2305</v>
@@ -19229,10 +19229,10 @@
         <v>1032</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>2540</v>
+        <v>2537</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>2494</v>
+        <v>2492</v>
       </c>
       <c r="H6" s="19" t="s">
         <v>2308</v>
@@ -19270,7 +19270,7 @@
         <v>1034</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>2541</v>
+        <v>2538</v>
       </c>
       <c r="G7" s="19" t="s">
         <v>2364</v>
@@ -19311,10 +19311,10 @@
         <v>1036</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>2542</v>
+        <v>2539</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>2495</v>
+        <v>2493</v>
       </c>
       <c r="H8" s="19" t="s">
         <v>2314</v>
@@ -19323,7 +19323,7 @@
         <v>1079</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>2566</v>
+        <v>2563</v>
       </c>
       <c r="K8" s="19" t="s">
         <v>1080</v>
@@ -19352,10 +19352,10 @@
         <v>1038</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>2543</v>
+        <v>2540</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>2496</v>
+        <v>2494</v>
       </c>
       <c r="H9" s="19" t="s">
         <v>2316</v>
@@ -19434,10 +19434,10 @@
         <v>634</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>2567</v>
+        <v>2564</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>2544</v>
+        <v>2541</v>
       </c>
       <c r="H11" s="19" t="s">
         <v>2322</v>
@@ -19475,7 +19475,7 @@
         <v>1040</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>2545</v>
+        <v>2542</v>
       </c>
       <c r="G12" s="19" t="s">
         <v>2366</v>
@@ -19516,7 +19516,7 @@
         <v>1042</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>2546</v>
+        <v>2543</v>
       </c>
       <c r="G13" s="19" t="s">
         <v>2367</v>
@@ -19557,7 +19557,7 @@
         <v>1043</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>2547</v>
+        <v>2544</v>
       </c>
       <c r="G14" s="19" t="s">
         <v>2368</v>
@@ -19575,7 +19575,7 @@
         <v>1102</v>
       </c>
       <c r="L14" s="19" t="s">
-        <v>2548</v>
+        <v>2545</v>
       </c>
       <c r="N14" s="22" t="s">
         <v>1319</v>
@@ -19598,7 +19598,7 @@
         <v>1045</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>2549</v>
+        <v>2546</v>
       </c>
       <c r="G15" s="19" t="s">
         <v>2369</v>
@@ -19639,10 +19639,10 @@
         <v>1047</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>2550</v>
+        <v>2547</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>2497</v>
+        <v>2495</v>
       </c>
       <c r="H16" s="19" t="s">
         <v>2336</v>
@@ -19680,7 +19680,7 @@
         <v>1051</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>2551</v>
+        <v>2548</v>
       </c>
       <c r="G17" s="19" t="s">
         <v>2370</v>
@@ -19692,7 +19692,7 @@
         <v>1089</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>2568</v>
+        <v>2565</v>
       </c>
       <c r="K17" s="19" t="s">
         <v>1105</v>
@@ -19721,10 +19721,10 @@
         <v>1054</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>2552</v>
+        <v>2549</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>2498</v>
+        <v>2496</v>
       </c>
       <c r="H18" s="19" t="s">
         <v>2341</v>
@@ -19762,7 +19762,7 @@
         <v>1052</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>2416</v>
+        <v>2414</v>
       </c>
       <c r="G19" s="19" t="s">
         <v>2371</v>
@@ -19803,7 +19803,7 @@
         <v>1058</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>2553</v>
+        <v>2550</v>
       </c>
       <c r="G20" s="19" t="s">
         <v>2372</v>
@@ -19844,7 +19844,7 @@
         <v>1056</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>2554</v>
+        <v>2551</v>
       </c>
       <c r="G21" s="19" t="s">
         <v>2373</v>
@@ -19888,7 +19888,7 @@
         <v>1725</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>2501</v>
+        <v>2499</v>
       </c>
       <c r="H22" s="19" t="s">
         <v>2353</v>
@@ -19932,7 +19932,7 @@
         <v>1096</v>
       </c>
       <c r="G23" s="19" t="s">
-        <v>2499</v>
+        <v>2497</v>
       </c>
       <c r="H23" s="19" t="s">
         <v>2356</v>
@@ -19947,7 +19947,7 @@
         <v>1098</v>
       </c>
       <c r="L23" s="19" t="s">
-        <v>2569</v>
+        <v>2566</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>2358</v>
@@ -19973,10 +19973,10 @@
         <v>1066</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>2555</v>
+        <v>2552</v>
       </c>
       <c r="G24" s="19" t="s">
-        <v>2556</v>
+        <v>2553</v>
       </c>
       <c r="H24" s="19" t="s">
         <v>2359</v>
@@ -19985,13 +19985,13 @@
         <v>1112</v>
       </c>
       <c r="J24" s="19" t="s">
-        <v>2557</v>
+        <v>2554</v>
       </c>
       <c r="K24" s="19" t="s">
         <v>1110</v>
       </c>
       <c r="L24" s="19" t="s">
-        <v>2558</v>
+        <v>2555</v>
       </c>
       <c r="M24" s="1" t="s">
         <v>2360</v>
@@ -20017,10 +20017,10 @@
         <v>1060</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>2559</v>
+        <v>2556</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>2500</v>
+        <v>2498</v>
       </c>
       <c r="H25" s="19" t="s">
         <v>2361</v>
@@ -20035,7 +20035,7 @@
         <v>1099</v>
       </c>
       <c r="L25" s="19" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
       <c r="M25" s="1" t="s">
         <v>2363</v>
@@ -20046,7 +20046,7 @@
     </row>
     <row r="26" spans="1:14" ht="174" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>2399</v>
+        <v>2397</v>
       </c>
       <c r="B26" s="1">
         <v>7</v>
@@ -20055,39 +20055,39 @@
         <v>624</v>
       </c>
       <c r="D26" s="19" t="s">
+        <v>2402</v>
+      </c>
+      <c r="E26" s="19" t="s">
         <v>2404</v>
       </c>
-      <c r="E26" s="19" t="s">
-        <v>2406</v>
-      </c>
       <c r="F26" s="19" t="s">
-        <v>2561</v>
+        <v>2558</v>
       </c>
       <c r="G26" s="19" t="s">
-        <v>2602</v>
+        <v>2596</v>
       </c>
       <c r="H26" s="19" t="s">
-        <v>2414</v>
+        <v>2412</v>
       </c>
       <c r="I26" s="19" t="s">
+        <v>2413</v>
+      </c>
+      <c r="J26" s="19" t="s">
         <v>2415</v>
       </c>
-      <c r="J26" s="19" t="s">
-        <v>2417</v>
-      </c>
       <c r="K26" s="19" t="s">
-        <v>2425</v>
+        <v>2423</v>
       </c>
       <c r="L26" s="19" t="s">
-        <v>2603</v>
+        <v>2597</v>
       </c>
       <c r="N26" s="6" t="s">
-        <v>2477</v>
+        <v>2475</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>2400</v>
+        <v>2398</v>
       </c>
       <c r="B27" s="1">
         <v>7</v>
@@ -20096,39 +20096,39 @@
         <v>946</v>
       </c>
       <c r="D27" s="19" t="s">
+        <v>2403</v>
+      </c>
+      <c r="E27" s="19" t="s">
         <v>2405</v>
       </c>
-      <c r="E27" s="19" t="s">
-        <v>2407</v>
-      </c>
       <c r="F27" s="19" t="s">
-        <v>2606</v>
+        <v>2600</v>
       </c>
       <c r="G27" s="19" t="s">
-        <v>2605</v>
+        <v>2599</v>
       </c>
       <c r="H27" s="19" t="s">
-        <v>2607</v>
+        <v>2601</v>
       </c>
       <c r="I27" s="19" t="s">
-        <v>2420</v>
+        <v>2418</v>
       </c>
       <c r="J27" s="19" t="s">
-        <v>2418</v>
+        <v>2416</v>
       </c>
       <c r="K27" s="19" t="s">
-        <v>2419</v>
+        <v>2417</v>
       </c>
       <c r="L27" s="19" t="s">
-        <v>2570</v>
+        <v>2567</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>2478</v>
+        <v>2476</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>2401</v>
+        <v>2399</v>
       </c>
       <c r="B28" s="1">
         <v>7</v>
@@ -20137,39 +20137,39 @@
         <v>624</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>2409</v>
+        <v>2407</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>2408</v>
+        <v>2406</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>2562</v>
+        <v>2559</v>
       </c>
       <c r="G28" s="19" t="s">
-        <v>2604</v>
+        <v>2598</v>
       </c>
       <c r="H28" s="19" t="s">
-        <v>2489</v>
+        <v>2487</v>
       </c>
       <c r="I28" s="19" t="s">
+        <v>2419</v>
+      </c>
+      <c r="J28" s="19" t="s">
+        <v>2420</v>
+      </c>
+      <c r="K28" s="19" t="s">
         <v>2421</v>
       </c>
-      <c r="J28" s="19" t="s">
+      <c r="L28" s="19" t="s">
         <v>2422</v>
       </c>
-      <c r="K28" s="19" t="s">
-        <v>2423</v>
-      </c>
-      <c r="L28" s="19" t="s">
-        <v>2424</v>
-      </c>
       <c r="N28" s="6" t="s">
-        <v>2479</v>
+        <v>2477</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>2402</v>
+        <v>2400</v>
       </c>
       <c r="B29" s="1">
         <v>7</v>
@@ -20178,39 +20178,39 @@
         <v>624</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>2411</v>
+        <v>2409</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>2412</v>
+        <v>2410</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>2563</v>
+        <v>2560</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>2572</v>
+        <v>2569</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>2608</v>
+        <v>2602</v>
       </c>
       <c r="I29" s="19" t="s">
+        <v>2424</v>
+      </c>
+      <c r="J29" s="19" t="s">
+        <v>2425</v>
+      </c>
+      <c r="K29" s="19" t="s">
         <v>2426</v>
       </c>
-      <c r="J29" s="19" t="s">
-        <v>2427</v>
-      </c>
-      <c r="K29" s="19" t="s">
-        <v>2428</v>
-      </c>
       <c r="L29" s="19" t="s">
-        <v>2571</v>
+        <v>2568</v>
       </c>
       <c r="N29" s="6" t="s">
-        <v>2480</v>
+        <v>2478</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>2403</v>
+        <v>2401</v>
       </c>
       <c r="B30" s="1">
         <v>7</v>
@@ -20219,34 +20219,34 @@
         <v>946</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>2410</v>
+        <v>2408</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>2413</v>
+        <v>2411</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>2564</v>
+        <v>2561</v>
       </c>
       <c r="G30" s="19" t="s">
-        <v>2429</v>
+        <v>2427</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>2429</v>
+        <v>2427</v>
       </c>
       <c r="I30" s="19" t="s">
-        <v>2430</v>
+        <v>2428</v>
       </c>
       <c r="J30" s="19" t="s">
-        <v>2429</v>
+        <v>2427</v>
       </c>
       <c r="K30" s="19" t="s">
-        <v>2430</v>
+        <v>2428</v>
       </c>
       <c r="L30" s="19" t="s">
-        <v>2429</v>
+        <v>2427</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>2481</v>
+        <v>2479</v>
       </c>
     </row>
   </sheetData>
@@ -24819,7 +24819,7 @@
         <v>100</v>
       </c>
       <c r="L108" s="23" t="s">
-        <v>2535</v>
+        <v>2532</v>
       </c>
       <c r="M108" s="25" t="s">
         <v>949</v>
@@ -25288,7 +25288,7 @@
         <v>0</v>
       </c>
       <c r="L119" s="23" t="s">
-        <v>2443</v>
+        <v>2441</v>
       </c>
       <c r="M119" s="25" t="s">
         <v>1214</v>
@@ -25962,7 +25962,7 @@
         <v>949</v>
       </c>
       <c r="N135" s="27" t="s">
-        <v>2575</v>
+        <v>2572</v>
       </c>
     </row>
     <row r="136" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
@@ -26363,7 +26363,7 @@
     </row>
     <row r="145" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A145" s="23" t="s">
-        <v>2431</v>
+        <v>2429</v>
       </c>
       <c r="B145" s="26">
         <v>7</v>
@@ -26396,15 +26396,15 @@
         <v>0</v>
       </c>
       <c r="L145" s="23" t="s">
-        <v>2440</v>
+        <v>2438</v>
       </c>
       <c r="N145" s="33" t="s">
-        <v>2573</v>
+        <v>2570</v>
       </c>
     </row>
     <row r="146" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A146" s="23" t="s">
-        <v>2432</v>
+        <v>2430</v>
       </c>
       <c r="B146" s="26">
         <v>7</v>
@@ -26437,15 +26437,15 @@
         <v>0</v>
       </c>
       <c r="L146" s="23" t="s">
-        <v>2442</v>
+        <v>2440</v>
       </c>
       <c r="N146" s="30" t="s">
-        <v>2476</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="147" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A147" s="23" t="s">
-        <v>2433</v>
+        <v>2431</v>
       </c>
       <c r="B147" s="26">
         <v>7</v>
@@ -26478,15 +26478,15 @@
         <v>0</v>
       </c>
       <c r="L147" s="23" t="s">
-        <v>2441</v>
+        <v>2439</v>
       </c>
       <c r="N147" s="30" t="s">
-        <v>2472</v>
+        <v>2470</v>
       </c>
     </row>
     <row r="148" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A148" s="23" t="s">
-        <v>2434</v>
+        <v>2432</v>
       </c>
       <c r="B148" s="26">
         <v>7</v>
@@ -26519,15 +26519,15 @@
         <v>0</v>
       </c>
       <c r="L148" s="23" t="s">
-        <v>2534</v>
+        <v>2531</v>
       </c>
       <c r="N148" s="30" t="s">
-        <v>2471</v>
+        <v>2469</v>
       </c>
     </row>
     <row r="149" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A149" s="23" t="s">
-        <v>2435</v>
+        <v>2433</v>
       </c>
       <c r="B149" s="26">
         <v>7</v>
@@ -26560,15 +26560,15 @@
         <v>0</v>
       </c>
       <c r="L149" s="23" t="s">
-        <v>2444</v>
+        <v>2442</v>
       </c>
       <c r="N149" s="30" t="s">
-        <v>2470</v>
+        <v>2468</v>
       </c>
     </row>
     <row r="150" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A150" s="23" t="s">
-        <v>2436</v>
+        <v>2434</v>
       </c>
       <c r="B150" s="26">
         <v>7</v>
@@ -26601,15 +26601,15 @@
         <v>0</v>
       </c>
       <c r="L150" s="23" t="s">
-        <v>2600</v>
+        <v>2594</v>
       </c>
       <c r="N150" s="30" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="151" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A151" s="23" t="s">
-        <v>2437</v>
+        <v>2435</v>
       </c>
       <c r="B151" s="26">
         <v>7</v>
@@ -26642,15 +26642,15 @@
         <v>0</v>
       </c>
       <c r="L151" s="23" t="s">
-        <v>2445</v>
+        <v>2443</v>
       </c>
       <c r="N151" s="30" t="s">
-        <v>2473</v>
+        <v>2471</v>
       </c>
     </row>
     <row r="152" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A152" s="23" t="s">
-        <v>2438</v>
+        <v>2436</v>
       </c>
       <c r="B152" s="26">
         <v>7</v>
@@ -26683,15 +26683,15 @@
         <v>0</v>
       </c>
       <c r="L152" s="23" t="s">
-        <v>2601</v>
+        <v>2595</v>
       </c>
       <c r="N152" s="30" t="s">
-        <v>2475</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="153" spans="1:14" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A153" s="23" t="s">
-        <v>2439</v>
+        <v>2437</v>
       </c>
       <c r="B153" s="26">
         <v>7</v>
@@ -26724,13 +26724,13 @@
         <v>0</v>
       </c>
       <c r="L153" s="23" t="s">
-        <v>2536</v>
+        <v>2533</v>
       </c>
       <c r="M153" s="25" t="s">
         <v>949</v>
       </c>
       <c r="N153" s="33" t="s">
-        <v>2574</v>
+        <v>2571</v>
       </c>
     </row>
     <row r="159" spans="1:14" ht="26.5" x14ac:dyDescent="0.35">
@@ -32935,15 +32935,15 @@
         <v>7</v>
       </c>
       <c r="C242" s="10" t="s">
-        <v>2446</v>
+        <v>2444</v>
       </c>
       <c r="D242" s="12" t="s">
-        <v>2466</v>
+        <v>2464</v>
       </c>
       <c r="E242" s="12"/>
       <c r="F242" s="14"/>
       <c r="G242" s="17" t="s">
-        <v>2456</v>
+        <v>2454</v>
       </c>
       <c r="H242" s="18"/>
     </row>
@@ -32956,19 +32956,19 @@
         <v>7</v>
       </c>
       <c r="C243" s="10" t="s">
-        <v>2447</v>
+        <v>2445</v>
       </c>
       <c r="D243" s="12" t="s">
-        <v>2467</v>
+        <v>2465</v>
       </c>
       <c r="E243" s="12" t="s">
         <v>2280</v>
       </c>
       <c r="F243" s="14" t="s">
-        <v>2482</v>
+        <v>2480</v>
       </c>
       <c r="G243" s="18" t="s">
-        <v>2457</v>
+        <v>2455</v>
       </c>
       <c r="H243" s="18"/>
     </row>
@@ -32981,19 +32981,19 @@
         <v>7</v>
       </c>
       <c r="C244" s="10" t="s">
-        <v>2448</v>
+        <v>2446</v>
       </c>
       <c r="D244" s="12" t="s">
-        <v>2468</v>
+        <v>2466</v>
       </c>
       <c r="E244" s="12" t="s">
         <v>2279</v>
       </c>
       <c r="F244" s="14" t="s">
-        <v>2483</v>
+        <v>2481</v>
       </c>
       <c r="G244" s="18" t="s">
-        <v>2458</v>
+        <v>2456</v>
       </c>
       <c r="H244" s="18"/>
     </row>
@@ -33006,19 +33006,19 @@
         <v>7</v>
       </c>
       <c r="C245" s="10" t="s">
-        <v>2449</v>
+        <v>2447</v>
       </c>
       <c r="D245" s="12" t="s">
-        <v>2469</v>
+        <v>2467</v>
       </c>
       <c r="E245" s="12" t="s">
         <v>2280</v>
       </c>
       <c r="F245" s="14" t="s">
-        <v>2484</v>
+        <v>2482</v>
       </c>
       <c r="G245" s="18" t="s">
-        <v>2459</v>
+        <v>2457</v>
       </c>
       <c r="H245" s="18"/>
     </row>
@@ -33031,17 +33031,17 @@
         <v>7</v>
       </c>
       <c r="C246" s="10" t="s">
-        <v>2450</v>
+        <v>2448</v>
       </c>
       <c r="D246" s="12" t="s">
-        <v>2466</v>
+        <v>2464</v>
       </c>
       <c r="E246" s="12" t="s">
         <v>2279</v>
       </c>
       <c r="F246" s="14"/>
       <c r="G246" s="18" t="s">
-        <v>2460</v>
+        <v>2458</v>
       </c>
       <c r="H246" s="18"/>
     </row>
@@ -33054,19 +33054,19 @@
         <v>7</v>
       </c>
       <c r="C247" s="10" t="s">
-        <v>2451</v>
+        <v>2449</v>
       </c>
       <c r="D247" s="12" t="s">
-        <v>2467</v>
+        <v>2465</v>
       </c>
       <c r="E247" s="12" t="s">
         <v>2280</v>
       </c>
       <c r="F247" s="14" t="s">
-        <v>2483</v>
+        <v>2481</v>
       </c>
       <c r="G247" s="18" t="s">
-        <v>2461</v>
+        <v>2459</v>
       </c>
       <c r="H247" s="18"/>
     </row>
@@ -33079,19 +33079,19 @@
         <v>7</v>
       </c>
       <c r="C248" s="10" t="s">
-        <v>2452</v>
+        <v>2450</v>
       </c>
       <c r="D248" s="12" t="s">
-        <v>2468</v>
+        <v>2466</v>
       </c>
       <c r="E248" s="12" t="s">
         <v>2279</v>
       </c>
       <c r="F248" s="14" t="s">
-        <v>2533</v>
+        <v>2530</v>
       </c>
       <c r="G248" s="18" t="s">
-        <v>2462</v>
+        <v>2460</v>
       </c>
       <c r="H248" s="18"/>
     </row>
@@ -33104,19 +33104,19 @@
         <v>7</v>
       </c>
       <c r="C249" s="10" t="s">
-        <v>2453</v>
+        <v>2451</v>
       </c>
       <c r="D249" s="12" t="s">
-        <v>2469</v>
+        <v>2467</v>
       </c>
       <c r="E249" s="12" t="s">
         <v>2280</v>
       </c>
       <c r="F249" s="14" t="s">
-        <v>2485</v>
+        <v>2483</v>
       </c>
       <c r="G249" s="18" t="s">
-        <v>2463</v>
+        <v>2461</v>
       </c>
       <c r="H249" s="18"/>
     </row>
@@ -33129,19 +33129,19 @@
         <v>7</v>
       </c>
       <c r="C250" s="10" t="s">
-        <v>2454</v>
+        <v>2452</v>
       </c>
       <c r="D250" s="12" t="s">
-        <v>2466</v>
+        <v>2464</v>
       </c>
       <c r="E250" s="12" t="s">
         <v>2279</v>
       </c>
       <c r="F250" s="14" t="s">
-        <v>2483</v>
+        <v>2481</v>
       </c>
       <c r="G250" s="18" t="s">
-        <v>2464</v>
+        <v>2462</v>
       </c>
       <c r="H250" s="18"/>
     </row>
@@ -33154,19 +33154,19 @@
         <v>7</v>
       </c>
       <c r="C251" s="10" t="s">
-        <v>2455</v>
+        <v>2453</v>
       </c>
       <c r="D251" s="12" t="s">
-        <v>2467</v>
+        <v>2465</v>
       </c>
       <c r="E251" s="12" t="s">
         <v>2279</v>
       </c>
       <c r="F251" s="14" t="s">
-        <v>2483</v>
+        <v>2481</v>
       </c>
       <c r="G251" s="18" t="s">
-        <v>2465</v>
+        <v>2463</v>
       </c>
       <c r="H251" s="18" t="s">
         <v>949</v>
@@ -35892,7 +35892,7 @@
         <v>624</v>
       </c>
       <c r="C20" t="s">
-        <v>2486</v>
+        <v>2484</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -35903,7 +35903,7 @@
         <v>946</v>
       </c>
       <c r="C21" t="s">
-        <v>2488</v>
+        <v>2486</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -35914,7 +35914,7 @@
         <v>612</v>
       </c>
       <c r="C22" t="s">
-        <v>2487</v>
+        <v>2485</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change db and constant
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\data\q-z\Realm Defense\CyraBot\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF4340D-FC32-4C86-BC84-22C05E27CC60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6670E7-7F3F-4375-BE3E-338EECE9B94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5407" uniqueCount="2634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5423" uniqueCount="2638">
   <si>
     <t>name</t>
   </si>
@@ -8425,6 +8425,18 @@
   <si>
     <t>(1) After __*Forge Weapon*__, applies an additional buff: +1000 shield points for 30s to allies without Forge Shield buff in range 3, and heals their shield points by `(0.1 ND)`
 (2) Gives __*Elara*__ and __*Cyra*__ 10% physical armor if they are on battlefield</t>
+  </si>
+  <si>
+    <t>Cooldown is reduced to 20s, damage is increased to `(200+2.05 ND) PD`, chance of stun is increased to 75%</t>
+  </si>
+  <si>
+    <t>Critical chance is increased to 3%</t>
+  </si>
+  <si>
+    <t>Damage is increased to `100 TD + (1.75 SD) PD`, the axe must bounce once, but the chance for the sequential bounces is reduced to 45%</t>
+  </si>
+  <si>
+    <t>When engaged, Hogan's move speed is increased by 30%, cast speed is increased by 70%</t>
   </si>
 </sst>
 </file>
@@ -14797,11 +14809,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D352"/>
+  <dimension ref="A1:D356"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A174" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D180" sqref="D180"/>
+      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D127" sqref="D127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16280,16 +16292,16 @@
     </row>
     <row r="116" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>110</v>
+        <v>249</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>106</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>317</v>
+        <v>34</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>2378</v>
+        <v>2634</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -16300,43 +16312,43 @@
         <v>106</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>298</v>
+        <v>317</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>2581</v>
+        <v>2378</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>106</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>317</v>
+        <v>298</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>2613</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>2581</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>106</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>298</v>
+        <v>34</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>2582</v>
+        <v>2635</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>106</v>
@@ -16345,12 +16357,12 @@
         <v>317</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>2563</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+        <v>2613</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>106</v>
@@ -16359,161 +16371,161 @@
         <v>298</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>2580</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>2582</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>250</v>
+        <v>111</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>106</v>
       </c>
+      <c r="C122" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="D122" s="1" t="s">
-        <v>2584</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+        <v>2636</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>250</v>
+        <v>113</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>106</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>266</v>
+        <v>317</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>2610</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>2563</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>106</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>261</v>
+        <v>298</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" ht="174" x14ac:dyDescent="0.35">
+        <v>2580</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>2370</v>
+        <v>113</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>106</v>
       </c>
       <c r="C125" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>2637</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A126" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>2584</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A127" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>2610</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A128" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="174" x14ac:dyDescent="0.35">
+      <c r="A129" s="1" t="s">
+        <v>2370</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C129" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="D125" s="1" t="s">
+      <c r="D129" s="1" t="s">
         <v>2585</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A127" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>2366</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A128" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>2366</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>1676</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A129" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>2366</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A130" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>2366</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>435</v>
-      </c>
-    </row>
+    <row r="130" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>249</v>
+        <v>13</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>2366</v>
       </c>
-      <c r="C131" s="1" t="s">
-        <v>298</v>
-      </c>
       <c r="D131" s="1" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
-        <v>110</v>
+        <v>13</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>2366</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>317</v>
+        <v>266</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
-        <v>110</v>
+        <v>13</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>2366</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>298</v>
+        <v>268</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
-        <v>111</v>
+        <v>249</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>2366</v>
@@ -16522,12 +16534,12 @@
         <v>317</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>2614</v>
+        <v>435</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
-        <v>111</v>
+        <v>249</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>2366</v>
@@ -16536,12 +16548,12 @@
         <v>298</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>2366</v>
@@ -16550,12 +16562,12 @@
         <v>317</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>2366</v>
@@ -16564,271 +16576,271 @@
         <v>298</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>250</v>
+        <v>111</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>2366</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>266</v>
+        <v>317</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>2379</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>2614</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>2366</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>261</v>
+        <v>298</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.35"/>
+        <v>438</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A140" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>2366</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
     <row r="141" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>2366</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A142" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>2366</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>2379</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A143" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>2366</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="145" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A145" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D141" s="1" t="s">
-        <v>2606</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A142" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>1678</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A143" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C143" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A144" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="D144" s="1" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A145" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C145" s="1" t="s">
-        <v>267</v>
-      </c>
       <c r="D145" s="1" t="s">
-        <v>398</v>
+        <v>2606</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
-        <v>119</v>
+        <v>14</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C146" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="D146" s="1" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>266</v>
+        <v>317</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>268</v>
+        <v>401</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>1589</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>1679</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>401</v>
+        <v>317</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>1680</v>
+        <v>600</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>317</v>
+        <v>266</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="154" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A153" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>401</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>2600</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
-        <v>251</v>
+        <v>123</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>317</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A157" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>597</v>
-      </c>
-    </row>
+        <v>551</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="158" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
-        <v>251</v>
+        <v>13</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C158" s="1" t="s">
-        <v>316</v>
-      </c>
       <c r="D158" s="1" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>42</v>
@@ -16837,12 +16849,12 @@
         <v>317</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>1681</v>
+        <v>595</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
-        <v>252</v>
+        <v>127</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>42</v>
@@ -16851,340 +16863,340 @@
         <v>298</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>266</v>
+        <v>315</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>347</v>
+        <v>597</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
-        <v>131</v>
+        <v>251</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>442</v>
+        <v>598</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
-        <v>131</v>
+        <v>252</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>298</v>
+        <v>317</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>1681</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
-        <v>133</v>
+        <v>252</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>317</v>
+        <v>298</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>1682</v>
+        <v>441</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
-        <v>133</v>
+        <v>252</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>298</v>
+        <v>266</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D166" s="3" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>317</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>261</v>
+        <v>298</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>1683</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="169" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A168" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
-        <v>13</v>
+        <v>133</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>139</v>
+        <v>42</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>298</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>2601</v>
+        <v>444</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A171" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>1683</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="173" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A173" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C170" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="D170" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A171" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="D171" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A172" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C172" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="D172" s="1" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" ht="87" x14ac:dyDescent="0.35">
-      <c r="A173" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C173" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="D173" s="1" t="s">
-        <v>2618</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>2601</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
-        <v>141</v>
+        <v>13</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>139</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
-        <v>253</v>
+        <v>13</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>139</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D175" s="3" t="s">
-        <v>445</v>
+        <v>303</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
-        <v>146</v>
+        <v>13</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>139</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>139</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>261</v>
+        <v>317</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>1207</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+        <v>2618</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
-        <v>2628</v>
+        <v>141</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="D178" s="3" t="s">
-        <v>2633</v>
+        <v>317</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A179" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A181" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A182" s="1" t="s">
+        <v>2628</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D182" s="3" t="s">
+        <v>2633</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A184" s="1" t="s">
         <v>1576</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D180" s="1" t="s">
-        <v>1660</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A181" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D181" s="1" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A182" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B182" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C182" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="D182" s="1" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A183" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B183" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C183" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D183" s="1" t="s">
-        <v>2483</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A184" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C184" s="1" t="s">
-        <v>298</v>
-      </c>
       <c r="D184" s="1" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
-        <v>153</v>
+        <v>13</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C185" s="1" t="s">
-        <v>317</v>
+        <v>43</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
-        <v>153</v>
+        <v>13</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>298</v>
+        <v>268</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A187" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>43</v>
@@ -17193,12 +17205,12 @@
         <v>317</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
+        <v>2483</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A188" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>43</v>
@@ -17207,26 +17219,26 @@
         <v>298</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A189" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>43</v>
+        <v>156</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>317</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A190" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>43</v>
@@ -17235,160 +17247,160 @@
         <v>298</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A191" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>269</v>
+        <v>317</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>2615</v>
+        <v>452</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A192" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>2616</v>
+        <v>298</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>2617</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A193" s="1" t="s">
-        <v>254</v>
+        <v>158</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>261</v>
+        <v>317</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A194" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A195" s="1" t="s">
-        <v>1579</v>
+        <v>158</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>269</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>2602</v>
+        <v>2615</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A196" s="1" t="s">
-        <v>13</v>
+        <v>158</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>2616</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>456</v>
+        <v>2617</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A197" s="1" t="s">
-        <v>13</v>
+        <v>254</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A198" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B198" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C198" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="D198" s="1" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A199" s="1" t="s">
-        <v>162</v>
+        <v>1579</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C199" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="D199" s="1" t="s">
-        <v>1657</v>
+        <v>2602</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
-        <v>162</v>
+        <v>13</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C200" s="1" t="s">
-        <v>298</v>
-      </c>
       <c r="D200" s="1" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A201" s="1" t="s">
-        <v>164</v>
+        <v>13</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>317</v>
+        <v>260</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.35">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="s">
-        <v>164</v>
+        <v>13</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>459</v>
+        <v>381</v>
       </c>
     </row>
     <row r="203" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A203" s="1" t="s">
-        <v>255</v>
+        <v>162</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>44</v>
@@ -17397,12 +17409,12 @@
         <v>317</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>460</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A204" s="1" t="s">
-        <v>255</v>
+        <v>162</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>44</v>
@@ -17411,12 +17423,12 @@
         <v>298</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A205" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>44</v>
@@ -17425,12 +17437,12 @@
         <v>317</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>393</v>
+        <v>458</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A206" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>44</v>
@@ -17439,270 +17451,270 @@
         <v>298</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.35">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A207" s="1" t="s">
-        <v>167</v>
+        <v>255</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>266</v>
+        <v>317</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A208" s="1" t="s">
-        <v>167</v>
+        <v>255</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C208" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A209" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A210" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A211" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A212" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C212" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="D208" s="1" t="s">
+      <c r="D212" s="1" t="s">
         <v>1652</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="210" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A210" s="1" t="s">
+    <row r="213" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="214" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A214" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B210" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D210" s="1" t="s">
-        <v>2596</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A211" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B211" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C211" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D211" s="1" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A212" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B212" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C212" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D212" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A213" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B213" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C213" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="D213" s="1" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A214" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C214" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="D214" s="1" t="s">
-        <v>1684</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.35">
+        <v>2596</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A215" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>169</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>298</v>
+        <v>317</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>356</v>
+        <v>382</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A216" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>169</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A217" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>169</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>462</v>
+        <v>383</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A218" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>169</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>298</v>
+        <v>317</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="219" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A219" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>169</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>317</v>
+        <v>298</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>464</v>
+        <v>356</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A220" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>169</v>
       </c>
       <c r="C220" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A221" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A222" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C222" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="D220" s="1" t="s">
+      <c r="D222" s="1" t="s">
         <v>463</v>
-      </c>
-    </row>
-    <row r="222" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A222" s="1" t="s">
-        <v>1566</v>
-      </c>
-      <c r="B222" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D222" s="1" t="s">
-        <v>1661</v>
       </c>
     </row>
     <row r="223" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A223" s="1" t="s">
-        <v>13</v>
+        <v>176</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>178</v>
+        <v>169</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>317</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>2597</v>
-      </c>
-    </row>
-    <row r="224" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>317</v>
+        <v>298</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A225" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B225" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C225" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D225" s="1" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.35">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A226" s="1" t="s">
-        <v>179</v>
+        <v>1566</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C226" s="1" t="s">
-        <v>267</v>
-      </c>
       <c r="D226" s="1" t="s">
-        <v>358</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="227" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A227" s="1" t="s">
-        <v>179</v>
+        <v>13</v>
       </c>
       <c r="B227" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C227" s="1" t="s">
-        <v>261</v>
-      </c>
       <c r="D227" s="1" t="s">
-        <v>467</v>
+        <v>2597</v>
       </c>
     </row>
     <row r="228" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>178</v>
@@ -17711,12 +17723,12 @@
         <v>317</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>1685</v>
+        <v>465</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A229" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>178</v>
@@ -17725,68 +17737,68 @@
         <v>298</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="230" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A230" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>178</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>1686</v>
+        <v>358</v>
       </c>
     </row>
     <row r="231" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A231" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B231" s="1" t="s">
         <v>178</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.35">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A232" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B232" s="1" t="s">
         <v>178</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>267</v>
+        <v>317</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>1685</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A233" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B233" s="1" t="s">
         <v>178</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>268</v>
+        <v>298</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>1986</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A234" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B234" s="1" t="s">
         <v>178</v>
@@ -17795,12 +17807,12 @@
         <v>317</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A235" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B235" s="1" t="s">
         <v>178</v>
@@ -17809,90 +17821,90 @@
         <v>298</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>359</v>
+        <v>469</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A236" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D236" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="237" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A237" s="1" t="s">
-        <v>1581</v>
+        <v>183</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>187</v>
+        <v>178</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>268</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>1662</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="238" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A238" s="1" t="s">
-        <v>13</v>
+        <v>185</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>187</v>
+        <v>178</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>317</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>2608</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A239" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>317</v>
+        <v>298</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A240" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B240" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C240" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="D240" s="1" t="s">
-        <v>384</v>
+        <v>359</v>
       </c>
     </row>
     <row r="241" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A241" s="1" t="s">
-        <v>190</v>
+        <v>1581</v>
       </c>
       <c r="B241" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C241" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="D241" s="1" t="s">
-        <v>473</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="242" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A242" s="1" t="s">
-        <v>192</v>
+        <v>13</v>
       </c>
       <c r="B242" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C242" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="D242" s="1" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.35">
+        <v>2608</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A243" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>187</v>
@@ -17901,174 +17913,174 @@
         <v>317</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.35">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A244" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B244" s="1" t="s">
         <v>187</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>360</v>
+        <v>384</v>
       </c>
     </row>
     <row r="245" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A245" s="1" t="s">
-        <v>288</v>
+        <v>190</v>
       </c>
       <c r="B245" s="1" t="s">
         <v>187</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>266</v>
+        <v>317</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
     </row>
     <row r="246" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A246" s="1" t="s">
-        <v>288</v>
+        <v>192</v>
       </c>
       <c r="B246" s="1" t="s">
         <v>187</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>261</v>
+        <v>317</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="248" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A247" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A248" s="1" t="s">
-        <v>1574</v>
+        <v>194</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>196</v>
+        <v>187</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>1663</v>
+        <v>360</v>
       </c>
     </row>
     <row r="249" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A249" s="1" t="s">
-        <v>13</v>
+        <v>288</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>196</v>
+        <v>187</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>266</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>2598</v>
-      </c>
-    </row>
-    <row r="250" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A250" s="1" t="s">
-        <v>197</v>
+        <v>288</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>317</v>
+        <v>261</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>1664</v>
-      </c>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A251" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B251" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C251" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D251" s="1" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.35">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A252" s="1" t="s">
-        <v>197</v>
+        <v>1574</v>
       </c>
       <c r="B252" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C252" s="1" t="s">
-        <v>268</v>
-      </c>
       <c r="D252" s="1" t="s">
-        <v>361</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="253" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A253" s="1" t="s">
-        <v>199</v>
+        <v>13</v>
       </c>
       <c r="B253" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C253" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D253" s="3" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="254" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="D253" s="1" t="s">
+        <v>2598</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A254" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B254" s="1" t="s">
         <v>196</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>298</v>
+        <v>317</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="255" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A255" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B255" s="1" t="s">
         <v>196</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>317</v>
+        <v>298</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A256" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B256" s="1" t="s">
         <v>196</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>298</v>
+        <v>268</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>480</v>
+        <v>361</v>
       </c>
     </row>
     <row r="257" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A257" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B257" s="1" t="s">
         <v>196</v>
@@ -18076,13 +18088,13 @@
       <c r="C257" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="D257" s="1" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D257" s="3" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A258" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B258" s="1" t="s">
         <v>196</v>
@@ -18091,411 +18103,411 @@
         <v>298</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="259" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A259" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B259" s="1" t="s">
         <v>196</v>
       </c>
       <c r="C259" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D259" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A260" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D260" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A261" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D261" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A262" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D262" s="1" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A263" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C263" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D259" s="1" t="s">
+      <c r="D263" s="1" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="260" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="261" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A261" s="1" t="s">
+    <row r="264" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="265" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A265" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B261" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D261" s="1" t="s">
-        <v>2599</v>
-      </c>
-    </row>
-    <row r="262" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A262" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B262" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C262" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D262" s="1" t="s">
-        <v>1687</v>
-      </c>
-    </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A263" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B263" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C263" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D263" s="1" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="264" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A264" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B264" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C264" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D264" s="1" t="s">
-        <v>1989</v>
-      </c>
-    </row>
-    <row r="265" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A265" s="1" t="s">
-        <v>256</v>
       </c>
       <c r="B265" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C265" s="1" t="s">
-        <v>298</v>
-      </c>
       <c r="D265" s="1" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="266" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+        <v>2599</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A266" s="1" t="s">
-        <v>256</v>
+        <v>14</v>
       </c>
       <c r="B266" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>267</v>
+        <v>317</v>
       </c>
       <c r="D266" s="1" t="s">
-        <v>1331</v>
-      </c>
-    </row>
-    <row r="267" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A267" s="1" t="s">
-        <v>257</v>
+        <v>14</v>
       </c>
       <c r="B267" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>317</v>
+        <v>298</v>
       </c>
       <c r="D267" s="1" t="s">
-        <v>1558</v>
-      </c>
-    </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.35">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A268" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B268" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>298</v>
+        <v>317</v>
       </c>
       <c r="D268" s="1" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="269" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+        <v>1989</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A269" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B269" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>267</v>
+        <v>298</v>
       </c>
       <c r="D269" s="1" t="s">
-        <v>1330</v>
-      </c>
-    </row>
-    <row r="270" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A270" s="1" t="s">
-        <v>208</v>
+        <v>256</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>1559</v>
-      </c>
-    </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A271" s="1" t="s">
-        <v>208</v>
+        <v>257</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>298</v>
+        <v>317</v>
       </c>
       <c r="D271" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="272" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A272" s="1" t="s">
-        <v>208</v>
+        <v>257</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>267</v>
+        <v>298</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="273" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A273" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B273" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="D273" s="1" t="s">
-        <v>1560</v>
-      </c>
-    </row>
-    <row r="274" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A274" s="1" t="s">
-        <v>258</v>
+        <v>208</v>
       </c>
       <c r="B274" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>298</v>
+        <v>317</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="275" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A275" s="1" t="s">
-        <v>258</v>
+        <v>208</v>
       </c>
       <c r="B275" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>267</v>
+        <v>298</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>1328</v>
-      </c>
-    </row>
-    <row r="276" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A276" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B276" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="D276" s="1" t="s">
-        <v>2365</v>
-      </c>
-    </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A277" s="1" t="s">
-        <v>214</v>
+        <v>258</v>
       </c>
       <c r="B277" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>266</v>
+        <v>317</v>
       </c>
       <c r="D277" s="1" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="278" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A278" s="1" t="s">
-        <v>216</v>
+        <v>258</v>
       </c>
       <c r="B278" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>268</v>
+        <v>298</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="279" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A279" s="1" t="s">
-        <v>217</v>
+        <v>258</v>
       </c>
       <c r="B279" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>1208</v>
-      </c>
-    </row>
-    <row r="280" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35"/>
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A280" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D280" s="1" t="s">
+        <v>2365</v>
+      </c>
+    </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A281" s="1" t="s">
-        <v>13</v>
+        <v>214</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>219</v>
+        <v>45</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>266</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>483</v>
+        <v>390</v>
       </c>
     </row>
     <row r="282" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A282" s="1" t="s">
-        <v>14</v>
+        <v>216</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>219</v>
+        <v>45</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>268</v>
       </c>
       <c r="D282" s="1" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="283" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A283" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>219</v>
+        <v>45</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>317</v>
+        <v>261</v>
       </c>
       <c r="D283" s="1" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A284" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B284" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C284" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D284" s="1" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="285" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A285" s="1" t="s">
-        <v>220</v>
+        <v>13</v>
       </c>
       <c r="B285" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C285" s="1" t="s">
-        <v>268</v>
-      </c>
       <c r="D285" s="1" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="286" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A286" s="1" t="s">
-        <v>222</v>
+        <v>14</v>
       </c>
       <c r="B286" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C286" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="D286" s="1" t="s">
-        <v>1689</v>
-      </c>
-    </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A287" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B287" s="1" t="s">
         <v>219</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>298</v>
+        <v>317</v>
       </c>
       <c r="D287" s="1" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="288" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A288" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B288" s="1" t="s">
         <v>219</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>317</v>
+        <v>298</v>
       </c>
       <c r="D288" s="1" t="s">
-        <v>1690</v>
-      </c>
-    </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.35">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A289" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B289" s="1" t="s">
         <v>219</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>298</v>
+        <v>268</v>
       </c>
       <c r="D289" s="1" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="290" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A290" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B290" s="1" t="s">
         <v>219</v>
@@ -18504,12 +18516,12 @@
         <v>317</v>
       </c>
       <c r="D290" s="1" t="s">
-        <v>1691</v>
-      </c>
-    </row>
-    <row r="291" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>1689</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A291" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B291" s="1" t="s">
         <v>219</v>
@@ -18518,119 +18530,119 @@
         <v>298</v>
       </c>
       <c r="D291" s="1" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="292" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A292" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B292" s="1" t="s">
         <v>219</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="D292" s="3" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="293" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>317</v>
+      </c>
+      <c r="D292" s="1" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A293" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B293" s="1" t="s">
         <v>219</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>261</v>
+        <v>298</v>
       </c>
       <c r="D293" s="1" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="294" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.35">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A294" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D294" s="1" t="s">
+        <v>1691</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A295" s="1" t="s">
-        <v>13</v>
+        <v>226</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>231</v>
+        <v>219</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>298</v>
       </c>
       <c r="D295" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="296" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A296" s="1" t="s">
-        <v>14</v>
+        <v>228</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D296" s="1" t="s">
-        <v>1692</v>
+        <v>219</v>
+      </c>
+      <c r="C296" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D296" s="3" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="297" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A297" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="C297" s="1" t="s">
-        <v>317</v>
+        <v>261</v>
       </c>
       <c r="D297" s="1" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A298" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="B298" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C298" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D298" s="1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="299" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A299" s="1" t="s">
-        <v>259</v>
+        <v>13</v>
       </c>
       <c r="B299" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C299" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="D299" s="1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.35">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A300" s="1" t="s">
-        <v>259</v>
+        <v>14</v>
       </c>
       <c r="B300" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C300" s="1" t="s">
-        <v>298</v>
-      </c>
       <c r="D300" s="1" t="s">
-        <v>1325</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="301" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A301" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B301" s="1" t="s">
         <v>231</v>
@@ -18639,12 +18651,12 @@
         <v>317</v>
       </c>
       <c r="D301" s="1" t="s">
-        <v>1693</v>
+        <v>594</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A302" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B302" s="1" t="s">
         <v>231</v>
@@ -18653,12 +18665,12 @@
         <v>298</v>
       </c>
       <c r="D302" s="1" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="303" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A303" s="1" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="B303" s="1" t="s">
         <v>231</v>
@@ -18667,12 +18679,12 @@
         <v>317</v>
       </c>
       <c r="D303" s="1" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="304" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A304" s="1" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="B304" s="1" t="s">
         <v>231</v>
@@ -18681,115 +18693,115 @@
         <v>298</v>
       </c>
       <c r="D304" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A305" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B305" s="1" t="s">
         <v>231</v>
       </c>
       <c r="C305" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D305" s="1" t="s">
+        <v>1693</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A306" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B306" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C306" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D306" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A307" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C307" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D307" s="1" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A308" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B308" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C308" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D308" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A309" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B309" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C309" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D305" s="1" t="s">
+      <c r="D309" s="1" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="307" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A307" s="1" t="s">
+    <row r="311" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A311" s="1" t="s">
         <v>1570</v>
-      </c>
-      <c r="B307" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="D307" s="1" t="s">
-        <v>1658</v>
-      </c>
-    </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A308" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B308" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="D308" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="309" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A309" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B309" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="D309" s="1" t="s">
-        <v>1695</v>
-      </c>
-    </row>
-    <row r="310" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A310" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="B310" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C310" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D310" s="4" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="311" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A311" s="1" t="s">
-        <v>318</v>
       </c>
       <c r="B311" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C311" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D311" s="4" t="s">
-        <v>336</v>
+      <c r="D311" s="1" t="s">
+        <v>1658</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A312" s="1" t="s">
-        <v>320</v>
+        <v>13</v>
       </c>
       <c r="B312" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C312" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="D312" s="1" t="s">
-        <v>1696</v>
-      </c>
-    </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.35">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A313" s="1" t="s">
-        <v>320</v>
+        <v>14</v>
       </c>
       <c r="B313" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C313" s="1" t="s">
-        <v>298</v>
-      </c>
       <c r="D313" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="314" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>1695</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A314" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B314" s="1" t="s">
         <v>275</v>
@@ -18797,13 +18809,13 @@
       <c r="C314" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="D314" s="1" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D314" s="4" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A315" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B315" s="1" t="s">
         <v>275</v>
@@ -18811,13 +18823,13 @@
       <c r="C315" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="D315" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="316" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="D315" s="4" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A316" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B316" s="1" t="s">
         <v>275</v>
@@ -18826,12 +18838,12 @@
         <v>317</v>
       </c>
       <c r="D316" s="1" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A317" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B317" s="1" t="s">
         <v>275</v>
@@ -18840,132 +18852,132 @@
         <v>298</v>
       </c>
       <c r="D317" s="1" t="s">
-        <v>364</v>
+        <v>392</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A318" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C318" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D318" s="1" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A319" s="1" t="s">
-        <v>1583</v>
+        <v>321</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>552</v>
+        <v>275</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>298</v>
       </c>
       <c r="D319" s="1" t="s">
-        <v>1585</v>
-      </c>
-    </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.35">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A320" s="1" t="s">
-        <v>13</v>
+        <v>322</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>552</v>
+        <v>275</v>
+      </c>
+      <c r="C320" s="1" t="s">
+        <v>317</v>
       </c>
       <c r="D320" s="1" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="321" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>1697</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A321" s="1" t="s">
-        <v>13</v>
+        <v>322</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>552</v>
+        <v>275</v>
       </c>
       <c r="C321" s="1" t="s">
-        <v>577</v>
+        <v>298</v>
       </c>
       <c r="D321" s="1" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A322" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B322" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="C322" s="1" t="s">
-        <v>578</v>
-      </c>
-      <c r="D322" s="1" t="s">
-        <v>579</v>
+        <v>364</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A323" s="1" t="s">
-        <v>13</v>
+        <v>1583</v>
       </c>
       <c r="B323" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="C323" s="1" t="s">
-        <v>267</v>
-      </c>
       <c r="D323" s="1" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="324" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A324" s="1" t="s">
-        <v>553</v>
+        <v>13</v>
       </c>
       <c r="B324" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="C324" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="D324" s="1" t="s">
-        <v>2612</v>
-      </c>
-    </row>
-    <row r="325" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A325" s="1" t="s">
-        <v>553</v>
+        <v>13</v>
       </c>
       <c r="B325" s="1" t="s">
         <v>552</v>
       </c>
       <c r="C325" s="1" t="s">
-        <v>269</v>
+        <v>577</v>
       </c>
       <c r="D325" s="1" t="s">
-        <v>2631</v>
-      </c>
-    </row>
-    <row r="326" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A326" s="1" t="s">
-        <v>565</v>
+        <v>13</v>
       </c>
       <c r="B326" s="1" t="s">
         <v>552</v>
       </c>
       <c r="C326" s="1" t="s">
-        <v>317</v>
+        <v>578</v>
       </c>
       <c r="D326" s="1" t="s">
-        <v>2484</v>
+        <v>579</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A327" s="1" t="s">
-        <v>565</v>
+        <v>13</v>
       </c>
       <c r="B327" s="1" t="s">
         <v>552</v>
       </c>
       <c r="C327" s="1" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="D327" s="1" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="328" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A328" s="1" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B328" s="1" t="s">
         <v>552</v>
@@ -18974,52 +18986,52 @@
         <v>317</v>
       </c>
       <c r="D328" s="1" t="s">
-        <v>2485</v>
-      </c>
-    </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.35">
+        <v>2612</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A329" s="1" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B329" s="1" t="s">
         <v>552</v>
       </c>
       <c r="C329" s="1" t="s">
-        <v>602</v>
+        <v>269</v>
       </c>
       <c r="D329" s="1" t="s">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="330" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>2631</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A330" s="1" t="s">
-        <v>555</v>
+        <v>565</v>
       </c>
       <c r="B330" s="1" t="s">
         <v>552</v>
       </c>
       <c r="C330" s="1" t="s">
-        <v>577</v>
+        <v>317</v>
       </c>
       <c r="D330" s="1" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="331" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>2484</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A331" s="1" t="s">
-        <v>555</v>
+        <v>565</v>
       </c>
       <c r="B331" s="1" t="s">
         <v>552</v>
       </c>
       <c r="C331" s="1" t="s">
-        <v>578</v>
+        <v>261</v>
       </c>
       <c r="D331" s="1" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.35">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A332" s="1" t="s">
         <v>555</v>
       </c>
@@ -19027,177 +19039,177 @@
         <v>552</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>267</v>
+        <v>317</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="333" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>2485</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A333" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B333" s="1" t="s">
         <v>552</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>317</v>
+        <v>602</v>
       </c>
       <c r="D333" s="1" t="s">
-        <v>969</v>
-      </c>
-    </row>
-    <row r="334" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A334" s="1" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="B334" s="1" t="s">
         <v>552</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>268</v>
+        <v>577</v>
       </c>
       <c r="D334" s="1" t="s">
-        <v>2559</v>
-      </c>
-    </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.35">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A335" s="1" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="B335" s="1" t="s">
         <v>552</v>
       </c>
       <c r="C335" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="D335" s="1" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A336" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B336" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="C336" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D336" s="1" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A337" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="C337" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D337" s="1" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+      <c r="A338" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D338" s="1" t="s">
+        <v>2559</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A339" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B339" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="C339" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="D335" s="1" t="s">
+      <c r="D339" s="1" t="s">
         <v>2619</v>
       </c>
     </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A337" s="1" t="s">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A341" s="1" t="s">
         <v>1583</v>
-      </c>
-      <c r="B337" s="1" t="s">
-        <v>561</v>
-      </c>
-      <c r="D337" s="1" t="s">
-        <v>1586</v>
-      </c>
-    </row>
-    <row r="338" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A338" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B338" s="1" t="s">
-        <v>561</v>
-      </c>
-      <c r="D338" s="1" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="339" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A339" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B339" s="1" t="s">
-        <v>561</v>
-      </c>
-      <c r="C339" s="1" t="s">
-        <v>582</v>
-      </c>
-      <c r="D339" s="1" t="s">
-        <v>2564</v>
-      </c>
-    </row>
-    <row r="340" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A340" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B340" s="1" t="s">
-        <v>561</v>
-      </c>
-      <c r="C340" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="D340" s="1" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="341" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A341" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="B341" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="C341" s="1" t="s">
-        <v>269</v>
-      </c>
       <c r="D341" s="1" t="s">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="342" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A342" s="1" t="s">
-        <v>562</v>
+        <v>13</v>
       </c>
       <c r="B342" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="C342" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="D342" s="1" t="s">
-        <v>2557</v>
+        <v>586</v>
       </c>
     </row>
     <row r="343" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A343" s="1" t="s">
-        <v>562</v>
+        <v>13</v>
       </c>
       <c r="B343" s="1" t="s">
         <v>561</v>
       </c>
       <c r="C343" s="1" t="s">
-        <v>269</v>
+        <v>582</v>
       </c>
       <c r="D343" s="1" t="s">
-        <v>2632</v>
-      </c>
-    </row>
-    <row r="344" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>2564</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A344" s="1" t="s">
-        <v>565</v>
+        <v>13</v>
       </c>
       <c r="B344" s="1" t="s">
         <v>561</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>317</v>
+        <v>577</v>
       </c>
       <c r="D344" s="1" t="s">
-        <v>2556</v>
-      </c>
-    </row>
-    <row r="345" spans="1:4" x14ac:dyDescent="0.35">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A345" s="1" t="s">
-        <v>565</v>
+        <v>13</v>
       </c>
       <c r="B345" s="1" t="s">
         <v>561</v>
       </c>
       <c r="C345" s="1" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="D345" s="1" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="346" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>2621</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4" ht="116" x14ac:dyDescent="0.35">
       <c r="A346" s="1" t="s">
-        <v>571</v>
+        <v>562</v>
       </c>
       <c r="B346" s="1" t="s">
         <v>561</v>
@@ -19206,52 +19218,52 @@
         <v>317</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>2566</v>
-      </c>
-    </row>
-    <row r="347" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>2557</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A347" s="1" t="s">
-        <v>571</v>
+        <v>562</v>
       </c>
       <c r="B347" s="1" t="s">
         <v>561</v>
       </c>
       <c r="C347" s="1" t="s">
-        <v>602</v>
+        <v>269</v>
       </c>
       <c r="D347" s="1" t="s">
-        <v>2565</v>
-      </c>
-    </row>
-    <row r="348" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>2632</v>
+      </c>
+    </row>
+    <row r="348" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A348" s="1" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="B348" s="1" t="s">
         <v>561</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>577</v>
+        <v>317</v>
       </c>
       <c r="D348" s="1" t="s">
-        <v>583</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A349" s="1" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="B349" s="1" t="s">
         <v>561</v>
       </c>
       <c r="C349" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="D349" s="1" t="s">
-        <v>2558</v>
-      </c>
-    </row>
-    <row r="350" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A350" s="1" t="s">
         <v>571</v>
       </c>
@@ -19259,37 +19271,93 @@
         <v>561</v>
       </c>
       <c r="C350" s="1" t="s">
-        <v>269</v>
+        <v>317</v>
       </c>
       <c r="D350" s="1" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="351" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+        <v>2566</v>
+      </c>
+    </row>
+    <row r="351" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A351" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B351" s="1" t="s">
         <v>561</v>
       </c>
       <c r="C351" s="1" t="s">
-        <v>317</v>
+        <v>602</v>
       </c>
       <c r="D351" s="1" t="s">
-        <v>2560</v>
-      </c>
-    </row>
-    <row r="352" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+        <v>2565</v>
+      </c>
+    </row>
+    <row r="352" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A352" s="1" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="B352" s="1" t="s">
         <v>561</v>
       </c>
       <c r="C352" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="D352" s="1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="353" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A353" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="B353" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="C353" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D353" s="1" t="s">
+        <v>2558</v>
+      </c>
+    </row>
+    <row r="354" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A354" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="C354" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D354" s="1" t="s">
+        <v>2620</v>
+      </c>
+    </row>
+    <row r="355" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A355" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B355" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="C355" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D355" s="1" t="s">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="356" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A356" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B356" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="C356" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="D352" s="1" t="s">
+      <c r="D356" s="1" t="s">
         <v>2611</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update Cyra/Elara R7 description
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\data\q-z\Realm Defense\CyraBot\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91510287-7EF5-488E-B479-2C34B17B65F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2987BD3-9C81-4E53-8AE4-48F3A0796B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hero" sheetId="1" r:id="rId1"/>
@@ -8390,12 +8390,6 @@
     <t>Agent of Chaos</t>
   </si>
   <si>
-    <t>Summon __*Elara*__ for a coordinated strike, Elara will trigger __*Comic Flux*__, transform to goddess form with divine protection, and then fight with Cyra for 12s</t>
-  </si>
-  <si>
-    <t>Summon __*Cyra*__ for a coordinated strike, Cyra will trigger __*Photon Launch*__ landing effect, transform to goddess form with divine protection, and then fight with Elara for 12s</t>
-  </si>
-  <si>
     <t>(1) After __*Forge Weapon*__, applies an additional buff: +1000 shield points for 30s to allies without Forge Shield buff in range 3, and heals their shield points by `(0.1 ND)`
 (2) Gives __*Elara*__ and __*Cyra*__ 10% physical armor if they are on battlefield</t>
   </si>
@@ -8443,6 +8437,12 @@
   </si>
   <si>
     <t>(200💰) 15s cooldown, the tower terrifies 3 furthest enemies in range 2.5 for 5s. The terror effect is nerfed to enemies that are affected by terror multiple times: 5s-&gt;4.75s-&gt;4.25s-&gt;3.5s</t>
+  </si>
+  <si>
+    <t>Summon __*Cyra*__ (unkillable) for a coordinated strike at **where you place Elara lastly**, Cyra will trigger __*Photon Launch*__ landing effect, transform to goddess form with divine protection,and disappear 12s after using the active</t>
+  </si>
+  <si>
+    <t>Summon __*Elara*__ (unkillable) for a coordinated strike at the target location, Elara will trigger __*Comic Flux*__, transform to goddess form with divine protection, and disappear 12s after using the active</t>
   </si>
 </sst>
 </file>
@@ -14817,9 +14817,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D356"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E95" sqref="E95"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A320" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D328" sqref="D328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16053,7 +16053,7 @@
         <v>309</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>2636</v>
+        <v>2634</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -16307,7 +16307,7 @@
         <v>34</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>2627</v>
+        <v>2625</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -16349,7 +16349,7 @@
         <v>34</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>2628</v>
+        <v>2626</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -16391,7 +16391,7 @@
         <v>34</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>2629</v>
+        <v>2627</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -16433,7 +16433,7 @@
         <v>34</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>2630</v>
+        <v>2628</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -17161,7 +17161,7 @@
         <v>269</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>2626</v>
+        <v>2624</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -17211,7 +17211,7 @@
         <v>317</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>2632</v>
+        <v>2630</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
@@ -17225,7 +17225,7 @@
         <v>298</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>2635</v>
+        <v>2633</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -17295,7 +17295,7 @@
         <v>317</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>2633</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -17309,7 +17309,7 @@
         <v>298</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>2634</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.35">
@@ -19006,7 +19006,7 @@
         <v>269</v>
       </c>
       <c r="D329" s="1" t="s">
-        <v>2624</v>
+        <v>2637</v>
       </c>
     </row>
     <row r="330" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -19238,7 +19238,7 @@
         <v>269</v>
       </c>
       <c r="D347" s="1" t="s">
-        <v>2625</v>
+        <v>2636</v>
       </c>
     </row>
     <row r="348" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -19364,7 +19364,7 @@
         <v>267</v>
       </c>
       <c r="D356" s="1" t="s">
-        <v>2631</v>
+        <v>2629</v>
       </c>
     </row>
   </sheetData>
@@ -19378,7 +19378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED1689C-43D8-4482-B475-EE9D75A4CF53}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
@@ -19723,7 +19723,7 @@
         <v>1068</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>2637</v>
+        <v>2635</v>
       </c>
       <c r="N8" s="22" t="s">
         <v>1314</v>

</xml_diff>

<commit_message>
new patch bug fix
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\data\q-z\Realm Defense\CyraBot\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D303BF8-6CA1-48F1-814E-77BD28D43CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9B4AC5-47AF-4796-B3AE-9F380B4150F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hero" sheetId="1" r:id="rId1"/>
@@ -8341,12 +8341,6 @@
     <t>10s cooldown, Sethos digs into the ground and moves to the designated location, deals `250 TD + (0.5 SD) PD` and stuns for 3s to enemies within range 1 of the trajectory, then he rises up, damages and stuns ground enemies in AOE range 1</t>
   </si>
   <si>
-    <t>When paired with __*Helios*__, in addition to the original effect:
-(1) Gains 15% chance to affect each flying enemy
-(2) At each trigger, selects 2 non-boss enemies, each of them has 2% chance to be inflicted "Dust Devils" effect
-(3) "Dust Devils" effect: when affected, the target receives `(1 SD) PD` and gets stun for 2s. During the next 18s, every 0.033s, deals `(0.033 SD) PD` to enemies within its range 0.5 (totally 54 times)</t>
-  </si>
-  <si>
     <t>Tank
 Opportunistic Strike</t>
   </si>
@@ -8523,20 +8517,12 @@
     <t>Melee attack decreases the armor of enemies by x0.8 for 4s</t>
   </si>
   <si>
-    <t>45s cooldown, Osan slams the ground and
-(1) Deals `(8 SD) PD` to enemies in range 3 and blind them (miss +50%) for 10s
-(2) Gains cloak for 18s</t>
-  </si>
-  <si>
     <t>Also gives 12s cloak buff to allies in range 2.75</t>
   </si>
   <si>
     <t>Range is increased to 5</t>
   </si>
   <si>
-    <t>8s cooldown, Osan throws poison grenades to a furthest enemy in range 3.5, in 5s deals totally `(12.75 SD) TD` at the location, and applies 3s poison to the affected enemies with `(1.5 SD) TD` every 0.42s</t>
-  </si>
-  <si>
     <t>10s cooldown, Broto throws emp grenades to a furthest enemy in range 3.5, deals `(8 SD) MD` to enemies in AOE range 1.5 and shocks them for 3s</t>
   </si>
   <si>
@@ -8544,10 +8530,6 @@
   </si>
   <si>
     <t>Improve ally heroes' poison, including Mabyn, Sethos, and Fee R7 with them</t>
-  </si>
-  <si>
-    <t>Osan is able to use two melee attacks: One with 1.6s cooldown, deals `(6 ND) PD` twice to a ground enemy; The other with 3s coodlown, deals `(8 ND) PD` to ground enemies in AOE range 1.5
-- When cloaked, the two attacks above will do crit hits (no damage increase now)</t>
   </si>
   <si>
     <t>Osan has a friend Broto fighting with him. Broto has 1.5 move speed, inherits stats from Osan and can not be targeted. It has a basic range skill:
@@ -8569,6 +8551,24 @@
   </si>
   <si>
     <t>When using her active, Shamiko stops engaging, gains cloak for 2.167s and plays a song, next time she will play the next one. __*Protective Psalm*__ will apply a shield buff (shield +50, physicalArmor +40% for 10s) to other heros in range 3.5</t>
+  </si>
+  <si>
+    <t>When paired with __*Helios*__, in addition to the original effect:
+(1) Gains 15% chance to affect each flying enemy
+(2) At each trigger, selects 2 non-boss enemies, each of them has 2% chance to be inflicted "Dust Devils" effect
+(3) "Dust Devils" effect: when affected, the target receives `(1 SD) PD` and gets stun for 2s. During the next 18s, consistently deals `(1.8 SD) PD` to enemies within its range 0.5</t>
+  </si>
+  <si>
+    <t>40s cooldown, Osan slams the ground and
+(1) Deals `(8 SD) PD` to enemies in range 3 and blind them (miss +50%) for 10s
+(2) Gains cloak for 18s</t>
+  </si>
+  <si>
+    <t>Osan is able to use two melee attacks: One with 1.6s cooldown, deals `(6 ND) PD` twice to a ground enemy; The other with 3s coodlown, deals `(8 ND) PD` to ground enemies in AOE range 1.5
+- When cloaked, the two attacks above will do crit hits, dealing `(12 ND) PD` and `(8 ND) PD` respectively</t>
+  </si>
+  <si>
+    <t>8s cooldown, Osan throws poison grenades to a furthest enemy in range 3.5, in 5s deals totally `(12.75 SD) TD` in AOE range 2.5 at the location, and applies 3s poison to the affected enemies with `(1.5 SD) TD` every 0.42s</t>
   </si>
 </sst>
 </file>
@@ -11025,7 +11025,7 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="B26">
         <v>7</v>
@@ -11094,10 +11094,10 @@
         <v>7</v>
       </c>
       <c r="X26" t="s">
+        <v>2637</v>
+      </c>
+      <c r="Y26" s="31" t="s">
         <v>2638</v>
-      </c>
-      <c r="Y26" s="31" t="s">
-        <v>2639</v>
       </c>
     </row>
   </sheetData>
@@ -13804,7 +13804,7 @@
         <v>-2</v>
       </c>
       <c r="H137" s="1" t="s">
-        <v>2606</v>
+        <v>2605</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -14922,7 +14922,7 @@
         <v>13</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>26</v>
@@ -14934,38 +14934,38 @@
         <v>-2</v>
       </c>
       <c r="H196" s="1" t="s">
-        <v>2655</v>
+        <v>2654</v>
       </c>
     </row>
     <row r="197" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A197" s="1" t="s">
-        <v>2640</v>
+        <v>2639</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>2646</v>
+        <v>2645</v>
       </c>
       <c r="G197" s="1">
         <v>0</v>
       </c>
       <c r="H197" s="1" t="s">
-        <v>2656</v>
+        <v>2655</v>
       </c>
       <c r="I197" s="20" t="s">
-        <v>2660</v>
+        <v>2659</v>
       </c>
     </row>
     <row r="198" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A198" s="1" t="s">
-        <v>2641</v>
+        <v>2640</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>27</v>
@@ -14974,24 +14974,24 @@
         <v>34</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>2647</v>
+        <v>2646</v>
       </c>
       <c r="F198" s="1" t="s">
-        <v>2653</v>
+        <v>2652</v>
       </c>
       <c r="G198" s="1">
         <v>1</v>
       </c>
       <c r="I198" s="20" t="s">
-        <v>2659</v>
+        <v>2658</v>
       </c>
     </row>
     <row r="199" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A199" s="1" t="s">
-        <v>2642</v>
+        <v>2641</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>27</v>
@@ -15000,50 +15000,50 @@
         <v>35</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>2648</v>
+        <v>2647</v>
       </c>
       <c r="G199" s="1">
         <v>2</v>
       </c>
       <c r="H199" s="1" t="s">
-        <v>2654</v>
+        <v>2653</v>
       </c>
       <c r="I199" s="20" t="s">
-        <v>2658</v>
+        <v>2657</v>
       </c>
     </row>
     <row r="200" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
-        <v>2643</v>
+        <v>2642</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>2652</v>
+        <v>2651</v>
       </c>
       <c r="D200" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="G200" s="1">
         <v>3</v>
       </c>
       <c r="H200" s="1" t="s">
-        <v>2654</v>
+        <v>2653</v>
       </c>
       <c r="I200" s="20" t="s">
-        <v>2657</v>
+        <v>2656</v>
       </c>
     </row>
     <row r="201" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A201" s="1" t="s">
-        <v>2644</v>
+        <v>2643</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>28</v>
@@ -15052,7 +15052,7 @@
         <v>267</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>2650</v>
+        <v>2649</v>
       </c>
       <c r="G201" s="1">
         <v>4</v>
@@ -15060,10 +15060,10 @@
     </row>
     <row r="202" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="s">
-        <v>2645</v>
+        <v>2644</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>27</v>
@@ -15072,7 +15072,7 @@
         <v>269</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>2651</v>
+        <v>2650</v>
       </c>
       <c r="G202" s="1">
         <v>5</v>
@@ -15187,8 +15187,8 @@
   <dimension ref="A1:D368"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C256" sqref="C256"/>
+      <pane ySplit="1" topLeftCell="A361" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D368" sqref="D368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15221,7 +15221,7 @@
         <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2562</v>
@@ -15235,7 +15235,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2326</v>
@@ -15375,7 +15375,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>2333</v>
@@ -15383,7 +15383,7 @@
     </row>
     <row r="14" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C14" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -15394,7 +15394,7 @@
         <v>46</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>386</v>
@@ -15408,7 +15408,7 @@
         <v>46</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>1641</v>
@@ -15598,7 +15598,7 @@
     </row>
     <row r="30" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C30" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -15609,7 +15609,7 @@
         <v>58</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>2566</v>
@@ -15623,7 +15623,7 @@
         <v>58</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>2614</v>
+        <v>2613</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>299</v>
@@ -15743,7 +15743,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C41" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -15754,7 +15754,7 @@
         <v>70</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>1630</v>
@@ -15768,7 +15768,7 @@
         <v>70</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>397</v>
@@ -15796,7 +15796,7 @@
         <v>70</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>1637</v>
@@ -15986,7 +15986,7 @@
     </row>
     <row r="59" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C59" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
@@ -15997,7 +15997,7 @@
         <v>41</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>401</v>
@@ -16011,7 +16011,7 @@
         <v>41</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>1642</v>
@@ -16229,7 +16229,7 @@
     </row>
     <row r="77" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C77" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
@@ -16240,7 +16240,7 @@
         <v>89</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>406</v>
@@ -16254,7 +16254,7 @@
         <v>247</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>1643</v>
@@ -16408,7 +16408,7 @@
         <v>89</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>2615</v>
+        <v>2614</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>2518</v>
@@ -16422,7 +16422,7 @@
         <v>89</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>2616</v>
+        <v>2615</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>1501</v>
@@ -16436,7 +16436,7 @@
         <v>89</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>2617</v>
+        <v>2616</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>2519</v>
@@ -16450,7 +16450,7 @@
         <v>89</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>2618</v>
+        <v>2617</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>2520</v>
@@ -16464,10 +16464,10 @@
         <v>89</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>2619</v>
+        <v>2618</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>2609</v>
+        <v>2608</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
@@ -16478,15 +16478,15 @@
         <v>89</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>2620</v>
+        <v>2619</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>2610</v>
+        <v>2609</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C96" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -16497,7 +16497,7 @@
         <v>98</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>1631</v>
@@ -16511,7 +16511,7 @@
         <v>98</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>411</v>
@@ -16525,7 +16525,7 @@
         <v>98</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>1646</v>
@@ -16673,7 +16673,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C110" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
@@ -16684,7 +16684,7 @@
         <v>106</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>418</v>
@@ -16838,7 +16838,7 @@
         <v>106</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>2543</v>
@@ -16888,7 +16888,7 @@
     </row>
     <row r="126" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C126" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
@@ -16899,7 +16899,7 @@
         <v>2335</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>418</v>
@@ -17075,7 +17075,7 @@
     </row>
     <row r="140" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C140" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -17086,7 +17086,7 @@
         <v>40</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>2565</v>
@@ -17100,7 +17100,7 @@
         <v>40</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>1649</v>
@@ -17128,7 +17128,7 @@
         <v>40</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>2621</v>
+        <v>2620</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>424</v>
@@ -17212,7 +17212,7 @@
         <v>40</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>2621</v>
+        <v>2620</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>1651</v>
@@ -17248,7 +17248,7 @@
     </row>
     <row r="153" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C153" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -17259,7 +17259,7 @@
         <v>42</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>2559</v>
@@ -17301,7 +17301,7 @@
         <v>42</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>2622</v>
+        <v>2621</v>
       </c>
       <c r="D157" s="1" t="s">
         <v>573</v>
@@ -17315,7 +17315,7 @@
         <v>42</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>2623</v>
+        <v>2622</v>
       </c>
       <c r="D158" s="1" t="s">
         <v>574</v>
@@ -17449,7 +17449,7 @@
     </row>
     <row r="168" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C168" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -17460,7 +17460,7 @@
         <v>139</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D169" s="1" t="s">
         <v>2560</v>
@@ -17474,7 +17474,7 @@
         <v>139</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>2624</v>
+        <v>2623</v>
       </c>
       <c r="D170" s="1" t="s">
         <v>335</v>
@@ -17488,7 +17488,7 @@
         <v>139</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>2625</v>
+        <v>2624</v>
       </c>
       <c r="D171" s="1" t="s">
         <v>336</v>
@@ -17502,7 +17502,7 @@
         <v>139</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>2626</v>
+        <v>2625</v>
       </c>
       <c r="D172" s="1" t="s">
         <v>364</v>
@@ -17594,7 +17594,7 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C179" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -17605,7 +17605,7 @@
         <v>43</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D180" s="1" t="s">
         <v>1632</v>
@@ -17619,7 +17619,7 @@
         <v>43</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D181" s="1" t="s">
         <v>431</v>
@@ -17675,10 +17675,10 @@
         <v>43</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>2627</v>
+        <v>2626</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>2611</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -17773,10 +17773,10 @@
         <v>43</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>2627</v>
+        <v>2626</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>2611</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.35">
@@ -17801,7 +17801,7 @@
         <v>43</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>2628</v>
+        <v>2627</v>
       </c>
       <c r="D194" s="1" t="s">
         <v>2573</v>
@@ -17823,7 +17823,7 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C196" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="197" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -17834,7 +17834,7 @@
         <v>44</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D197" s="1" t="s">
         <v>2561</v>
@@ -17848,7 +17848,7 @@
         <v>44</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D198" s="1" t="s">
         <v>437</v>
@@ -18024,7 +18024,7 @@
     </row>
     <row r="211" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C211" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="212" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18035,7 +18035,7 @@
         <v>169</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D212" s="1" t="s">
         <v>2555</v>
@@ -18077,7 +18077,7 @@
         <v>169</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>2629</v>
+        <v>2628</v>
       </c>
       <c r="D215" s="1" t="s">
         <v>368</v>
@@ -18119,7 +18119,7 @@
         <v>169</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>2630</v>
+        <v>2629</v>
       </c>
       <c r="D218" s="1" t="s">
         <v>343</v>
@@ -18183,7 +18183,7 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C223" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="224" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18194,7 +18194,7 @@
         <v>178</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D224" s="1" t="s">
         <v>1633</v>
@@ -18208,7 +18208,7 @@
         <v>178</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D225" s="1" t="s">
         <v>2556</v>
@@ -18384,7 +18384,7 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C238" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="239" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18395,7 +18395,7 @@
         <v>187</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D239" s="1" t="s">
         <v>1634</v>
@@ -18409,7 +18409,7 @@
         <v>187</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D240" s="1" t="s">
         <v>2567</v>
@@ -18529,7 +18529,7 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C249" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="250" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18540,7 +18540,7 @@
         <v>196</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D250" s="1" t="s">
         <v>1635</v>
@@ -18554,7 +18554,7 @@
         <v>196</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D251" s="1" t="s">
         <v>2557</v>
@@ -18571,7 +18571,7 @@
         <v>268</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>2607</v>
+        <v>2606</v>
       </c>
     </row>
     <row r="253" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -18655,7 +18655,7 @@
         <v>298</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="259" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18666,10 +18666,10 @@
         <v>196</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>2627</v>
+        <v>2626</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>2612</v>
+        <v>2611</v>
       </c>
     </row>
     <row r="260" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18711,7 +18711,7 @@
         <v>261</v>
       </c>
       <c r="D262" s="1" t="s">
-        <v>2608</v>
+        <v>2607</v>
       </c>
     </row>
     <row r="263" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
@@ -18722,15 +18722,15 @@
         <v>196</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>2631</v>
+        <v>2630</v>
       </c>
       <c r="D263" s="1" t="s">
-        <v>2605</v>
+        <v>2672</v>
       </c>
     </row>
     <row r="264" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C264" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="265" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -18741,7 +18741,7 @@
         <v>45</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D265" s="1" t="s">
         <v>2558</v>
@@ -18786,7 +18786,7 @@
         <v>303</v>
       </c>
       <c r="D268" s="1" t="s">
-        <v>2672</v>
+        <v>2668</v>
       </c>
     </row>
     <row r="269" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18828,7 +18828,7 @@
         <v>303</v>
       </c>
       <c r="D271" s="1" t="s">
-        <v>2673</v>
+        <v>2669</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.35">
@@ -18870,7 +18870,7 @@
         <v>303</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>2674</v>
+        <v>2670</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.35">
@@ -18912,7 +18912,7 @@
         <v>303</v>
       </c>
       <c r="D277" s="1" t="s">
-        <v>2675</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="278" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -19001,7 +19001,7 @@
     </row>
     <row r="284" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C284" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.35">
@@ -19012,7 +19012,7 @@
         <v>219</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D285" s="1" t="s">
         <v>463</v>
@@ -19026,7 +19026,7 @@
         <v>219</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D286" s="1" t="s">
         <v>1659</v>
@@ -19188,7 +19188,7 @@
     </row>
     <row r="298" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C298" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.35">
@@ -19199,7 +19199,7 @@
         <v>231</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D299" s="1" t="s">
         <v>469</v>
@@ -19213,7 +19213,7 @@
         <v>231</v>
       </c>
       <c r="C300" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D300" s="1" t="s">
         <v>1663</v>
@@ -19347,7 +19347,7 @@
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C310" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="311" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -19358,7 +19358,7 @@
         <v>275</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D311" s="1" t="s">
         <v>1630</v>
@@ -19372,7 +19372,7 @@
         <v>275</v>
       </c>
       <c r="C312" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D312" s="1" t="s">
         <v>397</v>
@@ -19386,7 +19386,7 @@
         <v>275</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D313" s="1" t="s">
         <v>1666</v>
@@ -19506,7 +19506,7 @@
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C322" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.35">
@@ -19517,7 +19517,7 @@
         <v>531</v>
       </c>
       <c r="C323" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D323" s="1" t="s">
         <v>1557</v>
@@ -19531,7 +19531,7 @@
         <v>531</v>
       </c>
       <c r="C324" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D324" s="1" t="s">
         <v>557</v>
@@ -19545,7 +19545,7 @@
         <v>531</v>
       </c>
       <c r="C325" s="1" t="s">
-        <v>2636</v>
+        <v>2635</v>
       </c>
       <c r="D325" s="1" t="s">
         <v>559</v>
@@ -19559,7 +19559,7 @@
         <v>531</v>
       </c>
       <c r="C326" s="1" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
       <c r="D326" s="1" t="s">
         <v>556</v>
@@ -19657,7 +19657,7 @@
         <v>531</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>2634</v>
+        <v>2633</v>
       </c>
       <c r="D333" s="1" t="s">
         <v>943</v>
@@ -19671,7 +19671,7 @@
         <v>531</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>2636</v>
+        <v>2635</v>
       </c>
       <c r="D334" s="1" t="s">
         <v>560</v>
@@ -19685,7 +19685,7 @@
         <v>531</v>
       </c>
       <c r="C335" s="1" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
       <c r="D335" s="1" t="s">
         <v>942</v>
@@ -19749,7 +19749,7 @@
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C340" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.35">
@@ -19760,7 +19760,7 @@
         <v>540</v>
       </c>
       <c r="C341" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D341" s="1" t="s">
         <v>1558</v>
@@ -19774,7 +19774,7 @@
         <v>540</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="D342" s="1" t="s">
         <v>562</v>
@@ -19788,7 +19788,7 @@
         <v>540</v>
       </c>
       <c r="C343" s="1" t="s">
-        <v>2635</v>
+        <v>2634</v>
       </c>
       <c r="D343" s="1" t="s">
         <v>2527</v>
@@ -19802,7 +19802,7 @@
         <v>540</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>2636</v>
+        <v>2635</v>
       </c>
       <c r="D344" s="1" t="s">
         <v>559</v>
@@ -19900,7 +19900,7 @@
         <v>540</v>
       </c>
       <c r="C351" s="1" t="s">
-        <v>2634</v>
+        <v>2633</v>
       </c>
       <c r="D351" s="1" t="s">
         <v>2528</v>
@@ -19914,7 +19914,7 @@
         <v>540</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>2636</v>
+        <v>2635</v>
       </c>
       <c r="D352" s="1" t="s">
         <v>559</v>
@@ -19976,15 +19976,15 @@
         <v>2590</v>
       </c>
     </row>
-    <row r="358" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A358" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="D358" s="1" t="s">
-        <v>2669</v>
+        <v>2674</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.35">
@@ -19992,127 +19992,127 @@
         <v>13</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="C359" s="1" t="s">
         <v>268</v>
       </c>
       <c r="D359" s="1" t="s">
-        <v>2661</v>
+        <v>2660</v>
       </c>
     </row>
     <row r="360" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A360" s="1" t="s">
-        <v>2640</v>
+        <v>2639</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="D360" s="1" t="s">
-        <v>2662</v>
+        <v>2673</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A361" s="1" t="s">
-        <v>2640</v>
+        <v>2639</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="C361" s="1" t="s">
         <v>261</v>
       </c>
       <c r="D361" s="1" t="s">
-        <v>2663</v>
+        <v>2661</v>
       </c>
     </row>
     <row r="362" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A362" s="1" t="s">
-        <v>2641</v>
+        <v>2640</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="D362" s="1" t="s">
-        <v>2670</v>
+        <v>2666</v>
       </c>
     </row>
     <row r="363" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A363" s="1" t="s">
-        <v>2642</v>
+        <v>2641</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="D363" s="1" t="s">
-        <v>2665</v>
+        <v>2675</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A364" s="1" t="s">
-        <v>2642</v>
+        <v>2641</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="C364" s="1" t="s">
         <v>266</v>
       </c>
       <c r="D364" s="1" t="s">
-        <v>2664</v>
+        <v>2662</v>
       </c>
     </row>
     <row r="365" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A365" s="1" t="s">
-        <v>2643</v>
+        <v>2642</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="D365" s="1" t="s">
-        <v>2666</v>
+        <v>2663</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A366" s="1" t="s">
-        <v>2643</v>
+        <v>2642</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="C366" s="1" t="s">
         <v>266</v>
       </c>
       <c r="D366" s="1" t="s">
-        <v>2667</v>
+        <v>2664</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A367" s="1" t="s">
-        <v>2644</v>
+        <v>2643</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="C367" s="1" t="s">
         <v>267</v>
       </c>
       <c r="D367" s="1" t="s">
-        <v>2668</v>
+        <v>2665</v>
       </c>
     </row>
     <row r="368" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A368" s="1" t="s">
-        <v>2645</v>
+        <v>2644</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="C368" s="1" t="s">
         <v>269</v>
       </c>
       <c r="D368" s="1" t="s">
-        <v>2671</v>
+        <v>2667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix some old version data
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\data\q-z\Realm Defense\CyraBot\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5401B5E9-44E7-427F-A045-11299684F67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9204DED-210A-4DA9-86BF-75F57E0B12B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hero" sheetId="1" r:id="rId1"/>
@@ -8309,12 +8309,6 @@
     <t>When using her active, Shamiko stops engaging, gains cloak for 2.167s and plays a song, next time she will play the next one. __*Protective Psalm*__ will apply a shield buff (shield +50, physicalArmor +40% for 10s) to other heros in range 3.5</t>
   </si>
   <si>
-    <t>When paired with __*Helios*__, in addition to the original effect:
-(1) Gains 15% chance to affect each flying enemy
-(2) At each trigger, selects 2 non-boss enemies, each of them has 2% chance to be inflicted "Dust Devils" effect
-(3) "Dust Devils" effect: when affected, the target receives `(1 SD) PD` and gets stun for 2s. During the next 18s, consistently deals `(1.8 SD) PD` to enemies within its range 0.5</t>
-  </si>
-  <si>
     <t>poison immunity</t>
   </si>
   <si>
@@ -8547,6 +8541,12 @@
 (2) Then bursts and deals `(30 ND) PD + (5 SD) MD` to enemies in AOE range 2 with 70% chance to slow by 50% for 6s or 30% chance to terrify for 6s
 (3) Transforms to __*Goddess Form*__ and starts __*imposing aura*__, triggers pulses of rifts from __*Galactic Burst*__
 (4) Gains divine protection immunity for 3/6/9s at rank 2/4/6</t>
+  </si>
+  <si>
+    <t>When paired with __*Helios*__, in addition to the original effect:
+(1) Gains 15% chance to affect each flying enemy
+(2) At each trigger, selects 2 non-boss enemies, each of them has 2% chance to be inflicted "Dust Devils" effect
+(3) "Dust Devils" effect: when affected, the target receives `(1 SD) PD` and gets stun for 2s. During the next 1.8s, consistently deals `(1.8 SD) PD` to enemies within range 0.5 of the location</t>
   </si>
 </sst>
 </file>
@@ -11115,7 +11115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H203"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A192" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E196" sqref="E196"/>
     </sheetView>
@@ -14823,7 +14823,7 @@
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A196" s="1" t="s">
-        <v>2602</v>
+        <v>2601</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>2569</v>
@@ -14832,7 +14832,7 @@
         <v>28</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="F196" s="1">
         <v>-3</v>
@@ -15104,9 +15104,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D369"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A357" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D347" sqref="D347"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A261" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D264" sqref="D264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15156,7 +15156,7 @@
         <v>2565</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>2625</v>
+        <v>2624</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -15329,7 +15329,7 @@
         <v>2565</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>2624</v>
+        <v>2623</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -15427,7 +15427,7 @@
         <v>294</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>2615</v>
+        <v>2614</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -15441,7 +15441,7 @@
         <v>289</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>2616</v>
+        <v>2615</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -15497,7 +15497,7 @@
         <v>260</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>2617</v>
+        <v>2616</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -15530,7 +15530,7 @@
         <v>2565</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>2626</v>
+        <v>2625</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
@@ -15558,7 +15558,7 @@
         <v>294</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>2627</v>
+        <v>2626</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
@@ -15759,7 +15759,7 @@
         <v>294</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>2628</v>
+        <v>2627</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
@@ -15815,7 +15815,7 @@
         <v>294</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>2629</v>
+        <v>2628</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
@@ -15871,7 +15871,7 @@
         <v>294</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>2630</v>
+        <v>2629</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
@@ -16175,7 +16175,7 @@
         <v>2565</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>2631</v>
+        <v>2630</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
@@ -16273,7 +16273,7 @@
         <v>294</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
@@ -16301,7 +16301,7 @@
         <v>294</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
@@ -16385,7 +16385,7 @@
         <v>2551</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>2607</v>
+        <v>2606</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="203" x14ac:dyDescent="0.35">
@@ -16399,7 +16399,7 @@
         <v>2552</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>2606</v>
+        <v>2605</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
@@ -16530,7 +16530,7 @@
         <v>260</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>2605</v>
+        <v>2604</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -16605,7 +16605,7 @@
         <v>2565</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>2634</v>
+        <v>2633</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -16675,7 +16675,7 @@
         <v>294</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>2635</v>
+        <v>2634</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
@@ -16820,7 +16820,7 @@
         <v>2565</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>2636</v>
+        <v>2635</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -16890,7 +16890,7 @@
         <v>294</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
@@ -17007,7 +17007,7 @@
         <v>2565</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>2638</v>
+        <v>2637</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -17021,7 +17021,7 @@
         <v>2565</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>2639</v>
+        <v>2638</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -17180,7 +17180,7 @@
         <v>2565</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>2640</v>
+        <v>2639</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -17381,7 +17381,7 @@
         <v>2565</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>2653</v>
+        <v>2652</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.35">
@@ -17437,7 +17437,7 @@
         <v>294</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>2654</v>
+        <v>2653</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -17596,7 +17596,7 @@
         <v>2559</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>2608</v>
+        <v>2607</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -17694,7 +17694,7 @@
         <v>2559</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>2608</v>
+        <v>2607</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.35">
@@ -17769,7 +17769,7 @@
         <v>2565</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>2655</v>
+        <v>2654</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.35">
@@ -17956,7 +17956,7 @@
         <v>2565</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>2641</v>
+        <v>2640</v>
       </c>
     </row>
     <row r="213" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18012,7 +18012,7 @@
         <v>294</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>2656</v>
+        <v>2655</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.35">
@@ -18129,7 +18129,7 @@
         <v>2565</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>2642</v>
+        <v>2641</v>
       </c>
     </row>
     <row r="226" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18330,7 +18330,7 @@
         <v>2565</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>2643</v>
+        <v>2642</v>
       </c>
     </row>
     <row r="241" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18475,7 +18475,7 @@
         <v>2565</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>2644</v>
+        <v>2643</v>
       </c>
     </row>
     <row r="252" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18587,7 +18587,7 @@
         <v>2559</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>2609</v>
+        <v>2608</v>
       </c>
     </row>
     <row r="260" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18643,7 +18643,7 @@
         <v>2563</v>
       </c>
       <c r="D263" s="1" t="s">
-        <v>2601</v>
+        <v>2657</v>
       </c>
     </row>
     <row r="264" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -18662,7 +18662,7 @@
         <v>2565</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>2645</v>
+        <v>2644</v>
       </c>
     </row>
     <row r="266" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18690,7 +18690,7 @@
         <v>289</v>
       </c>
       <c r="D267" s="1" t="s">
-        <v>2646</v>
+        <v>2645</v>
       </c>
     </row>
     <row r="268" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -18900,7 +18900,7 @@
         <v>266</v>
       </c>
       <c r="D282" s="1" t="s">
-        <v>2648</v>
+        <v>2647</v>
       </c>
     </row>
     <row r="283" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -18914,7 +18914,7 @@
         <v>260</v>
       </c>
       <c r="D283" s="1" t="s">
-        <v>2647</v>
+        <v>2646</v>
       </c>
     </row>
     <row r="284" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -19321,7 +19321,7 @@
         <v>294</v>
       </c>
       <c r="D314" s="4" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
     </row>
     <row r="315" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -19522,7 +19522,7 @@
         <v>267</v>
       </c>
       <c r="D329" s="1" t="s">
-        <v>2618</v>
+        <v>2617</v>
       </c>
     </row>
     <row r="330" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -19564,7 +19564,7 @@
         <v>294</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>2623</v>
+        <v>2622</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.35">
@@ -19634,7 +19634,7 @@
         <v>294</v>
       </c>
       <c r="D337" s="1" t="s">
-        <v>2622</v>
+        <v>2621</v>
       </c>
     </row>
     <row r="338" spans="1:4" ht="87" x14ac:dyDescent="0.35">
@@ -19695,7 +19695,7 @@
         <v>2565</v>
       </c>
       <c r="D342" s="1" t="s">
-        <v>2650</v>
+        <v>2649</v>
       </c>
     </row>
     <row r="343" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -19751,7 +19751,7 @@
         <v>294</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>2657</v>
+        <v>2656</v>
       </c>
     </row>
     <row r="347" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -19765,7 +19765,7 @@
         <v>267</v>
       </c>
       <c r="D347" s="1" t="s">
-        <v>2651</v>
+        <v>2650</v>
       </c>
     </row>
     <row r="348" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -19807,7 +19807,7 @@
         <v>294</v>
       </c>
       <c r="D350" s="1" t="s">
-        <v>2652</v>
+        <v>2651</v>
       </c>
     </row>
     <row r="351" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -19896,13 +19896,13 @@
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A358" s="1" t="s">
-        <v>2602</v>
+        <v>2601</v>
       </c>
       <c r="B358" s="1" t="s">
         <v>2569</v>
       </c>
       <c r="D358" s="1" t="s">
-        <v>2603</v>
+        <v>2602</v>
       </c>
     </row>
     <row r="359" spans="1:4" ht="87" x14ac:dyDescent="0.35">
@@ -19913,7 +19913,7 @@
         <v>2569</v>
       </c>
       <c r="D359" s="1" t="s">
-        <v>2621</v>
+        <v>2620</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.35">
@@ -19938,7 +19938,7 @@
         <v>2569</v>
       </c>
       <c r="D361" s="1" t="s">
-        <v>2610</v>
+        <v>2609</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.35">
@@ -19952,7 +19952,7 @@
         <v>260</v>
       </c>
       <c r="D362" s="1" t="s">
-        <v>2619</v>
+        <v>2618</v>
       </c>
     </row>
     <row r="363" spans="1:4" ht="87" x14ac:dyDescent="0.35">
@@ -19963,7 +19963,7 @@
         <v>2569</v>
       </c>
       <c r="D363" s="1" t="s">
-        <v>2620</v>
+        <v>2619</v>
       </c>
     </row>
     <row r="364" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
@@ -19974,7 +19974,7 @@
         <v>2569</v>
       </c>
       <c r="D364" s="1" t="s">
-        <v>2614</v>
+        <v>2613</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.35">
@@ -20041,7 +20041,7 @@
         <v>267</v>
       </c>
       <c r="D369" s="1" t="s">
-        <v>2611</v>
+        <v>2610</v>
       </c>
     </row>
   </sheetData>
@@ -20956,7 +20956,7 @@
         <v>1000</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
       <c r="G22" s="19" t="s">
         <v>2405</v>
@@ -21358,7 +21358,7 @@
   <dimension ref="A1:N159"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L135" sqref="L135"/>
     </sheetView>
   </sheetViews>
@@ -26945,7 +26945,7 @@
         <v>0</v>
       </c>
       <c r="L133" s="23" t="s">
-        <v>2612</v>
+        <v>2611</v>
       </c>
       <c r="N133" s="27" t="s">
         <v>1404</v>

</xml_diff>

<commit_message>
world 7 new levels
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\data\q-z\Realm Defense\CyraBot\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1D4B61-6A26-4D2C-B1BE-A19F9362E8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADD5B68-DAA2-40D2-A7D8-DF05AF56D8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hero" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5601" uniqueCount="2675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5626" uniqueCount="2691">
   <si>
     <t>name</t>
   </si>
@@ -7315,9 +7315,6 @@
     <t>**Melee**: 1.2s cooldown, deals `(1 ND) PD`</t>
   </si>
   <si>
-    <t>**Melee**: 1.75s cooldown, deals `(1 ND) PD`</t>
-  </si>
-  <si>
     <t>**Melee**: 1.2s cooldown, deals `(1 ND) PD`
 **Sticky Body**: When killed, covers all enemies in range 0.5 by slime: reduce move speed by 40% and damage by 20%, last 10s</t>
   </si>
@@ -7838,11 +7835,6 @@
 **Lv3** (65💰): 137 HP, 60 ND (Spear), 547 HP, 288 ND (Volari)</t>
   </si>
   <si>
-    <t>**Lv1** (150💰): 8 ND
-**Lv2** (150💰): 12 ND
-**Lv3** (100💰): 17 ND</t>
-  </si>
-  <si>
     <t>Hogan has two friends: Bacon and boar. They have 1.5 move speed and inherit Hogan's ND but cannot be hasted. When Hogan is within range 1.5 of Bacon, he is healed `(50+1 SD)` every 2s</t>
   </si>
   <si>
@@ -8609,6 +8601,76 @@
     <t>Osan gains the following effects:
 (1) A new ranged skill which can be used once per wave: 3s cooldown, Osan gains immunity for 2.33s and revives a nearest hero in range 3 by 30% HP with 3.8s invincibility
 (2) When out of combat, Osan gives heroes in range 2.5 (including himself) base life regen +666, and cleanses poison effects; Osan will be in combat after using his melee skills &amp; active or being attacked, and out of combat after 5s of no combat</t>
+  </si>
+  <si>
+    <t>**Lv1** (150💰): 12 ND
+**Lv2** (150💰): 17 ND
+**Lv3** (100💰): 22 ND</t>
+  </si>
+  <si>
+    <t>Omega Spider</t>
+  </si>
+  <si>
+    <t>Elysium Pebble</t>
+  </si>
+  <si>
+    <t>**Melee**: 1.25s cooldown, deals `(1 ND) PD`</t>
+  </si>
+  <si>
+    <t>**Melee**: 0.75s cooldown, deals `(1 ND) PD`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Melee**: 1.75s cooldown, deals `(1 ND) PD`
+**Underground Move**: Cloak and burried in ground when moving, deals `(1 ND) PD` to enemies in range 1 when emerge from underground </t>
+  </si>
+  <si>
+    <t>Chamekeon Sentry</t>
+  </si>
+  <si>
+    <t>**Melee**: 0.6s cooldown, deals `(1 ND) PD`
+**Cloak**
+**Bionics**: When it's uncloaked and unterrified, it starts pulling enemies: 2s cooldown, pulls an enemy in range 3 and deals `(0.25 ND) PD + (0.75 ND) MD`, this attack has lifesteal ratio 0.5, and can be used 30 times</t>
+  </si>
+  <si>
+    <t>Slime Shooter</t>
+  </si>
+  <si>
+    <t>**Melee**: 3s cooldown, deals `(0.5 ND) PD` to enemies within range 0.5 of itself
+**Slime Shot**: 2s cooldown, deals `(1 ND) PD` to an enemy in range 2.5, cover all enemies in AOE range 0.5 by slime for 10s: move speed x0.6 and damage x0.8, max 50 shots</t>
+  </si>
+  <si>
+    <t>Rock Flinger</t>
+  </si>
+  <si>
+    <t>Satyr Sentinel</t>
+  </si>
+  <si>
+    <t>Elysium Rock</t>
+  </si>
+  <si>
+    <t>**Melee**: 1.75s cooldown, deals `(1 ND) PD`
+**Entangle**: 6s cooldown, entangles 2 enemies in range 2 or 1 enemy in melee, deals `(0.5 ND) PD + (0.5 ND) MD`, make them not able to move, this skill can be used 25 times
+**Rock Thrower**: 2s cooldown, throw a rock to an enemy in range 2.5 and deals `(1 ND) PD` to all enemies in AOE range 1, max 25 shots</t>
+  </si>
+  <si>
+    <t>**Melee**: 1.75s cooldown, deals `(1 ND) PD`
+**Slam**: 2.5s cooldown, deals `(1 ND) PD` to enemies in AOE range ?
+**Elysium Soldier**: When killed, spawns a Elysium Pebble which inherits 50% HP and damage</t>
+  </si>
+  <si>
+    <t>**Melee**: 1.5s cooldown, deals `(0.5 ND) PD + (0.5 ND) MD`
+**Slam**: 4s cooldown, deals `(0.5 ND) PD + (0.5 ND) MD` to enemies in AOE range 1.25
+**Slime Blade**: 5s cooldown, deals `(0.5 ND) PD + (0.5 ND) MD` to an enemy, covers all enemies in AOE range 1 by slime: move speed x0.6 and damage x0.8, last 6s, and gives ground slimes in AOE range 1 a slime cover buff: HP x2, damage x1.5. Then it launches 2 slime shots to enemy, each deals `(1 ND) PD` and cover all enemies in AOE range 0.5 by slime for 10s</t>
+  </si>
+  <si>
+    <t>Arachnamech</t>
+  </si>
+  <si>
+    <t>**Slam**: 3s cooldown, deals `(1 ND) PD` to enemies in AOE range 2 and stun them for 2s
+**Stab**: If there is an enemy covered by slime in range 2, attack deals `(1 ND) PD + (0.5 ND) MD` with 0.75 lifesteal ratio, and applies bleeding for 10s
+**Slime Shot**: 10s cooldown, launches 3 shots to enemies in range 3.75, each shot covers all enemies in AOE range 1 by slime: move speed x0.6 and damage x0.8, last 10s, and give ground slimes in AOE range 1 a slime cover buff: HP x2, damage x1.5
+**Powered Slime Shot**: 15s cooldown, launch 1 shot to an enemy in range 3, covers all enemies in AOE range 2 by slime, and give ground slimes in AOE range 2 a slime cover buff
+**Spider Web**: Leap in or out of battlefield when the wave progresses, when leaping in, deals `(1 ND) PD` to enemies in AOE range 3 and stuns them for 5s</t>
   </si>
 </sst>
 </file>
@@ -9286,7 +9348,7 @@
         <v>7</v>
       </c>
       <c r="X2" t="s">
-        <v>2381</v>
+        <v>2380</v>
       </c>
       <c r="Y2" s="31" t="s">
         <v>1569</v>
@@ -9363,7 +9425,7 @@
         <v>7</v>
       </c>
       <c r="X3" t="s">
-        <v>2382</v>
+        <v>2381</v>
       </c>
       <c r="Y3" s="31" t="s">
         <v>1570</v>
@@ -9440,7 +9502,7 @@
         <v>7</v>
       </c>
       <c r="X4" t="s">
-        <v>2383</v>
+        <v>2382</v>
       </c>
       <c r="Y4" s="31" t="s">
         <v>1571</v>
@@ -9517,7 +9579,7 @@
         <v>6</v>
       </c>
       <c r="X5" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
       <c r="Y5" s="31" t="s">
         <v>1552</v>
@@ -9594,7 +9656,7 @@
         <v>6</v>
       </c>
       <c r="X6" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="Y6" s="31" t="s">
         <v>1553</v>
@@ -9671,7 +9733,7 @@
         <v>7</v>
       </c>
       <c r="X7" t="s">
-        <v>2389</v>
+        <v>2388</v>
       </c>
       <c r="Y7" s="31" t="s">
         <v>1554</v>
@@ -9748,7 +9810,7 @@
         <v>6</v>
       </c>
       <c r="X8" t="s">
-        <v>2390</v>
+        <v>2389</v>
       </c>
       <c r="Y8" s="31" t="s">
         <v>1555</v>
@@ -9825,7 +9887,7 @@
         <v>7</v>
       </c>
       <c r="X9" t="s">
-        <v>2391</v>
+        <v>2390</v>
       </c>
       <c r="Y9" s="31" t="s">
         <v>1556</v>
@@ -9902,7 +9964,7 @@
         <v>6</v>
       </c>
       <c r="X10" t="s">
-        <v>2391</v>
+        <v>2390</v>
       </c>
       <c r="Y10" s="31" t="s">
         <v>1556</v>
@@ -9979,7 +10041,7 @@
         <v>6</v>
       </c>
       <c r="X11" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="Y11" s="31" t="s">
         <v>1557</v>
@@ -10056,7 +10118,7 @@
         <v>7</v>
       </c>
       <c r="X12" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="Y12" s="31" t="s">
         <v>1558</v>
@@ -10133,7 +10195,7 @@
         <v>7</v>
       </c>
       <c r="X13" t="s">
-        <v>2394</v>
+        <v>2393</v>
       </c>
       <c r="Y13" s="31" t="s">
         <v>1559</v>
@@ -10210,7 +10272,7 @@
         <v>7</v>
       </c>
       <c r="X14" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Y14" s="31" t="s">
         <v>1560</v>
@@ -10287,7 +10349,7 @@
         <v>7</v>
       </c>
       <c r="X15" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="Y15" s="31" t="s">
         <v>1561</v>
@@ -10364,7 +10426,7 @@
         <v>6</v>
       </c>
       <c r="X16" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
       <c r="Y16" s="31" t="s">
         <v>1562</v>
@@ -10441,7 +10503,7 @@
         <v>6</v>
       </c>
       <c r="X17" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
       <c r="Y17" s="31" t="s">
         <v>1563</v>
@@ -10518,7 +10580,7 @@
         <v>6</v>
       </c>
       <c r="X18" t="s">
-        <v>2399</v>
+        <v>2398</v>
       </c>
       <c r="Y18" s="31" t="s">
         <v>1564</v>
@@ -10595,7 +10657,7 @@
         <v>6</v>
       </c>
       <c r="X19" t="s">
-        <v>2400</v>
+        <v>2399</v>
       </c>
       <c r="Y19" s="31" t="s">
         <v>1565</v>
@@ -10672,7 +10734,7 @@
         <v>6</v>
       </c>
       <c r="X20" t="s">
-        <v>2401</v>
+        <v>2400</v>
       </c>
       <c r="Y20" s="31" t="s">
         <v>1566</v>
@@ -10749,7 +10811,7 @@
         <v>6</v>
       </c>
       <c r="X21" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="Y21" s="31" t="s">
         <v>1567</v>
@@ -10826,7 +10888,7 @@
         <v>6</v>
       </c>
       <c r="X22" t="s">
-        <v>2403</v>
+        <v>2402</v>
       </c>
       <c r="Y22" s="31" t="s">
         <v>1568</v>
@@ -10903,7 +10965,7 @@
         <v>1</v>
       </c>
       <c r="X23" t="s">
-        <v>2385</v>
+        <v>2384</v>
       </c>
       <c r="Y23" s="31" t="s">
         <v>1552</v>
@@ -10980,7 +11042,7 @@
         <v>7</v>
       </c>
       <c r="X24" t="s">
-        <v>2386</v>
+        <v>2385</v>
       </c>
       <c r="Y24" s="31" t="s">
         <v>1572</v>
@@ -11057,7 +11119,7 @@
         <v>7</v>
       </c>
       <c r="X25" t="s">
-        <v>2388</v>
+        <v>2387</v>
       </c>
       <c r="Y25" s="31" t="s">
         <v>1573</v>
@@ -11065,7 +11127,7 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="B26">
         <v>7</v>
@@ -11134,10 +11196,10 @@
         <v>7</v>
       </c>
       <c r="X26" t="s">
-        <v>2533</v>
+        <v>2531</v>
       </c>
       <c r="Y26" s="31" t="s">
-        <v>2534</v>
+        <v>2532</v>
       </c>
     </row>
   </sheetData>
@@ -11277,7 +11339,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>2466</v>
+        <v>2464</v>
       </c>
       <c r="H4" s="20" t="s">
         <v>1137</v>
@@ -11421,7 +11483,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>2467</v>
+        <v>2465</v>
       </c>
       <c r="H12" s="20" t="s">
         <v>1141</v>
@@ -11470,7 +11532,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>2468</v>
+        <v>2466</v>
       </c>
       <c r="H14" s="20" t="s">
         <v>1161</v>
@@ -11521,7 +11583,7 @@
     </row>
     <row r="17" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>2473</v>
+        <v>2471</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>45</v>
@@ -11533,7 +11595,7 @@
         <v>267</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="F17" s="1">
         <v>5</v>
@@ -11557,7 +11619,7 @@
         <v>-2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>2469</v>
+        <v>2467</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="58" x14ac:dyDescent="0.35">
@@ -11603,7 +11665,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>2470</v>
+        <v>2468</v>
       </c>
       <c r="H21" s="20" t="s">
         <v>1184</v>
@@ -11906,7 +11968,7 @@
         <v>0</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>2621</v>
+        <v>2619</v>
       </c>
       <c r="H37" s="20" t="s">
         <v>1213</v>
@@ -11958,7 +12020,7 @@
         <v>2</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>2622</v>
+        <v>2620</v>
       </c>
       <c r="H39" s="20" t="s">
         <v>1154</v>
@@ -12305,7 +12367,7 @@
     </row>
     <row r="58" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>2650</v>
+        <v>2648</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>97</v>
@@ -12317,7 +12379,7 @@
         <v>265</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>2651</v>
+        <v>2649</v>
       </c>
       <c r="F58" s="1">
         <v>4</v>
@@ -12364,7 +12426,7 @@
         <v>0</v>
       </c>
       <c r="H61" s="20" t="s">
-        <v>2451</v>
+        <v>2450</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -12384,7 +12446,7 @@
         <v>1</v>
       </c>
       <c r="H62" s="20" t="s">
-        <v>2454</v>
+        <v>2453</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
@@ -12404,7 +12466,7 @@
         <v>2</v>
       </c>
       <c r="H63" s="20" t="s">
-        <v>2453</v>
+        <v>2452</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -12424,7 +12486,7 @@
         <v>3</v>
       </c>
       <c r="H64" s="20" t="s">
-        <v>2452</v>
+        <v>2451</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -13078,19 +13140,19 @@
     </row>
     <row r="99" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>2490</v>
+        <v>2488</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>148</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>2489</v>
+        <v>2487</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>267</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>2491</v>
+        <v>2489</v>
       </c>
       <c r="F99" s="1">
         <v>5</v>
@@ -13151,7 +13213,7 @@
         <v>0</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>2492</v>
+        <v>2490</v>
       </c>
       <c r="H103" s="20" t="s">
         <v>1218</v>
@@ -13223,7 +13285,7 @@
         <v>3</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>2492</v>
+        <v>2490</v>
       </c>
       <c r="H106" s="20" t="s">
         <v>1182</v>
@@ -13231,7 +13293,7 @@
     </row>
     <row r="107" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>2635</v>
+        <v>2633</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>42</v>
@@ -13243,7 +13305,7 @@
         <v>264</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>2636</v>
+        <v>2634</v>
       </c>
       <c r="F107" s="1">
         <v>4</v>
@@ -13402,19 +13464,19 @@
     </row>
     <row r="116" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>2639</v>
+        <v>2637</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>2640</v>
+        <v>2638</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>267</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>2641</v>
+        <v>2639</v>
       </c>
       <c r="F116" s="1">
         <v>4</v>
@@ -13860,7 +13922,7 @@
         <v>-2</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>2505</v>
+        <v>2503</v>
       </c>
     </row>
     <row r="141" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -14693,7 +14755,7 @@
         <v>0</v>
       </c>
       <c r="G185" s="1" t="s">
-        <v>2485</v>
+        <v>2483</v>
       </c>
       <c r="H185" s="20" t="s">
         <v>1220</v>
@@ -14794,7 +14856,7 @@
         <v>4</v>
       </c>
       <c r="G189" s="1" t="s">
-        <v>2485</v>
+        <v>2483</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.35">
@@ -14831,7 +14893,7 @@
         <v>-2</v>
       </c>
       <c r="G192" s="1" t="s">
-        <v>2486</v>
+        <v>2484</v>
       </c>
     </row>
     <row r="193" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -14851,7 +14913,7 @@
         <v>0</v>
       </c>
       <c r="G193" s="1" t="s">
-        <v>2487</v>
+        <v>2485</v>
       </c>
       <c r="H193" s="20" t="s">
         <v>1219</v>
@@ -14903,7 +14965,7 @@
         <v>2</v>
       </c>
       <c r="G195" s="1" t="s">
-        <v>2488</v>
+        <v>2486</v>
       </c>
       <c r="H195" s="20" t="s">
         <v>1188</v>
@@ -14954,16 +15016,16 @@
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A199" s="1" t="s">
-        <v>2564</v>
+        <v>2562</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>2566</v>
+        <v>2564</v>
       </c>
       <c r="F199" s="1">
         <v>-3</v>
@@ -14974,7 +15036,7 @@
         <v>13</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>26</v>
@@ -14986,38 +15048,38 @@
         <v>-2</v>
       </c>
       <c r="G200" s="1" t="s">
-        <v>2549</v>
+        <v>2547</v>
       </c>
     </row>
     <row r="201" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A201" s="1" t="s">
-        <v>2535</v>
+        <v>2533</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>2541</v>
+        <v>2539</v>
       </c>
       <c r="F201" s="1">
         <v>0</v>
       </c>
       <c r="G201" s="1" t="s">
-        <v>2550</v>
+        <v>2548</v>
       </c>
       <c r="H201" s="20" t="s">
-        <v>2554</v>
+        <v>2552</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="s">
-        <v>2536</v>
+        <v>2534</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>27</v>
@@ -15026,21 +15088,21 @@
         <v>34</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>2542</v>
+        <v>2540</v>
       </c>
       <c r="F202" s="1">
         <v>1</v>
       </c>
       <c r="H202" s="20" t="s">
-        <v>2553</v>
+        <v>2551</v>
       </c>
     </row>
     <row r="203" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A203" s="1" t="s">
-        <v>2537</v>
+        <v>2535</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>271</v>
@@ -15049,50 +15111,50 @@
         <v>35</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>2543</v>
+        <v>2541</v>
       </c>
       <c r="F203" s="1">
         <v>2</v>
       </c>
       <c r="G203" s="1" t="s">
-        <v>2548</v>
+        <v>2546</v>
       </c>
       <c r="H203" s="20" t="s">
-        <v>2552</v>
+        <v>2550</v>
       </c>
     </row>
     <row r="204" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A204" s="1" t="s">
-        <v>2538</v>
+        <v>2536</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>2547</v>
+        <v>2545</v>
       </c>
       <c r="D204" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>2544</v>
+        <v>2542</v>
       </c>
       <c r="F204" s="1">
         <v>3</v>
       </c>
       <c r="G204" s="1" t="s">
-        <v>2548</v>
+        <v>2546</v>
       </c>
       <c r="H204" s="20" t="s">
-        <v>2551</v>
+        <v>2549</v>
       </c>
     </row>
     <row r="205" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A205" s="1" t="s">
-        <v>2539</v>
+        <v>2537</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>28</v>
@@ -15101,7 +15163,7 @@
         <v>265</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>2545</v>
+        <v>2543</v>
       </c>
       <c r="F205" s="1">
         <v>4</v>
@@ -15109,10 +15171,10 @@
     </row>
     <row r="206" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A206" s="1" t="s">
-        <v>2540</v>
+        <v>2538</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>27</v>
@@ -15121,7 +15183,7 @@
         <v>267</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
       <c r="F206" s="1">
         <v>5</v>
@@ -15235,7 +15297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D376"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A371" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D376" sqref="D376"/>
     </sheetView>
@@ -15270,10 +15332,10 @@
         <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>2476</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -15284,10 +15346,10 @@
         <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>2579</v>
+        <v>2577</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -15357,7 +15419,7 @@
         <v>266</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>2633</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -15371,7 +15433,7 @@
         <v>267</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>2477</v>
+        <v>2475</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -15424,7 +15486,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>2263</v>
@@ -15432,7 +15494,7 @@
     </row>
     <row r="14" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C14" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -15443,7 +15505,7 @@
         <v>45</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>364</v>
@@ -15457,10 +15519,10 @@
         <v>45</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>2578</v>
+        <v>2576</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -15516,7 +15578,7 @@
         <v>266</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>2472</v>
+        <v>2470</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -15544,7 +15606,7 @@
         <v>289</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>2616</v>
+        <v>2614</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -15558,7 +15620,7 @@
         <v>293</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>2572</v>
+        <v>2570</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -15572,7 +15634,7 @@
         <v>289</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>2573</v>
+        <v>2571</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -15586,7 +15648,7 @@
         <v>266</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>2472</v>
+        <v>2470</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -15628,12 +15690,12 @@
         <v>260</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>2574</v>
+        <v>2572</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>2473</v>
+        <v>2471</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>45</v>
@@ -15642,12 +15704,12 @@
         <v>267</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>2668</v>
+        <v>2666</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C30" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -15658,10 +15720,10 @@
         <v>57</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>2580</v>
+        <v>2578</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
@@ -15672,7 +15734,7 @@
         <v>57</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>2509</v>
+        <v>2507</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>290</v>
@@ -15689,7 +15751,7 @@
         <v>293</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>2581</v>
+        <v>2579</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
@@ -15731,7 +15793,7 @@
         <v>267</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>2471</v>
+        <v>2469</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -15792,7 +15854,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C41" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -15803,7 +15865,7 @@
         <v>69</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>1580</v>
@@ -15817,7 +15879,7 @@
         <v>69</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>373</v>
@@ -15845,7 +15907,7 @@
         <v>69</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>1586</v>
@@ -15890,7 +15952,7 @@
         <v>293</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>2582</v>
+        <v>2580</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
@@ -15946,7 +16008,7 @@
         <v>293</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>2583</v>
+        <v>2581</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
@@ -16002,7 +16064,7 @@
         <v>293</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>2584</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
@@ -16030,12 +16092,12 @@
         <v>260</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>2617</v>
+        <v>2615</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C59" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
@@ -16046,7 +16108,7 @@
         <v>40</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>376</v>
@@ -16060,7 +16122,7 @@
         <v>40</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>1589</v>
@@ -16119,7 +16181,7 @@
         <v>264</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>2658</v>
+        <v>2656</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
@@ -16245,7 +16307,7 @@
         <v>264</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>2658</v>
+        <v>2656</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -16306,7 +16368,7 @@
     </row>
     <row r="79" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C79" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
@@ -16317,7 +16379,7 @@
         <v>88</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>381</v>
@@ -16331,10 +16393,10 @@
         <v>246</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>2585</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
@@ -16432,7 +16494,7 @@
         <v>293</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>2623</v>
+        <v>2621</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
@@ -16446,7 +16508,7 @@
         <v>289</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>2624</v>
+        <v>2622</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -16460,7 +16522,7 @@
         <v>293</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
@@ -16485,10 +16547,10 @@
         <v>88</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>2510</v>
+        <v>2508</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>2625</v>
+        <v>2623</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -16499,10 +16561,10 @@
         <v>88</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>2511</v>
+        <v>2509</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>2626</v>
+        <v>2624</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -16513,10 +16575,10 @@
         <v>88</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>2512</v>
+        <v>2510</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>2662</v>
+        <v>2660</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -16527,10 +16589,10 @@
         <v>88</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>2513</v>
+        <v>2511</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>2627</v>
+        <v>2625</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -16541,10 +16603,10 @@
         <v>88</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>2514</v>
+        <v>2512</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>2628</v>
+        <v>2626</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="203" x14ac:dyDescent="0.35">
@@ -16555,10 +16617,10 @@
         <v>88</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>2515</v>
+        <v>2513</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>2659</v>
+        <v>2657</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -16569,15 +16631,15 @@
         <v>88</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>2629</v>
+        <v>2627</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>2660</v>
+        <v>2658</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C99" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -16588,7 +16650,7 @@
         <v>97</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>1581</v>
@@ -16602,7 +16664,7 @@
         <v>97</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>385</v>
@@ -16616,7 +16678,7 @@
         <v>97</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>1590</v>
@@ -16703,7 +16765,7 @@
         <v>260</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>2567</v>
+        <v>2565</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -16764,7 +16826,7 @@
     </row>
     <row r="113" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>2650</v>
+        <v>2648</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>97</v>
@@ -16773,7 +16835,7 @@
         <v>265</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>2652</v>
+        <v>2650</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -16784,10 +16846,10 @@
         <v>105</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -16815,7 +16877,7 @@
         <v>266</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>2449</v>
+        <v>2448</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -16829,7 +16891,7 @@
         <v>293</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>2502</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -16843,7 +16905,7 @@
         <v>289</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>2493</v>
+        <v>2491</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
@@ -16857,7 +16919,7 @@
         <v>293</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
@@ -16871,7 +16933,7 @@
         <v>289</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>2494</v>
+        <v>2492</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -16885,7 +16947,7 @@
         <v>293</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>2501</v>
+        <v>2499</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -16899,7 +16961,7 @@
         <v>289</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>2500</v>
+        <v>2498</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -16913,7 +16975,7 @@
         <v>293</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>2503</v>
+        <v>2501</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -16927,7 +16989,7 @@
         <v>289</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>2631</v>
+        <v>2629</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -16938,10 +17000,10 @@
         <v>105</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>2464</v>
+        <v>2462</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
@@ -16955,7 +17017,7 @@
         <v>264</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>2606</v>
+        <v>2604</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -16969,7 +17031,7 @@
         <v>260</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>2632</v>
+        <v>2630</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="174" x14ac:dyDescent="0.35">
@@ -16983,12 +17045,12 @@
         <v>267</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>2465</v>
+        <v>2463</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C130" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -16999,10 +17061,10 @@
         <v>2265</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -17072,7 +17134,7 @@
         <v>293</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
@@ -17100,7 +17162,7 @@
         <v>293</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>2480</v>
+        <v>2478</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
@@ -17170,12 +17232,12 @@
         <v>260</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>2630</v>
+        <v>2628</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C144" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -17186,10 +17248,10 @@
         <v>39</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -17200,10 +17262,10 @@
         <v>39</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -17228,7 +17290,7 @@
         <v>39</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>2516</v>
+        <v>2514</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>397</v>
@@ -17312,7 +17374,7 @@
         <v>39</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>2516</v>
+        <v>2514</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>1593</v>
@@ -17348,7 +17410,7 @@
     </row>
     <row r="157" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C157" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -17359,10 +17421,10 @@
         <v>41</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>2593</v>
+        <v>2591</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -17401,10 +17463,10 @@
         <v>41</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>2517</v>
+        <v>2515</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>2634</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -17415,7 +17477,7 @@
         <v>41</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>2518</v>
+        <v>2516</v>
       </c>
       <c r="D162" s="1" t="s">
         <v>530</v>
@@ -17549,7 +17611,7 @@
     </row>
     <row r="172" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C172" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -17560,10 +17622,10 @@
         <v>138</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>2603</v>
+        <v>2601</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.35">
@@ -17574,7 +17636,7 @@
         <v>138</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>2519</v>
+        <v>2517</v>
       </c>
       <c r="D174" s="1" t="s">
         <v>323</v>
@@ -17588,7 +17650,7 @@
         <v>138</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>2520</v>
+        <v>2518</v>
       </c>
       <c r="D175" s="1" t="s">
         <v>324</v>
@@ -17602,7 +17664,7 @@
         <v>138</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>2521</v>
+        <v>2519</v>
       </c>
       <c r="D176" s="1" t="s">
         <v>349</v>
@@ -17619,7 +17681,7 @@
         <v>293</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>2604</v>
+        <v>2602</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -17647,7 +17709,7 @@
         <v>293</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>2667</v>
+        <v>2665</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -17680,7 +17742,7 @@
     </row>
     <row r="182" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A182" s="1" t="s">
-        <v>2490</v>
+        <v>2488</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>148</v>
@@ -17689,12 +17751,12 @@
         <v>267</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>2669</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C183" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -17705,7 +17767,7 @@
         <v>42</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D184" s="1" t="s">
         <v>1582</v>
@@ -17719,7 +17781,7 @@
         <v>42</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D185" s="1" t="s">
         <v>403</v>
@@ -17736,7 +17798,7 @@
         <v>266</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>2647</v>
+        <v>2645</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
@@ -17750,7 +17812,7 @@
         <v>293</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>2495</v>
+        <v>2493</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
@@ -17764,7 +17826,7 @@
         <v>289</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>2498</v>
+        <v>2496</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.35">
@@ -17775,10 +17837,10 @@
         <v>42</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>2522</v>
+        <v>2520</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>2638</v>
+        <v>2636</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -17792,7 +17854,7 @@
         <v>267</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>2661</v>
+        <v>2659</v>
       </c>
     </row>
     <row r="191" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -17862,7 +17924,7 @@
         <v>293</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>2496</v>
+        <v>2494</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -17876,7 +17938,7 @@
         <v>289</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>2497</v>
+        <v>2495</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.35">
@@ -17887,10 +17949,10 @@
         <v>42</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>2522</v>
+        <v>2520</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>2638</v>
+        <v>2636</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.35">
@@ -17904,7 +17966,7 @@
         <v>267</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>2481</v>
+        <v>2479</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.35">
@@ -17915,15 +17977,15 @@
         <v>42</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>2523</v>
+        <v>2521</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>2615</v>
+        <v>2613</v>
       </c>
     </row>
     <row r="200" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
-        <v>2635</v>
+        <v>2633</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>42</v>
@@ -17932,7 +17994,7 @@
         <v>264</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>2637</v>
+        <v>2635</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.35">
@@ -17951,7 +18013,7 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C202" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="203" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -17962,10 +18024,10 @@
         <v>43</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>2475</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="204" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -17976,10 +18038,10 @@
         <v>43</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>2605</v>
+        <v>2603</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.35">
@@ -18035,7 +18097,7 @@
         <v>289</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>2642</v>
+        <v>2640</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -18152,7 +18214,7 @@
     </row>
     <row r="217" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A217" s="1" t="s">
-        <v>2639</v>
+        <v>2637</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>43</v>
@@ -18161,7 +18223,7 @@
         <v>267</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>2643</v>
+        <v>2641</v>
       </c>
     </row>
     <row r="218" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -18173,10 +18235,10 @@
         <v>168</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>2594</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="220" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18215,10 +18277,10 @@
         <v>168</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>2524</v>
+        <v>2522</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>2646</v>
+        <v>2644</v>
       </c>
     </row>
     <row r="223" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18232,7 +18294,7 @@
         <v>293</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>2645</v>
+        <v>2643</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.35">
@@ -18246,7 +18308,7 @@
         <v>289</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>2644</v>
+        <v>2642</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.35">
@@ -18257,7 +18319,7 @@
         <v>168</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>2525</v>
+        <v>2523</v>
       </c>
       <c r="D225" s="1" t="s">
         <v>330</v>
@@ -18321,7 +18383,7 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C230" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="231" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18332,7 +18394,7 @@
         <v>177</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D231" s="1" t="s">
         <v>1583</v>
@@ -18346,10 +18408,10 @@
         <v>177</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>2595</v>
+        <v>2593</v>
       </c>
     </row>
     <row r="233" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18405,7 +18467,7 @@
         <v>260</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>2648</v>
+        <v>2646</v>
       </c>
     </row>
     <row r="237" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18522,7 +18584,7 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C245" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="246" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18533,7 +18595,7 @@
         <v>186</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D246" s="1" t="s">
         <v>1584</v>
@@ -18547,10 +18609,10 @@
         <v>186</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>2596</v>
+        <v>2594</v>
       </c>
     </row>
     <row r="248" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18578,7 +18640,7 @@
         <v>266</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
     </row>
     <row r="250" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18667,7 +18729,7 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C256" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="257" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18678,10 +18740,10 @@
         <v>195</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>2655</v>
+        <v>2653</v>
       </c>
     </row>
     <row r="258" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18692,10 +18754,10 @@
         <v>195</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>2597</v>
+        <v>2595</v>
       </c>
     </row>
     <row r="259" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18709,7 +18771,7 @@
         <v>266</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>2506</v>
+        <v>2504</v>
       </c>
     </row>
     <row r="260" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -18723,7 +18785,7 @@
         <v>293</v>
       </c>
       <c r="D260" s="1" t="s">
-        <v>2504</v>
+        <v>2502</v>
       </c>
     </row>
     <row r="261" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18737,7 +18799,7 @@
         <v>289</v>
       </c>
       <c r="D261" s="1" t="s">
-        <v>2654</v>
+        <v>2652</v>
       </c>
     </row>
     <row r="262" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18751,7 +18813,7 @@
         <v>293</v>
       </c>
       <c r="D262" s="3" t="s">
-        <v>2656</v>
+        <v>2654</v>
       </c>
     </row>
     <row r="263" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18793,7 +18855,7 @@
         <v>289</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>2508</v>
+        <v>2506</v>
       </c>
     </row>
     <row r="266" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18804,10 +18866,10 @@
         <v>195</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>2522</v>
+        <v>2520</v>
       </c>
       <c r="D266" s="1" t="s">
-        <v>2568</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="267" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18835,7 +18897,7 @@
         <v>289</v>
       </c>
       <c r="D268" s="1" t="s">
-        <v>2664</v>
+        <v>2662</v>
       </c>
     </row>
     <row r="269" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18849,7 +18911,7 @@
         <v>260</v>
       </c>
       <c r="D269" s="1" t="s">
-        <v>2507</v>
+        <v>2505</v>
       </c>
     </row>
     <row r="270" spans="1:4" ht="116" x14ac:dyDescent="0.35">
@@ -18860,15 +18922,15 @@
         <v>195</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>2526</v>
+        <v>2524</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>2666</v>
+        <v>2664</v>
       </c>
     </row>
     <row r="271" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C271" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="272" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -18879,10 +18941,10 @@
         <v>44</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>2598</v>
+        <v>2596</v>
       </c>
     </row>
     <row r="273" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18910,7 +18972,7 @@
         <v>289</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>2599</v>
+        <v>2597</v>
       </c>
     </row>
     <row r="275" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -18924,7 +18986,7 @@
         <v>293</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>2560</v>
+        <v>2558</v>
       </c>
     </row>
     <row r="276" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -18966,7 +19028,7 @@
         <v>293</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>2561</v>
+        <v>2559</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.35">
@@ -19008,7 +19070,7 @@
         <v>293</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>2562</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.35">
@@ -19050,7 +19112,7 @@
         <v>293</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>2563</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="285" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -19120,7 +19182,7 @@
         <v>266</v>
       </c>
       <c r="D289" s="1" t="s">
-        <v>2601</v>
+        <v>2599</v>
       </c>
     </row>
     <row r="290" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -19134,12 +19196,12 @@
         <v>260</v>
       </c>
       <c r="D290" s="1" t="s">
-        <v>2600</v>
+        <v>2598</v>
       </c>
     </row>
     <row r="291" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C291" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.35">
@@ -19150,7 +19212,7 @@
         <v>218</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D292" s="1" t="s">
         <v>428</v>
@@ -19164,7 +19226,7 @@
         <v>218</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D293" s="1" t="s">
         <v>1600</v>
@@ -19321,12 +19383,12 @@
         <v>260</v>
       </c>
       <c r="D304" s="1" t="s">
-        <v>2657</v>
+        <v>2655</v>
       </c>
     </row>
     <row r="305" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C305" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.35">
@@ -19337,7 +19399,7 @@
         <v>230</v>
       </c>
       <c r="C306" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D306" s="1" t="s">
         <v>434</v>
@@ -19351,7 +19413,7 @@
         <v>230</v>
       </c>
       <c r="C307" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D307" s="1" t="s">
         <v>1604</v>
@@ -19485,7 +19547,7 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C317" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="318" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -19496,7 +19558,7 @@
         <v>270</v>
       </c>
       <c r="C318" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D318" s="1" t="s">
         <v>1580</v>
@@ -19510,7 +19572,7 @@
         <v>270</v>
       </c>
       <c r="C319" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D319" s="1" t="s">
         <v>373</v>
@@ -19524,7 +19586,7 @@
         <v>270</v>
       </c>
       <c r="C320" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D320" s="1" t="s">
         <v>1607</v>
@@ -19541,7 +19603,7 @@
         <v>293</v>
       </c>
       <c r="D321" s="4" t="s">
-        <v>2602</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="322" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -19644,7 +19706,7 @@
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C329" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.35">
@@ -19655,7 +19717,7 @@
         <v>495</v>
       </c>
       <c r="C330" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D330" s="1" t="s">
         <v>1508</v>
@@ -19669,7 +19731,7 @@
         <v>495</v>
       </c>
       <c r="C331" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D331" s="1" t="s">
         <v>518</v>
@@ -19683,7 +19745,7 @@
         <v>495</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>2531</v>
+        <v>2529</v>
       </c>
       <c r="D332" s="1" t="s">
         <v>520</v>
@@ -19697,7 +19759,7 @@
         <v>495</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>2527</v>
+        <v>2525</v>
       </c>
       <c r="D333" s="1" t="s">
         <v>517</v>
@@ -19728,7 +19790,7 @@
         <v>293</v>
       </c>
       <c r="D335" s="1" t="s">
-        <v>2479</v>
+        <v>2477</v>
       </c>
     </row>
     <row r="336" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -19742,7 +19804,7 @@
         <v>267</v>
       </c>
       <c r="D336" s="1" t="s">
-        <v>2673</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="337" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -19756,7 +19818,7 @@
         <v>293</v>
       </c>
       <c r="D337" s="1" t="s">
-        <v>2380</v>
+        <v>2379</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.35">
@@ -19784,7 +19846,7 @@
         <v>293</v>
       </c>
       <c r="D339" s="1" t="s">
-        <v>2577</v>
+        <v>2575</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.35">
@@ -19795,7 +19857,7 @@
         <v>495</v>
       </c>
       <c r="C340" s="1" t="s">
-        <v>2529</v>
+        <v>2527</v>
       </c>
       <c r="D340" s="1" t="s">
         <v>899</v>
@@ -19809,7 +19871,7 @@
         <v>495</v>
       </c>
       <c r="C341" s="1" t="s">
-        <v>2531</v>
+        <v>2529</v>
       </c>
       <c r="D341" s="1" t="s">
         <v>521</v>
@@ -19823,7 +19885,7 @@
         <v>495</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>2527</v>
+        <v>2525</v>
       </c>
       <c r="D342" s="1" t="s">
         <v>898</v>
@@ -19854,7 +19916,7 @@
         <v>293</v>
       </c>
       <c r="D344" s="1" t="s">
-        <v>2608</v>
+        <v>2606</v>
       </c>
     </row>
     <row r="345" spans="1:4" ht="87" x14ac:dyDescent="0.35">
@@ -19868,7 +19930,7 @@
         <v>266</v>
       </c>
       <c r="D345" s="1" t="s">
-        <v>2448</v>
+        <v>2447</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.35">
@@ -19882,12 +19944,12 @@
         <v>267</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>2482</v>
+        <v>2480</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C347" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.35">
@@ -19898,7 +19960,7 @@
         <v>503</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D348" s="1" t="s">
         <v>1509</v>
@@ -19912,10 +19974,10 @@
         <v>503</v>
       </c>
       <c r="C349" s="1" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
       <c r="D349" s="1" t="s">
-        <v>2620</v>
+        <v>2618</v>
       </c>
     </row>
     <row r="350" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -19926,10 +19988,10 @@
         <v>503</v>
       </c>
       <c r="C350" s="1" t="s">
-        <v>2530</v>
+        <v>2528</v>
       </c>
       <c r="D350" s="1" t="s">
-        <v>2607</v>
+        <v>2605</v>
       </c>
     </row>
     <row r="351" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -19940,7 +20002,7 @@
         <v>503</v>
       </c>
       <c r="C351" s="1" t="s">
-        <v>2531</v>
+        <v>2529</v>
       </c>
       <c r="D351" s="1" t="s">
         <v>520</v>
@@ -19957,7 +20019,7 @@
         <v>267</v>
       </c>
       <c r="D352" s="1" t="s">
-        <v>2484</v>
+        <v>2482</v>
       </c>
     </row>
     <row r="353" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
@@ -19971,7 +20033,7 @@
         <v>293</v>
       </c>
       <c r="D353" s="1" t="s">
-        <v>2671</v>
+        <v>2669</v>
       </c>
     </row>
     <row r="354" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -19985,7 +20047,7 @@
         <v>267</v>
       </c>
       <c r="D354" s="1" t="s">
-        <v>2672</v>
+        <v>2670</v>
       </c>
     </row>
     <row r="355" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -19999,7 +20061,7 @@
         <v>293</v>
       </c>
       <c r="D355" s="1" t="s">
-        <v>2446</v>
+        <v>2445</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.35">
@@ -20027,7 +20089,7 @@
         <v>293</v>
       </c>
       <c r="D357" s="1" t="s">
-        <v>2618</v>
+        <v>2616</v>
       </c>
     </row>
     <row r="358" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -20038,10 +20100,10 @@
         <v>503</v>
       </c>
       <c r="C358" s="1" t="s">
-        <v>2529</v>
+        <v>2527</v>
       </c>
       <c r="D358" s="1" t="s">
-        <v>2450</v>
+        <v>2449</v>
       </c>
     </row>
     <row r="359" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -20052,7 +20114,7 @@
         <v>503</v>
       </c>
       <c r="C359" s="1" t="s">
-        <v>2531</v>
+        <v>2529</v>
       </c>
       <c r="D359" s="1" t="s">
         <v>520</v>
@@ -20069,7 +20131,7 @@
         <v>266</v>
       </c>
       <c r="D360" s="1" t="s">
-        <v>2447</v>
+        <v>2446</v>
       </c>
     </row>
     <row r="361" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -20083,7 +20145,7 @@
         <v>267</v>
       </c>
       <c r="D361" s="1" t="s">
-        <v>2483</v>
+        <v>2481</v>
       </c>
     </row>
     <row r="362" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -20097,7 +20159,7 @@
         <v>293</v>
       </c>
       <c r="D362" s="1" t="s">
-        <v>2619</v>
+        <v>2617</v>
       </c>
     </row>
     <row r="363" spans="1:4" ht="87" x14ac:dyDescent="0.35">
@@ -20111,18 +20173,18 @@
         <v>265</v>
       </c>
       <c r="D363" s="1" t="s">
-        <v>2670</v>
+        <v>2668</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A365" s="1" t="s">
-        <v>2564</v>
+        <v>2562</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="D365" s="1" t="s">
-        <v>2565</v>
+        <v>2563</v>
       </c>
     </row>
     <row r="366" spans="1:4" ht="87" x14ac:dyDescent="0.35">
@@ -20130,10 +20192,10 @@
         <v>13</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="D366" s="1" t="s">
-        <v>2576</v>
+        <v>2574</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.35">
@@ -20141,127 +20203,127 @@
         <v>13</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="C367" s="1" t="s">
         <v>266</v>
       </c>
       <c r="D367" s="1" t="s">
-        <v>2555</v>
+        <v>2553</v>
       </c>
     </row>
     <row r="368" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A368" s="1" t="s">
-        <v>2535</v>
+        <v>2533</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="D368" s="1" t="s">
-        <v>2663</v>
+        <v>2661</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A369" s="1" t="s">
-        <v>2535</v>
+        <v>2533</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="C369" s="1" t="s">
         <v>260</v>
       </c>
       <c r="D369" s="1" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
     </row>
     <row r="370" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A370" s="1" t="s">
-        <v>2536</v>
+        <v>2534</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="D370" s="1" t="s">
-        <v>2649</v>
+        <v>2647</v>
       </c>
     </row>
     <row r="371" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A371" s="1" t="s">
-        <v>2537</v>
+        <v>2535</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="D371" s="1" t="s">
-        <v>2571</v>
+        <v>2569</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A372" s="1" t="s">
-        <v>2537</v>
+        <v>2535</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="C372" s="1" t="s">
         <v>264</v>
       </c>
       <c r="D372" s="1" t="s">
-        <v>2556</v>
+        <v>2554</v>
       </c>
     </row>
     <row r="373" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A373" s="1" t="s">
-        <v>2538</v>
+        <v>2536</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="D373" s="1" t="s">
-        <v>2557</v>
+        <v>2555</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A374" s="1" t="s">
-        <v>2538</v>
+        <v>2536</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="C374" s="1" t="s">
         <v>264</v>
       </c>
       <c r="D374" s="1" t="s">
-        <v>2558</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A375" s="1" t="s">
-        <v>2539</v>
+        <v>2537</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="C375" s="1" t="s">
         <v>265</v>
       </c>
       <c r="D375" s="1" t="s">
-        <v>2559</v>
+        <v>2557</v>
       </c>
     </row>
     <row r="376" spans="1:4" ht="116" x14ac:dyDescent="0.35">
       <c r="A376" s="1" t="s">
-        <v>2540</v>
+        <v>2538</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="C376" s="1" t="s">
         <v>267</v>
       </c>
       <c r="D376" s="1" t="s">
-        <v>2674</v>
+        <v>2672</v>
       </c>
     </row>
   </sheetData>
@@ -20276,9 +20338,9 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="K16" sqref="K16"/>
+      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20356,10 +20418,10 @@
         <v>945</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>2408</v>
+        <v>2407</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>2368</v>
+        <v>2367</v>
       </c>
       <c r="H2" s="19" t="s">
         <v>2182</v>
@@ -20397,10 +20459,10 @@
         <v>947</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>2409</v>
+        <v>2408</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>2369</v>
+        <v>2368</v>
       </c>
       <c r="H3" s="19" t="s">
         <v>2185</v>
@@ -20438,10 +20500,10 @@
         <v>949</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>2435</v>
+        <v>2434</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>2370</v>
+        <v>2369</v>
       </c>
       <c r="H4" s="19" t="s">
         <v>2188</v>
@@ -20479,10 +20541,10 @@
         <v>951</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>2410</v>
+        <v>2409</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>2371</v>
+        <v>2370</v>
       </c>
       <c r="H5" s="19" t="s">
         <v>2191</v>
@@ -20520,10 +20582,10 @@
         <v>953</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>2411</v>
+        <v>2410</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="H6" s="19" t="s">
         <v>2194</v>
@@ -20561,7 +20623,7 @@
         <v>955</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>2412</v>
+        <v>2411</v>
       </c>
       <c r="G7" s="19" t="s">
         <v>2248</v>
@@ -20602,10 +20664,10 @@
         <v>957</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>2413</v>
+        <v>2412</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
       <c r="H8" s="19" t="s">
         <v>2200</v>
@@ -20614,13 +20676,13 @@
         <v>1000</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>2436</v>
+        <v>2435</v>
       </c>
       <c r="K8" s="19" t="s">
         <v>1001</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>2499</v>
+        <v>2497</v>
       </c>
       <c r="N8" s="22" t="s">
         <v>1245</v>
@@ -20643,10 +20705,10 @@
         <v>959</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>2374</v>
+        <v>2373</v>
       </c>
       <c r="H9" s="19" t="s">
         <v>2201</v>
@@ -20725,10 +20787,10 @@
         <v>556</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>2437</v>
+        <v>2436</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>2415</v>
+        <v>2414</v>
       </c>
       <c r="H11" s="19" t="s">
         <v>2207</v>
@@ -20766,7 +20828,7 @@
         <v>961</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>2416</v>
+        <v>2415</v>
       </c>
       <c r="G12" s="19" t="s">
         <v>2250</v>
@@ -20807,7 +20869,7 @@
         <v>963</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>2417</v>
+        <v>2416</v>
       </c>
       <c r="G13" s="19" t="s">
         <v>2251</v>
@@ -20848,7 +20910,7 @@
         <v>964</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>2418</v>
+        <v>2417</v>
       </c>
       <c r="G14" s="19" t="s">
         <v>2252</v>
@@ -20866,7 +20928,7 @@
         <v>1023</v>
       </c>
       <c r="L14" s="19" t="s">
-        <v>2419</v>
+        <v>2418</v>
       </c>
       <c r="N14" s="22" t="s">
         <v>1238</v>
@@ -20889,7 +20951,7 @@
         <v>966</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="G15" s="19" t="s">
         <v>2253</v>
@@ -20901,7 +20963,7 @@
         <v>1008</v>
       </c>
       <c r="J15" s="19" t="s">
-        <v>2665</v>
+        <v>2663</v>
       </c>
       <c r="K15" s="19" t="s">
         <v>1024</v>
@@ -20930,10 +20992,10 @@
         <v>968</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>2421</v>
+        <v>2420</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
       <c r="H16" s="19" t="s">
         <v>2220</v>
@@ -20971,7 +21033,7 @@
         <v>972</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>2422</v>
+        <v>2421</v>
       </c>
       <c r="G17" s="19" t="s">
         <v>2254</v>
@@ -20983,7 +21045,7 @@
         <v>1010</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>2438</v>
+        <v>2437</v>
       </c>
       <c r="K17" s="19" t="s">
         <v>1026</v>
@@ -21012,10 +21074,10 @@
         <v>975</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>2423</v>
+        <v>2422</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>2376</v>
+        <v>2375</v>
       </c>
       <c r="H18" s="19" t="s">
         <v>2225</v>
@@ -21094,7 +21156,7 @@
         <v>979</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>2424</v>
+        <v>2423</v>
       </c>
       <c r="G20" s="19" t="s">
         <v>2256</v>
@@ -21135,7 +21197,7 @@
         <v>977</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>2425</v>
+        <v>2424</v>
       </c>
       <c r="G21" s="19" t="s">
         <v>2257</v>
@@ -21176,10 +21238,10 @@
         <v>984</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>2570</v>
+        <v>2568</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>2379</v>
+        <v>2378</v>
       </c>
       <c r="H22" s="19" t="s">
         <v>2237</v>
@@ -21223,7 +21285,7 @@
         <v>1017</v>
       </c>
       <c r="G23" s="19" t="s">
-        <v>2377</v>
+        <v>2376</v>
       </c>
       <c r="H23" s="19" t="s">
         <v>2240</v>
@@ -21238,7 +21300,7 @@
         <v>1019</v>
       </c>
       <c r="L23" s="19" t="s">
-        <v>2439</v>
+        <v>2438</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>2242</v>
@@ -21264,10 +21326,10 @@
         <v>987</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>2478</v>
+        <v>2476</v>
       </c>
       <c r="G24" s="19" t="s">
-        <v>2426</v>
+        <v>2425</v>
       </c>
       <c r="H24" s="19" t="s">
         <v>2243</v>
@@ -21276,13 +21338,13 @@
         <v>1033</v>
       </c>
       <c r="J24" s="19" t="s">
-        <v>2427</v>
+        <v>2426</v>
       </c>
       <c r="K24" s="19" t="s">
         <v>1031</v>
       </c>
       <c r="L24" s="19" t="s">
-        <v>2428</v>
+        <v>2427</v>
       </c>
       <c r="M24" s="1" t="s">
         <v>2244</v>
@@ -21308,10 +21370,10 @@
         <v>981</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>2429</v>
+        <v>2428</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>2378</v>
+        <v>2377</v>
       </c>
       <c r="H25" s="19" t="s">
         <v>2245</v>
@@ -21326,7 +21388,7 @@
         <v>1020</v>
       </c>
       <c r="L25" s="19" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
       <c r="M25" s="1" t="s">
         <v>2247</v>
@@ -21352,10 +21414,10 @@
         <v>2284</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
       <c r="G26" s="19" t="s">
-        <v>2457</v>
+        <v>2456</v>
       </c>
       <c r="H26" s="19" t="s">
         <v>2292</v>
@@ -21370,10 +21432,10 @@
         <v>2303</v>
       </c>
       <c r="L26" s="19" t="s">
-        <v>2458</v>
+        <v>2457</v>
       </c>
       <c r="N26" s="6" t="s">
-        <v>2355</v>
+        <v>2354</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="188.5" x14ac:dyDescent="0.35">
@@ -21393,13 +21455,13 @@
         <v>2285</v>
       </c>
       <c r="F27" s="19" t="s">
+        <v>2460</v>
+      </c>
+      <c r="G27" s="19" t="s">
+        <v>2459</v>
+      </c>
+      <c r="H27" s="19" t="s">
         <v>2461</v>
-      </c>
-      <c r="G27" s="19" t="s">
-        <v>2460</v>
-      </c>
-      <c r="H27" s="19" t="s">
-        <v>2462</v>
       </c>
       <c r="I27" s="19" t="s">
         <v>2298</v>
@@ -21411,10 +21473,10 @@
         <v>2297</v>
       </c>
       <c r="L27" s="19" t="s">
-        <v>2440</v>
+        <v>2439</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>2356</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
@@ -21434,13 +21496,13 @@
         <v>2286</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>2432</v>
+        <v>2431</v>
       </c>
       <c r="G28" s="19" t="s">
-        <v>2459</v>
+        <v>2458</v>
       </c>
       <c r="H28" s="19" t="s">
-        <v>2367</v>
+        <v>2366</v>
       </c>
       <c r="I28" s="19" t="s">
         <v>2299</v>
@@ -21455,7 +21517,7 @@
         <v>2302</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>2357</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="159.5" x14ac:dyDescent="0.35">
@@ -21475,13 +21537,13 @@
         <v>2290</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>2442</v>
+        <v>2441</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>2463</v>
+        <v>2673</v>
       </c>
       <c r="I29" s="19" t="s">
         <v>2304</v>
@@ -21493,10 +21555,10 @@
         <v>2306</v>
       </c>
       <c r="L29" s="19" t="s">
-        <v>2441</v>
+        <v>2440</v>
       </c>
       <c r="N29" s="6" t="s">
-        <v>2358</v>
+        <v>2357</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="246.5" x14ac:dyDescent="0.35">
@@ -21516,7 +21578,7 @@
         <v>2291</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>2434</v>
+        <v>2433</v>
       </c>
       <c r="G30" s="19" t="s">
         <v>2307</v>
@@ -21537,7 +21599,7 @@
         <v>2307</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>2359</v>
+        <v>2358</v>
       </c>
     </row>
   </sheetData>
@@ -21575,11 +21637,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B78993A1-ED23-4BA3-9898-CFB8D57B537E}">
-  <dimension ref="A1:N159"/>
+  <dimension ref="A1:N166"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L142" sqref="L142"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N161" sqref="N161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22387,7 +22449,7 @@
         <v>5</v>
       </c>
       <c r="L19" s="23" t="s">
-        <v>2610</v>
+        <v>2608</v>
       </c>
       <c r="M19" s="25" t="s">
         <v>871</v>
@@ -23181,7 +23243,7 @@
         <v>0</v>
       </c>
       <c r="L38" s="23" t="s">
-        <v>2609</v>
+        <v>2607</v>
       </c>
       <c r="M38" s="25" t="s">
         <v>871</v>
@@ -23313,7 +23375,7 @@
         <v>0</v>
       </c>
       <c r="L41" s="23" t="s">
-        <v>2611</v>
+        <v>2609</v>
       </c>
       <c r="M41" s="25" t="s">
         <v>871</v>
@@ -25028,7 +25090,7 @@
         <v>0</v>
       </c>
       <c r="L82" s="23" t="s">
-        <v>2612</v>
+        <v>2610</v>
       </c>
       <c r="M82" s="25" t="s">
         <v>871</v>
@@ -26110,7 +26172,7 @@
         <v>100</v>
       </c>
       <c r="L108" s="23" t="s">
-        <v>2406</v>
+        <v>2405</v>
       </c>
       <c r="M108" s="25" t="s">
         <v>871</v>
@@ -26198,7 +26260,7 @@
         <v>0</v>
       </c>
       <c r="L110" s="23" t="s">
-        <v>2613</v>
+        <v>2611</v>
       </c>
       <c r="M110" s="25" t="s">
         <v>871</v>
@@ -26579,7 +26641,7 @@
         <v>0</v>
       </c>
       <c r="L119" s="23" t="s">
-        <v>2321</v>
+        <v>2320</v>
       </c>
       <c r="M119" s="25" t="s">
         <v>1134</v>
@@ -27165,7 +27227,7 @@
         <v>0</v>
       </c>
       <c r="L133" s="23" t="s">
-        <v>2569</v>
+        <v>2567</v>
       </c>
       <c r="N133" s="27" t="s">
         <v>1388</v>
@@ -27253,7 +27315,7 @@
         <v>871</v>
       </c>
       <c r="N135" s="27" t="s">
-        <v>2445</v>
+        <v>2444</v>
       </c>
     </row>
     <row r="136" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
@@ -27379,7 +27441,7 @@
         <v>0</v>
       </c>
       <c r="L138" s="23" t="s">
-        <v>2614</v>
+        <v>2612</v>
       </c>
       <c r="M138" s="25" t="s">
         <v>871</v>
@@ -27690,7 +27752,7 @@
         <v>2318</v>
       </c>
       <c r="N145" s="33" t="s">
-        <v>2443</v>
+        <v>2442</v>
       </c>
     </row>
     <row r="146" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
@@ -27728,15 +27790,15 @@
         <v>0</v>
       </c>
       <c r="L146" s="23" t="s">
-        <v>2320</v>
+        <v>2319</v>
       </c>
       <c r="N146" s="30" t="s">
-        <v>2354</v>
-      </c>
-    </row>
-    <row r="147" spans="1:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="A147" s="23" t="s">
-        <v>2311</v>
+        <v>2353</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A147" s="25" t="s">
+        <v>2674</v>
       </c>
       <c r="B147" s="26">
         <v>7</v>
@@ -27745,16 +27807,16 @@
         <v>544</v>
       </c>
       <c r="D147" s="26">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="E147" s="26">
         <v>0</v>
       </c>
       <c r="F147" s="26">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G147" s="26">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="H147" s="26">
         <v>1</v>
@@ -27769,15 +27831,12 @@
         <v>0</v>
       </c>
       <c r="L147" s="23" t="s">
-        <v>2319</v>
-      </c>
-      <c r="N147" s="30" t="s">
-        <v>2350</v>
-      </c>
-    </row>
-    <row r="148" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A148" s="23" t="s">
-        <v>2312</v>
+        <v>2676</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A148" s="25" t="s">
+        <v>2675</v>
       </c>
       <c r="B148" s="26">
         <v>7</v>
@@ -27786,22 +27845,22 @@
         <v>544</v>
       </c>
       <c r="D148" s="26">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="E148" s="26">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="F148" s="26">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G148" s="26">
-        <v>0.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H148" s="26">
         <v>1</v>
       </c>
       <c r="I148" s="26">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="J148" s="26">
         <v>0</v>
@@ -27810,15 +27869,12 @@
         <v>0</v>
       </c>
       <c r="L148" s="23" t="s">
-        <v>2405</v>
-      </c>
-      <c r="N148" s="30" t="s">
-        <v>2349</v>
-      </c>
-    </row>
-    <row r="149" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+        <v>2677</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A149" s="23" t="s">
-        <v>2313</v>
+        <v>2311</v>
       </c>
       <c r="B149" s="26">
         <v>7</v>
@@ -27827,22 +27883,22 @@
         <v>544</v>
       </c>
       <c r="D149" s="26">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="E149" s="26">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="F149" s="26">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G149" s="26">
-        <v>0.75</v>
+        <v>1.5</v>
       </c>
       <c r="H149" s="26">
         <v>1</v>
       </c>
       <c r="I149" s="26">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="J149" s="26">
         <v>0</v>
@@ -27851,15 +27907,15 @@
         <v>0</v>
       </c>
       <c r="L149" s="23" t="s">
-        <v>2322</v>
+        <v>2678</v>
       </c>
       <c r="N149" s="30" t="s">
-        <v>2348</v>
-      </c>
-    </row>
-    <row r="150" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+        <v>2349</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A150" s="23" t="s">
-        <v>2314</v>
+        <v>2679</v>
       </c>
       <c r="B150" s="26">
         <v>7</v>
@@ -27868,22 +27924,22 @@
         <v>544</v>
       </c>
       <c r="D150" s="26">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="E150" s="26">
+        <v>0</v>
+      </c>
+      <c r="F150" s="26">
         <v>0.1</v>
       </c>
-      <c r="F150" s="26">
-        <v>0.3</v>
-      </c>
       <c r="G150" s="26">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
       <c r="H150" s="26">
         <v>1</v>
       </c>
       <c r="I150" s="26">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="J150" s="26">
         <v>0</v>
@@ -27892,15 +27948,12 @@
         <v>0</v>
       </c>
       <c r="L150" s="23" t="s">
-        <v>2455</v>
-      </c>
-      <c r="N150" s="30" t="s">
-        <v>2352</v>
-      </c>
-    </row>
-    <row r="151" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+        <v>2680</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A151" s="23" t="s">
-        <v>2315</v>
+        <v>2681</v>
       </c>
       <c r="B151" s="26">
         <v>7</v>
@@ -27909,22 +27962,22 @@
         <v>544</v>
       </c>
       <c r="D151" s="26">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="E151" s="26">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="F151" s="26">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="G151" s="26">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="H151" s="26">
         <v>1</v>
       </c>
       <c r="I151" s="26">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="J151" s="26">
         <v>0</v>
@@ -27933,15 +27986,12 @@
         <v>0</v>
       </c>
       <c r="L151" s="23" t="s">
-        <v>2323</v>
-      </c>
-      <c r="N151" s="30" t="s">
-        <v>2351</v>
-      </c>
-    </row>
-    <row r="152" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+        <v>2682</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A152" s="23" t="s">
-        <v>2316</v>
+        <v>2312</v>
       </c>
       <c r="B152" s="26">
         <v>7</v>
@@ -27950,22 +28000,22 @@
         <v>544</v>
       </c>
       <c r="D152" s="26">
-        <v>2200</v>
+        <v>400</v>
       </c>
       <c r="E152" s="26">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F152" s="26">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G152" s="26">
-        <v>0.35</v>
+        <v>0.8</v>
       </c>
       <c r="H152" s="26">
         <v>1</v>
       </c>
       <c r="I152" s="26">
-        <v>190</v>
+        <v>50</v>
       </c>
       <c r="J152" s="26">
         <v>0</v>
@@ -27974,15 +28024,15 @@
         <v>0</v>
       </c>
       <c r="L152" s="23" t="s">
-        <v>2456</v>
+        <v>2404</v>
       </c>
       <c r="N152" s="30" t="s">
-        <v>2353</v>
-      </c>
-    </row>
-    <row r="153" spans="1:14" ht="130.5" x14ac:dyDescent="0.35">
+        <v>2348</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A153" s="23" t="s">
-        <v>2317</v>
+        <v>2313</v>
       </c>
       <c r="B153" s="26">
         <v>7</v>
@@ -27991,41 +28041,360 @@
         <v>544</v>
       </c>
       <c r="D153" s="26">
-        <v>43700000</v>
+        <v>400</v>
       </c>
       <c r="E153" s="26">
-        <v>0.55000000000000004</v>
+        <v>0.3</v>
       </c>
       <c r="F153" s="26">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G153" s="26">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="H153" s="26">
         <v>1</v>
       </c>
       <c r="I153" s="26">
+        <v>40</v>
+      </c>
+      <c r="J153" s="26">
+        <v>0</v>
+      </c>
+      <c r="K153" s="26">
+        <v>0</v>
+      </c>
+      <c r="L153" s="23" t="s">
+        <v>2321</v>
+      </c>
+      <c r="N153" s="30" t="s">
+        <v>2347</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A154" s="23" t="s">
+        <v>2314</v>
+      </c>
+      <c r="B154" s="26">
+        <v>7</v>
+      </c>
+      <c r="C154" s="26" t="s">
+        <v>544</v>
+      </c>
+      <c r="D154" s="26">
+        <v>500</v>
+      </c>
+      <c r="E154" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="F154" s="26">
+        <v>0.3</v>
+      </c>
+      <c r="G154" s="26">
+        <v>0.85</v>
+      </c>
+      <c r="H154" s="26">
+        <v>1</v>
+      </c>
+      <c r="I154" s="26">
+        <v>110</v>
+      </c>
+      <c r="J154" s="26">
+        <v>0</v>
+      </c>
+      <c r="K154" s="26">
+        <v>0</v>
+      </c>
+      <c r="L154" s="23" t="s">
+        <v>2454</v>
+      </c>
+      <c r="N154" s="30" t="s">
+        <v>2351</v>
+      </c>
+    </row>
+    <row r="155" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A155" s="23" t="s">
+        <v>2315</v>
+      </c>
+      <c r="B155" s="26">
+        <v>7</v>
+      </c>
+      <c r="C155" s="26" t="s">
+        <v>544</v>
+      </c>
+      <c r="D155" s="26">
+        <v>600</v>
+      </c>
+      <c r="E155" s="26">
+        <v>0.3</v>
+      </c>
+      <c r="F155" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="G155" s="26">
+        <v>0.7</v>
+      </c>
+      <c r="H155" s="26">
+        <v>1</v>
+      </c>
+      <c r="I155" s="26">
+        <v>40</v>
+      </c>
+      <c r="J155" s="26">
+        <v>0</v>
+      </c>
+      <c r="K155" s="26">
+        <v>0</v>
+      </c>
+      <c r="L155" s="23" t="s">
+        <v>2322</v>
+      </c>
+      <c r="N155" s="30" t="s">
+        <v>2350</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A156" s="23" t="s">
+        <v>2683</v>
+      </c>
+      <c r="B156" s="26">
+        <v>7</v>
+      </c>
+      <c r="C156" s="26" t="s">
+        <v>544</v>
+      </c>
+      <c r="D156" s="26">
+        <v>600</v>
+      </c>
+      <c r="E156" s="26">
+        <v>0.6</v>
+      </c>
+      <c r="F156" s="26">
+        <v>0</v>
+      </c>
+      <c r="G156" s="26">
+        <v>0.25</v>
+      </c>
+      <c r="H156" s="26">
+        <v>1</v>
+      </c>
+      <c r="I156" s="26">
+        <v>40</v>
+      </c>
+      <c r="J156" s="26">
+        <v>0</v>
+      </c>
+      <c r="K156" s="26">
+        <v>0</v>
+      </c>
+      <c r="L156" s="23" t="s">
+        <v>2686</v>
+      </c>
+    </row>
+    <row r="157" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A157" s="23" t="s">
+        <v>2684</v>
+      </c>
+      <c r="B157" s="26">
+        <v>7</v>
+      </c>
+      <c r="C157" s="26" t="s">
+        <v>544</v>
+      </c>
+      <c r="D157" s="26">
+        <v>1200</v>
+      </c>
+      <c r="E157" s="26">
+        <v>0</v>
+      </c>
+      <c r="F157" s="26">
+        <v>0.25</v>
+      </c>
+      <c r="G157" s="26">
+        <v>0.8</v>
+      </c>
+      <c r="H157" s="26">
+        <v>1</v>
+      </c>
+      <c r="I157" s="26">
+        <v>60</v>
+      </c>
+      <c r="J157" s="26">
+        <v>0</v>
+      </c>
+      <c r="K157" s="26">
+        <v>0</v>
+      </c>
+      <c r="L157" s="23" t="s">
+        <v>2688</v>
+      </c>
+    </row>
+    <row r="158" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+      <c r="A158" s="23" t="s">
+        <v>2685</v>
+      </c>
+      <c r="B158" s="26">
+        <v>7</v>
+      </c>
+      <c r="C158" s="26" t="s">
+        <v>544</v>
+      </c>
+      <c r="D158" s="26">
+        <v>2000</v>
+      </c>
+      <c r="E158" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F158" s="26">
+        <v>0</v>
+      </c>
+      <c r="G158" s="26">
+        <v>0.65</v>
+      </c>
+      <c r="H158" s="26">
+        <v>1</v>
+      </c>
+      <c r="I158" s="26">
+        <v>75</v>
+      </c>
+      <c r="J158" s="26">
+        <v>0</v>
+      </c>
+      <c r="K158" s="26">
+        <v>0</v>
+      </c>
+      <c r="L158" s="23" t="s">
+        <v>2687</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14" ht="87" x14ac:dyDescent="0.35">
+      <c r="A159" s="23" t="s">
+        <v>2316</v>
+      </c>
+      <c r="B159" s="26">
+        <v>7</v>
+      </c>
+      <c r="C159" s="26" t="s">
+        <v>544</v>
+      </c>
+      <c r="D159" s="26">
+        <v>2200</v>
+      </c>
+      <c r="E159" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F159" s="26">
+        <v>0</v>
+      </c>
+      <c r="G159" s="26">
+        <v>0.35</v>
+      </c>
+      <c r="H159" s="26">
+        <v>1</v>
+      </c>
+      <c r="I159" s="26">
+        <v>190</v>
+      </c>
+      <c r="J159" s="26">
+        <v>0</v>
+      </c>
+      <c r="K159" s="26">
+        <v>0</v>
+      </c>
+      <c r="L159" s="23" t="s">
+        <v>2455</v>
+      </c>
+      <c r="N159" s="30" t="s">
+        <v>2352</v>
+      </c>
+    </row>
+    <row r="160" spans="1:14" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A160" s="23" t="s">
+        <v>2317</v>
+      </c>
+      <c r="B160" s="26">
+        <v>7</v>
+      </c>
+      <c r="C160" s="26" t="s">
+        <v>544</v>
+      </c>
+      <c r="D160" s="26">
+        <v>43700000</v>
+      </c>
+      <c r="E160" s="26">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F160" s="26">
+        <v>0.3</v>
+      </c>
+      <c r="G160" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="H160" s="26">
+        <v>1</v>
+      </c>
+      <c r="I160" s="26">
         <v>4200</v>
       </c>
-      <c r="J153" s="26">
-        <v>0</v>
-      </c>
-      <c r="K153" s="26">
-        <v>0</v>
-      </c>
-      <c r="L153" s="23" t="s">
-        <v>2407</v>
-      </c>
-      <c r="M153" s="25" t="s">
+      <c r="J160" s="26">
+        <v>0</v>
+      </c>
+      <c r="K160" s="26">
+        <v>0</v>
+      </c>
+      <c r="L160" s="23" t="s">
+        <v>2406</v>
+      </c>
+      <c r="M160" s="25" t="s">
         <v>871</v>
       </c>
-      <c r="N153" s="33" t="s">
-        <v>2444</v>
-      </c>
-    </row>
-    <row r="159" spans="1:14" ht="26.5" x14ac:dyDescent="0.35">
-      <c r="N159" s="29"/>
+      <c r="N160" s="33" t="s">
+        <v>2443</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14" ht="145" x14ac:dyDescent="0.35">
+      <c r="A161" s="23" t="s">
+        <v>2689</v>
+      </c>
+      <c r="B161" s="26">
+        <v>7</v>
+      </c>
+      <c r="C161" s="26" t="s">
+        <v>544</v>
+      </c>
+      <c r="D161" s="26">
+        <v>43700000</v>
+      </c>
+      <c r="E161" s="26">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F161" s="26">
+        <v>0.3</v>
+      </c>
+      <c r="G161" s="26">
+        <v>1.5</v>
+      </c>
+      <c r="H161" s="26">
+        <v>1</v>
+      </c>
+      <c r="I161" s="26">
+        <v>4200</v>
+      </c>
+      <c r="J161" s="26">
+        <v>0</v>
+      </c>
+      <c r="K161" s="26">
+        <v>0</v>
+      </c>
+      <c r="L161" s="23" t="s">
+        <v>2690</v>
+      </c>
+      <c r="M161" s="25" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" ht="26.5" x14ac:dyDescent="0.35">
+      <c r="N166" s="29"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -28172,7 +28541,7 @@
     <hyperlink ref="N144" r:id="rId141" xr:uid="{94F8F863-4995-440F-AC42-04ECC832B018}"/>
     <hyperlink ref="N22" r:id="rId142" xr:uid="{ABC9D378-BFCA-4E9E-BF38-C445452246DC}"/>
     <hyperlink ref="N145" r:id="rId143" xr:uid="{AD081480-D024-455C-AF62-AA070797A984}"/>
-    <hyperlink ref="N153" r:id="rId144" xr:uid="{8E4D9ECA-CBBA-4DD5-894C-9A70E7D74938}"/>
+    <hyperlink ref="N160" r:id="rId144" xr:uid="{8E4D9ECA-CBBA-4DD5-894C-9A70E7D74938}"/>
     <hyperlink ref="N135" r:id="rId145" xr:uid="{470152B2-D794-462F-A63D-55A53D73F3B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -34226,15 +34595,15 @@
         <v>7</v>
       </c>
       <c r="C242" s="10" t="s">
-        <v>2324</v>
+        <v>2323</v>
       </c>
       <c r="D242" s="12" t="s">
-        <v>2344</v>
+        <v>2343</v>
       </c>
       <c r="E242" s="12"/>
       <c r="F242" s="14"/>
       <c r="G242" s="17" t="s">
-        <v>2334</v>
+        <v>2333</v>
       </c>
       <c r="H242" s="18"/>
     </row>
@@ -34247,19 +34616,19 @@
         <v>7</v>
       </c>
       <c r="C243" s="10" t="s">
-        <v>2325</v>
+        <v>2324</v>
       </c>
       <c r="D243" s="12" t="s">
-        <v>2345</v>
+        <v>2344</v>
       </c>
       <c r="E243" s="12" t="s">
         <v>2166</v>
       </c>
       <c r="F243" s="14" t="s">
-        <v>2360</v>
+        <v>2359</v>
       </c>
       <c r="G243" s="18" t="s">
-        <v>2335</v>
+        <v>2334</v>
       </c>
       <c r="H243" s="18"/>
     </row>
@@ -34272,19 +34641,19 @@
         <v>7</v>
       </c>
       <c r="C244" s="10" t="s">
-        <v>2326</v>
+        <v>2325</v>
       </c>
       <c r="D244" s="12" t="s">
-        <v>2346</v>
+        <v>2345</v>
       </c>
       <c r="E244" s="12" t="s">
         <v>2165</v>
       </c>
       <c r="F244" s="14" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="G244" s="18" t="s">
-        <v>2336</v>
+        <v>2335</v>
       </c>
       <c r="H244" s="18"/>
     </row>
@@ -34297,19 +34666,19 @@
         <v>7</v>
       </c>
       <c r="C245" s="10" t="s">
-        <v>2327</v>
+        <v>2326</v>
       </c>
       <c r="D245" s="12" t="s">
-        <v>2347</v>
+        <v>2346</v>
       </c>
       <c r="E245" s="12" t="s">
         <v>2166</v>
       </c>
       <c r="F245" s="14" t="s">
-        <v>2362</v>
+        <v>2361</v>
       </c>
       <c r="G245" s="18" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
       <c r="H245" s="18"/>
     </row>
@@ -34322,17 +34691,17 @@
         <v>7</v>
       </c>
       <c r="C246" s="10" t="s">
-        <v>2328</v>
+        <v>2327</v>
       </c>
       <c r="D246" s="12" t="s">
-        <v>2344</v>
+        <v>2343</v>
       </c>
       <c r="E246" s="12" t="s">
         <v>2165</v>
       </c>
       <c r="F246" s="14"/>
       <c r="G246" s="18" t="s">
-        <v>2338</v>
+        <v>2337</v>
       </c>
       <c r="H246" s="18"/>
     </row>
@@ -34345,19 +34714,19 @@
         <v>7</v>
       </c>
       <c r="C247" s="10" t="s">
-        <v>2329</v>
+        <v>2328</v>
       </c>
       <c r="D247" s="12" t="s">
-        <v>2345</v>
+        <v>2344</v>
       </c>
       <c r="E247" s="12" t="s">
         <v>2166</v>
       </c>
       <c r="F247" s="14" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="G247" s="18" t="s">
-        <v>2339</v>
+        <v>2338</v>
       </c>
       <c r="H247" s="18"/>
     </row>
@@ -34370,19 +34739,19 @@
         <v>7</v>
       </c>
       <c r="C248" s="10" t="s">
-        <v>2330</v>
+        <v>2329</v>
       </c>
       <c r="D248" s="12" t="s">
-        <v>2346</v>
+        <v>2345</v>
       </c>
       <c r="E248" s="12" t="s">
         <v>2165</v>
       </c>
       <c r="F248" s="14" t="s">
-        <v>2404</v>
+        <v>2403</v>
       </c>
       <c r="G248" s="18" t="s">
-        <v>2340</v>
+        <v>2339</v>
       </c>
       <c r="H248" s="18"/>
     </row>
@@ -34395,19 +34764,19 @@
         <v>7</v>
       </c>
       <c r="C249" s="10" t="s">
-        <v>2331</v>
+        <v>2330</v>
       </c>
       <c r="D249" s="12" t="s">
-        <v>2347</v>
+        <v>2346</v>
       </c>
       <c r="E249" s="12" t="s">
         <v>2166</v>
       </c>
       <c r="F249" s="14" t="s">
-        <v>2363</v>
+        <v>2362</v>
       </c>
       <c r="G249" s="18" t="s">
-        <v>2341</v>
+        <v>2340</v>
       </c>
       <c r="H249" s="18"/>
     </row>
@@ -34420,19 +34789,19 @@
         <v>7</v>
       </c>
       <c r="C250" s="10" t="s">
-        <v>2332</v>
+        <v>2331</v>
       </c>
       <c r="D250" s="12" t="s">
-        <v>2344</v>
+        <v>2343</v>
       </c>
       <c r="E250" s="12" t="s">
         <v>2165</v>
       </c>
       <c r="F250" s="14" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="G250" s="18" t="s">
-        <v>2342</v>
+        <v>2341</v>
       </c>
       <c r="H250" s="18"/>
     </row>
@@ -34445,19 +34814,19 @@
         <v>7</v>
       </c>
       <c r="C251" s="10" t="s">
-        <v>2333</v>
+        <v>2332</v>
       </c>
       <c r="D251" s="12" t="s">
-        <v>2345</v>
+        <v>2344</v>
       </c>
       <c r="E251" s="12" t="s">
         <v>2165</v>
       </c>
       <c r="F251" s="14" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="G251" s="18" t="s">
-        <v>2343</v>
+        <v>2342</v>
       </c>
       <c r="H251" s="18" t="s">
         <v>871</v>
@@ -37183,7 +37552,7 @@
         <v>546</v>
       </c>
       <c r="C20" t="s">
-        <v>2364</v>
+        <v>2363</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -37194,7 +37563,7 @@
         <v>868</v>
       </c>
       <c r="C21" t="s">
-        <v>2366</v>
+        <v>2365</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -37205,7 +37574,7 @@
         <v>534</v>
       </c>
       <c r="C22" t="s">
-        <v>2365</v>
+        <v>2364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change some enemy text
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\data\q-z\Realm Defense\CyraBot\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951A4C67-EF8A-43AC-BBFE-06AF42BE3B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8B2A6F-2DA6-46FC-9BEC-F76A909D9CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8947,9 +8947,6 @@
     <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/6/6c/T67._Yamada.PNG/revision/latest?cb=20220504124529</t>
   </si>
   <si>
-    <t>**Judoka**: 2.6s cooldown, melee attack is seperated into 4 light attacks `(0.2 ND) PD` and 1 heavy attack `(0.5 ND) PD` with total `(1.3 ND) PD`.</t>
-  </si>
-  <si>
     <t>**Melee**: 2s cooldown, deals `(1 ND) MD` to a target.
 **Ama no Murakumo no Turugi**: 10s cooldown, empowers 2 random allies for 20s. Doubles their speed and health and increases damage x10.
 **Inside Beauty**: Her appearance now matches her spirit. Ama no Murakumo no Turugi's cooldown is reduced to 5s</t>
@@ -9021,78 +9018,81 @@
 **Unhandleable Power**: Gains complete invincibility before wave 5.</t>
   </si>
   <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/f/f5/211.jpg/revision/latest?cb=20220704185235</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/5/5a/212.jpg/revision/latest?cb=20220704185246</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/9/9d/213.jpg/revision/latest?cb=20220704185255</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/2/27/214.jpg/revision/latest?cb=20220704185306</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/b/b4/215.jpg/revision/latest?cb=20220704185314</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/f/fa/216.jpg/revision/latest?cb=20220704185322</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/f/fa/217.jpg/revision/latest?cb=20220704185329</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/8d/218.jpg/revision/latest?cb=20220704185339</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/1/1d/219.jpg/revision/latest?cb=20220704185347</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/5/5a/220.jpg/revision/latest?cb=20220704185353</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/5/51/Elysium_Pebble.jpg/revision/latest?cb=20220704185403</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/84/Omega_Spider.jpg/revision/latest?cb=20220704185409</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/89/Chameleon_Sentry.jpg/revision/latest?cb=20220704185415</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/5/5a/Slime_Shooter.jpg/revision/latest?cb=20220704185425</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/6/66/Rock_Flinger.jpg/revision/latest?cb=20220704185439</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/3/3f/Satyr_Sentinel.jpg/revision/latest?cb=20220704185432</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/8f/Elysium_Rock.jpg/revision/latest?cb=20220704185448</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/1/19/Arachnamech.jpg/revision/latest?cb=20220704185458</t>
+  </si>
+  <si>
+    <t>Lever switch on bottom right (*trap*): damage and stun enemies</t>
+  </si>
+  <si>
+    <t>**Melee**: 1.75s cooldown, deals `(1 ND) PD`.
+**Entangle**: 6s cooldown, entangles 2 enemies in range 2 or 1 enemy in melee, deals `(0.5 ND) PD + (0.5 ND) MD`, make them not able to move for 3s, this skill can be used 25 times.
+**Rock Thrower**: 2s cooldown, throw a rock to an enemy in range 2.5 and deals `(1 ND) PD` to all enemies in AOE range 1, max 25 shots.</t>
+  </si>
+  <si>
+    <t>**Melee**: 0.6s cooldown, deals `(1 ND) PD`.
+**Stealth**: Cloak at the beginning, move speed +0.5 when cloak, remove cloak when damaged.
+**Bionics**: When it's uncloaked and unterrified, it starts pulling enemies: 2s cooldown, pulls an enemy in range 3 and deals `(0.25 ND) PD + (0.75 ND) MD`, this attack has lifesteal ratio 0.5, and can be used 30 times.</t>
+  </si>
+  <si>
+    <t>**Judoka**: 2.6s cooldown, melee attack is seperated into 4 light attacks `(0.2 ND) PD` and 1 heavy attack `(0.5 ND) PD`, deals totally `(1.3 ND) PD`.</t>
+  </si>
+  <si>
     <t>**Slam**: 3s cooldown, deals `(1 ND) PD` to enemies in AOE range 2 and stun them for 2s.
 **Stab**: If there is an enemy covered by slime in range 2, attack deals `(1 ND) PD + (0.5 ND) MD` with 0.75 lifesteal ratio, and applies bleeding for 10s.
 **Slime Shot**: 10s cooldown, launches 3 shots to enemies in range 3.75, each shot covers all enemies in AOE range 1 by slime: move speed x0.6 and damage x0.8, last 10s, and give ground slimes in AOE range 1 a slime cover buff: HP x2, damage x1.5.
 **Powered Slime Shot**: 15s cooldown, launch 1 shot to an enemy in range 3, covers all enemies in AOE range 2 by slime, and give ground slimes in AOE range 2 a slime cover buff.
-**Spider Web**: Leap in or out of battlefield when the wave progresses, when leaping in, deals `(1 ND) PD` to enemies in AOE range 3 and stuns them for 5s.</t>
-  </si>
-  <si>
-    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/f/f5/211.jpg/revision/latest?cb=20220704185235</t>
-  </si>
-  <si>
-    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/5/5a/212.jpg/revision/latest?cb=20220704185246</t>
-  </si>
-  <si>
-    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/9/9d/213.jpg/revision/latest?cb=20220704185255</t>
-  </si>
-  <si>
-    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/2/27/214.jpg/revision/latest?cb=20220704185306</t>
-  </si>
-  <si>
-    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/b/b4/215.jpg/revision/latest?cb=20220704185314</t>
-  </si>
-  <si>
-    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/f/fa/216.jpg/revision/latest?cb=20220704185322</t>
-  </si>
-  <si>
-    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/f/fa/217.jpg/revision/latest?cb=20220704185329</t>
-  </si>
-  <si>
-    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/8d/218.jpg/revision/latest?cb=20220704185339</t>
-  </si>
-  <si>
-    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/1/1d/219.jpg/revision/latest?cb=20220704185347</t>
-  </si>
-  <si>
-    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/5/5a/220.jpg/revision/latest?cb=20220704185353</t>
-  </si>
-  <si>
-    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/5/51/Elysium_Pebble.jpg/revision/latest?cb=20220704185403</t>
-  </si>
-  <si>
-    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/84/Omega_Spider.jpg/revision/latest?cb=20220704185409</t>
-  </si>
-  <si>
-    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/89/Chameleon_Sentry.jpg/revision/latest?cb=20220704185415</t>
-  </si>
-  <si>
-    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/5/5a/Slime_Shooter.jpg/revision/latest?cb=20220704185425</t>
-  </si>
-  <si>
-    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/6/66/Rock_Flinger.jpg/revision/latest?cb=20220704185439</t>
-  </si>
-  <si>
-    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/3/3f/Satyr_Sentinel.jpg/revision/latest?cb=20220704185432</t>
-  </si>
-  <si>
-    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/8/8f/Elysium_Rock.jpg/revision/latest?cb=20220704185448</t>
-  </si>
-  <si>
-    <t>https://static.wikia.nocookie.net/realm-defense-hero-legends-td/images/1/19/Arachnamech.jpg/revision/latest?cb=20220704185458</t>
-  </si>
-  <si>
-    <t>**Melee**: 0.6s cooldown, deals `(1 ND) PD`.
-**Cloak**: remove cloak when damaged.
-**Bionics**: When it's uncloaked and unterrified, it starts pulling enemies: 2s cooldown, pulls an enemy in range 3 and deals `(0.25 ND) PD + (0.75 ND) MD`, this attack has lifesteal ratio 0.5, and can be used 30 times.</t>
-  </si>
-  <si>
-    <t>Lever switch on bottom right (*trap*): damage and stun enemies</t>
-  </si>
-  <si>
-    <t>**Melee**: 1.75s cooldown, deals `(1 ND) PD`.
-**Entangle**: 6s cooldown, entangles 2 enemies in range 2 or 1 enemy in melee, deals `(0.5 ND) PD + (0.5 ND) MD`, make them not able to move for 3s, this skill can be used 25 times.
-**Rock Thrower**: 2s cooldown, throw a rock to an enemy in range 2.5 and deals `(1 ND) PD` to all enemies in AOE range 1, max 25 shots.</t>
+**Spider Web**: Leap in or out of battlefield as the wave progresses, when leaping in, deals `(1 ND) PD` to enemies in AOE range 3 and stuns them for 5s.</t>
   </si>
 </sst>
 </file>
@@ -22062,8 +22062,8 @@
   <dimension ref="A1:N166"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L157" sqref="L157"/>
+      <pane ySplit="1" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L145" sqref="L145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26811,7 +26811,7 @@
         <v>0</v>
       </c>
       <c r="L113" s="23" t="s">
-        <v>2795</v>
+        <v>2794</v>
       </c>
       <c r="M113" s="25" t="s">
         <v>1130</v>
@@ -27274,7 +27274,7 @@
         <v>0</v>
       </c>
       <c r="L124" s="23" t="s">
-        <v>2793</v>
+        <v>2830</v>
       </c>
       <c r="N124" s="27" t="s">
         <v>1375</v>
@@ -27775,7 +27775,7 @@
         <v>0</v>
       </c>
       <c r="L136" s="23" t="s">
-        <v>2794</v>
+        <v>2793</v>
       </c>
       <c r="M136" s="25" t="s">
         <v>870</v>
@@ -28171,7 +28171,7 @@
         <v>0</v>
       </c>
       <c r="L145" s="23" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="N145" s="33" t="s">
         <v>2428</v>
@@ -28212,7 +28212,7 @@
         <v>0</v>
       </c>
       <c r="L146" s="23" t="s">
-        <v>2797</v>
+        <v>2796</v>
       </c>
       <c r="M146" s="25" t="s">
         <v>1130</v>
@@ -28256,10 +28256,10 @@
         <v>0</v>
       </c>
       <c r="L147" s="23" t="s">
-        <v>2798</v>
+        <v>2797</v>
       </c>
       <c r="N147" s="30" t="s">
-        <v>2822</v>
+        <v>2820</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.35">
@@ -28297,10 +28297,10 @@
         <v>0</v>
       </c>
       <c r="L148" s="23" t="s">
-        <v>2799</v>
+        <v>2798</v>
       </c>
       <c r="N148" s="30" t="s">
-        <v>2821</v>
+        <v>2819</v>
       </c>
     </row>
     <row r="149" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
@@ -28338,13 +28338,13 @@
         <v>0</v>
       </c>
       <c r="L149" s="23" t="s">
-        <v>2800</v>
+        <v>2799</v>
       </c>
       <c r="N149" s="30" t="s">
         <v>2339</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:14" ht="87" x14ac:dyDescent="0.35">
       <c r="A150" s="23" t="s">
         <v>2665</v>
       </c>
@@ -28382,7 +28382,7 @@
         <v>2829</v>
       </c>
       <c r="N150" s="30" t="s">
-        <v>2823</v>
+        <v>2821</v>
       </c>
     </row>
     <row r="151" spans="1:14" ht="58" x14ac:dyDescent="0.35">
@@ -28420,10 +28420,10 @@
         <v>0</v>
       </c>
       <c r="L151" s="23" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="N151" s="30" t="s">
-        <v>2824</v>
+        <v>2822</v>
       </c>
     </row>
     <row r="152" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
@@ -28461,7 +28461,7 @@
         <v>0</v>
       </c>
       <c r="L152" s="23" t="s">
-        <v>2802</v>
+        <v>2801</v>
       </c>
       <c r="N152" s="33" t="s">
         <v>2338</v>
@@ -28502,7 +28502,7 @@
         <v>0</v>
       </c>
       <c r="L153" s="23" t="s">
-        <v>2803</v>
+        <v>2802</v>
       </c>
       <c r="N153" s="30" t="s">
         <v>2337</v>
@@ -28543,7 +28543,7 @@
         <v>0</v>
       </c>
       <c r="L154" s="23" t="s">
-        <v>2804</v>
+        <v>2803</v>
       </c>
       <c r="N154" s="30" t="s">
         <v>2341</v>
@@ -28584,7 +28584,7 @@
         <v>0</v>
       </c>
       <c r="L155" s="23" t="s">
-        <v>2805</v>
+        <v>2804</v>
       </c>
       <c r="N155" s="30" t="s">
         <v>2340</v>
@@ -28625,10 +28625,10 @@
         <v>0</v>
       </c>
       <c r="L156" s="23" t="s">
-        <v>2831</v>
+        <v>2828</v>
       </c>
       <c r="N156" s="30" t="s">
-        <v>2825</v>
+        <v>2823</v>
       </c>
     </row>
     <row r="157" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
@@ -28666,10 +28666,10 @@
         <v>0</v>
       </c>
       <c r="L157" s="23" t="s">
-        <v>2806</v>
+        <v>2805</v>
       </c>
       <c r="N157" s="30" t="s">
-        <v>2826</v>
+        <v>2824</v>
       </c>
     </row>
     <row r="158" spans="1:14" ht="58" x14ac:dyDescent="0.35">
@@ -28707,10 +28707,10 @@
         <v>0</v>
       </c>
       <c r="L158" s="23" t="s">
-        <v>2807</v>
+        <v>2806</v>
       </c>
       <c r="N158" s="30" t="s">
-        <v>2827</v>
+        <v>2825</v>
       </c>
     </row>
     <row r="159" spans="1:14" ht="87" x14ac:dyDescent="0.35">
@@ -28748,7 +28748,7 @@
         <v>0</v>
       </c>
       <c r="L159" s="23" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="N159" s="30" t="s">
         <v>2342</v>
@@ -28789,7 +28789,7 @@
         <v>0</v>
       </c>
       <c r="L160" s="23" t="s">
-        <v>2809</v>
+        <v>2808</v>
       </c>
       <c r="M160" s="25" t="s">
         <v>870</v>
@@ -28833,13 +28833,13 @@
         <v>0</v>
       </c>
       <c r="L161" s="23" t="s">
-        <v>2810</v>
+        <v>2831</v>
       </c>
       <c r="M161" s="25" t="s">
         <v>870</v>
       </c>
       <c r="N161" s="30" t="s">
-        <v>2828</v>
+        <v>2826</v>
       </c>
     </row>
     <row r="166" spans="1:14" ht="26.5" x14ac:dyDescent="0.35">
@@ -35036,7 +35036,7 @@
       <c r="F252" s="14"/>
       <c r="G252" s="14"/>
       <c r="H252" s="18" t="s">
-        <v>2811</v>
+        <v>2809</v>
       </c>
       <c r="I252" s="18"/>
     </row>
@@ -35064,7 +35064,7 @@
         <v>2349</v>
       </c>
       <c r="H253" s="18" t="s">
-        <v>2812</v>
+        <v>2810</v>
       </c>
       <c r="I253" s="18"/>
     </row>
@@ -35090,7 +35090,7 @@
         <v>2349</v>
       </c>
       <c r="H254" s="18" t="s">
-        <v>2813</v>
+        <v>2811</v>
       </c>
       <c r="I254" s="18"/>
     </row>
@@ -35116,7 +35116,7 @@
       </c>
       <c r="G255" s="14"/>
       <c r="H255" s="18" t="s">
-        <v>2814</v>
+        <v>2812</v>
       </c>
       <c r="I255" s="18"/>
     </row>
@@ -35142,7 +35142,7 @@
       </c>
       <c r="G256" s="14"/>
       <c r="H256" s="18" t="s">
-        <v>2815</v>
+        <v>2813</v>
       </c>
       <c r="I256" s="18"/>
     </row>
@@ -35166,7 +35166,7 @@
       <c r="F257" s="14"/>
       <c r="G257" s="14"/>
       <c r="H257" s="18" t="s">
-        <v>2816</v>
+        <v>2814</v>
       </c>
       <c r="I257" s="18"/>
     </row>
@@ -35188,11 +35188,11 @@
         <v>2159</v>
       </c>
       <c r="F258" s="14" t="s">
-        <v>2830</v>
+        <v>2827</v>
       </c>
       <c r="G258" s="14"/>
       <c r="H258" s="18" t="s">
-        <v>2817</v>
+        <v>2815</v>
       </c>
       <c r="I258" s="18"/>
     </row>
@@ -35217,7 +35217,7 @@
         <v>2349</v>
       </c>
       <c r="H259" s="18" t="s">
-        <v>2818</v>
+        <v>2816</v>
       </c>
       <c r="I259" s="18"/>
     </row>
@@ -35241,7 +35241,7 @@
       <c r="F260" s="14"/>
       <c r="G260" s="14"/>
       <c r="H260" s="18" t="s">
-        <v>2819</v>
+        <v>2817</v>
       </c>
       <c r="I260" s="18"/>
     </row>
@@ -35265,7 +35265,7 @@
       <c r="F261" s="14"/>
       <c r="G261" s="14"/>
       <c r="H261" s="18" t="s">
-        <v>2820</v>
+        <v>2818</v>
       </c>
       <c r="I261" s="18" t="s">
         <v>870</v>

</xml_diff>

<commit_message>
change uppercase of several names, may have bug
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\data\q-z\Realm Defense\CyraBot\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F333C8-72F7-4F85-805C-CFFF9774AAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70F8B4A-4A38-4350-ABD6-60742503FEDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="388" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hero" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6088" uniqueCount="2856">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6084" uniqueCount="2856">
   <si>
     <t>name</t>
   </si>
@@ -9685,7 +9685,7 @@
   <dimension ref="A1:Y27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -11812,9 +11812,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H215"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A164" sqref="A164"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12012,20 +12012,6 @@
       </c>
       <c r="F8" s="1">
         <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>2279</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>2279</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>2279</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>2279</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -16612,7 +16598,7 @@
   <dimension ref="A1:D392"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A387" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D385" sqref="D385"/>
     </sheetView>
   </sheetViews>
@@ -22043,7 +22029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED1689C-43D8-4482-B475-EE9D75A4CF53}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
@@ -29505,7 +29491,7 @@
         <v>2135</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A147" s="20" t="s">
         <v>2406</v>
       </c>
@@ -29546,7 +29532,7 @@
         <v>2568</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A148" s="20" t="s">
         <v>2407</v>
       </c>

</xml_diff>